<commit_message>
Auto-committed on 2022/05/18 週三 17:50:41.91
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -24,7 +24,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">X月!$A$1:$G$51</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3049,172 +3049,128 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="54" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3270,55 +3226,99 @@
     <xf numFmtId="181" fontId="54" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4027,7 +4027,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -4050,30 +4050,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="156" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
       <c r="H1" s="30"/>
       <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="219"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
+      <c r="A2" s="142"/>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
       <c r="H2" s="30"/>
       <c r="J2" s="32"/>
-      <c r="K2" s="225"/>
-      <c r="L2" s="225"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4098,21 +4098,21 @@
       <c r="O3" s="31"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="185"/>
-      <c r="D4" s="186" t="s">
+      <c r="C4" s="160"/>
+      <c r="D4" s="161" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="187"/>
-      <c r="F4" s="188" t="s">
+      <c r="E4" s="162"/>
+      <c r="F4" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="220" t="s">
+      <c r="G4" s="143" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="71"/>
@@ -4124,7 +4124,7 @@
       <c r="N4" s="72"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="148"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="36" t="s">
         <v>35</v>
       </c>
@@ -4137,8 +4137,8 @@
       <c r="E5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="189"/>
-      <c r="G5" s="221"/>
+      <c r="F5" s="164"/>
+      <c r="G5" s="144"/>
       <c r="H5" s="72"/>
       <c r="I5" s="72"/>
       <c r="J5" s="72"/>
@@ -4162,8 +4162,8 @@
       <c r="G6" s="29"/>
       <c r="H6" s="75"/>
       <c r="I6" s="72"/>
-      <c r="J6" s="226"/>
-      <c r="K6" s="226"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
       <c r="L6" s="76">
         <f>J6-G6</f>
         <v>0</v>
@@ -4190,8 +4190,8 @@
       <c r="I7" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="226"/>
-      <c r="K7" s="226"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
       <c r="L7" s="76">
         <f>J7-G7</f>
         <v>0</v>
@@ -4301,12 +4301,12 @@
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
-      <c r="D11" s="170"/>
-      <c r="E11" s="217" t="s">
+      <c r="D11" s="145"/>
+      <c r="E11" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="170"/>
-      <c r="G11" s="170"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
       <c r="H11" s="87"/>
       <c r="I11" s="88">
         <f>H11-E10</f>
@@ -4319,15 +4319,15 @@
       <c r="N11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="199" t="s">
+      <c r="A12" s="183" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="200"/>
-      <c r="C12" s="200"/>
-      <c r="D12" s="222"/>
-      <c r="E12" s="218"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
+      <c r="B12" s="184"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="40"/>
       <c r="I12" s="40"/>
       <c r="J12" s="86"/>
@@ -4337,17 +4337,17 @@
       <c r="N12" s="72"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="201"/>
-      <c r="B13" s="202"/>
-      <c r="C13" s="202"/>
+      <c r="A13" s="185"/>
+      <c r="B13" s="186"/>
+      <c r="C13" s="186"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="197" t="s">
+      <c r="E13" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="172" t="s">
+      <c r="F13" s="198" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="173"/>
+      <c r="G13" s="199"/>
       <c r="H13" s="89" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
@@ -4365,16 +4365,16 @@
       <c r="A14" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="227" t="s">
+      <c r="B14" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="228"/>
+      <c r="C14" s="155"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="198"/>
-      <c r="F14" s="174" t="s">
+      <c r="E14" s="182"/>
+      <c r="F14" s="200" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="175"/>
+      <c r="G14" s="201"/>
       <c r="H14" s="40"/>
       <c r="I14" s="40"/>
       <c r="J14" s="86"/>
@@ -4387,19 +4387,19 @@
       <c r="A15" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="223" t="s">
+      <c r="B15" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="224"/>
+      <c r="C15" s="151"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="180" t="s">
+      <c r="E15" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="139" t="e">
+      <c r="F15" s="220" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="140"/>
+      <c r="G15" s="221"/>
       <c r="H15" s="40"/>
       <c r="I15" s="40"/>
       <c r="J15" s="86"/>
@@ -4409,18 +4409,18 @@
       <c r="N15" s="72"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="180" t="s">
+      <c r="A16" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="193" t="e">
+      <c r="B16" s="177" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="194"/>
+      <c r="C16" s="178"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="142"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="222"/>
+      <c r="G16" s="223"/>
       <c r="H16" s="40"/>
       <c r="I16" s="92"/>
       <c r="J16" s="72"/>
@@ -4430,15 +4430,15 @@
       <c r="N16" s="72"/>
     </row>
     <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="181"/>
-      <c r="B17" s="195"/>
-      <c r="C17" s="196"/>
+      <c r="A17" s="149"/>
+      <c r="B17" s="179"/>
+      <c r="C17" s="180"/>
       <c r="D17" s="40"/>
       <c r="E17" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="145"/>
-      <c r="G17" s="146"/>
+      <c r="F17" s="175"/>
+      <c r="G17" s="176"/>
       <c r="H17" s="93">
         <f>G10-H18</f>
         <v>0</v>
@@ -4456,20 +4456,20 @@
       <c r="N17" s="72"/>
     </row>
     <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="207" t="s">
+      <c r="A18" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="208" t="e">
+      <c r="B18" s="192" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="209"/>
+      <c r="C18" s="193"/>
       <c r="D18" s="40"/>
       <c r="E18" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="143"/>
-      <c r="G18" s="144"/>
+      <c r="F18" s="224"/>
+      <c r="G18" s="225"/>
       <c r="H18" s="93">
         <f>G7</f>
         <v>0</v>
@@ -4488,15 +4488,15 @@
       <c r="N18" s="72"/>
     </row>
     <row r="19" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="207"/>
-      <c r="B19" s="208"/>
-      <c r="C19" s="209"/>
+      <c r="A19" s="191"/>
+      <c r="B19" s="192"/>
+      <c r="C19" s="193"/>
       <c r="D19" s="40"/>
       <c r="E19" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="145"/>
-      <c r="G19" s="146"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="176"/>
       <c r="H19" s="93">
         <f>G10-H20</f>
         <v>0</v>
@@ -4512,17 +4512,17 @@
       <c r="N19" s="72"/>
     </row>
     <row r="20" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="190" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="203"/>
-      <c r="C20" s="204"/>
+      <c r="B20" s="187"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="40"/>
       <c r="E20" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="143"/>
-      <c r="G20" s="144"/>
+      <c r="F20" s="224"/>
+      <c r="G20" s="225"/>
       <c r="H20" s="23"/>
       <c r="I20" s="96">
         <f>F7</f>
@@ -4538,9 +4538,9 @@
       <c r="N20" s="72"/>
     </row>
     <row r="21" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="206"/>
-      <c r="B21" s="203"/>
-      <c r="C21" s="204"/>
+      <c r="A21" s="190"/>
+      <c r="B21" s="187"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
@@ -4554,17 +4554,17 @@
       <c r="N21" s="72"/>
     </row>
     <row r="22" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="206"/>
-      <c r="B22" s="203"/>
-      <c r="C22" s="204"/>
+      <c r="A22" s="190"/>
+      <c r="B22" s="187"/>
+      <c r="C22" s="188"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="147" t="s">
+      <c r="E22" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="147" t="s">
+      <c r="F22" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="147" t="s">
+      <c r="G22" s="165" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="93"/>
@@ -4576,18 +4576,18 @@
       <c r="N22" s="72"/>
     </row>
     <row r="23" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="205" t="s">
+      <c r="A23" s="189" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="210">
+      <c r="B23" s="194">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="211"/>
+      <c r="C23" s="195"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
+      <c r="E23" s="158"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="158"/>
       <c r="H23" s="93"/>
       <c r="I23" s="99"/>
       <c r="J23" s="72"/>
@@ -4597,9 +4597,9 @@
       <c r="N23" s="72"/>
     </row>
     <row r="24" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="205"/>
-      <c r="B24" s="210"/>
-      <c r="C24" s="211"/>
+      <c r="A24" s="189"/>
+      <c r="B24" s="194"/>
+      <c r="C24" s="195"/>
       <c r="D24" s="40"/>
       <c r="E24" s="47" t="s">
         <v>32</v>
@@ -4615,9 +4615,9 @@
       <c r="N24" s="72"/>
     </row>
     <row r="25" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="205"/>
-      <c r="B25" s="210"/>
-      <c r="C25" s="211"/>
+      <c r="A25" s="189"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="195"/>
       <c r="D25" s="40"/>
       <c r="E25" s="48" t="s">
         <v>31</v>
@@ -4639,8 +4639,8 @@
       <c r="A26" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="155"/>
-      <c r="C26" s="155"/>
+      <c r="B26" s="228"/>
+      <c r="C26" s="228"/>
       <c r="D26" s="50"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
@@ -4658,40 +4658,40 @@
       <c r="N26" s="40"/>
     </row>
     <row r="27" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="147" t="s">
+      <c r="A27" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="158"/>
-      <c r="C27" s="191"/>
-      <c r="D27" s="162" t="s">
+      <c r="B27" s="169"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="163"/>
-      <c r="F27" s="158"/>
+      <c r="E27" s="218"/>
+      <c r="F27" s="169"/>
       <c r="G27" s="51" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="104"/>
       <c r="I27" s="105"/>
-      <c r="J27" s="215" t="s">
+      <c r="J27" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="216"/>
-      <c r="L27" s="212" t="s">
+      <c r="K27" s="139"/>
+      <c r="L27" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="213"/>
-      <c r="N27" s="214"/>
+      <c r="M27" s="136"/>
+      <c r="N27" s="137"/>
     </row>
     <row r="28" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="190"/>
-      <c r="B28" s="159"/>
-      <c r="C28" s="192"/>
-      <c r="D28" s="149" t="s">
+      <c r="A28" s="166"/>
+      <c r="B28" s="171"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="226" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="150"/>
-      <c r="F28" s="159"/>
+      <c r="E28" s="227"/>
+      <c r="F28" s="171"/>
       <c r="G28" s="52" t="s">
         <v>22</v>
       </c>
@@ -4707,21 +4707,21 @@
       <c r="A29" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="151">
-        <f>H29+SUM(B30:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="153" t="e">
+      <c r="B29" s="167">
+        <f>SUM(B30:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="168"/>
+      <c r="D29" s="173" t="e">
         <f>CONCATENATE(TEXT($G$10-B29,"0,000"),"       ",TEXT(($G$10-B29)/B29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="154" t="str">
+      <c r="E29" s="174" t="str">
         <f t="shared" ref="E29:E33" si="1">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F29" s="54">
-        <f t="shared" ref="F29:F33" si="2">L29</f>
+        <f>SUM(F30:F32)</f>
         <v>0</v>
       </c>
       <c r="G29" s="19" t="e">
@@ -4737,7 +4737,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="115" t="e">
-        <f t="shared" ref="K29:K35" si="3">J29/B29</f>
+        <f t="shared" ref="K29:K35" si="2">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L29" s="113"/>
@@ -4746,7 +4746,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="115" t="e">
-        <f t="shared" ref="N29:N35" si="4">M29/F29</f>
+        <f t="shared" ref="N29:N35" si="3">M29/F29</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4754,14 +4754,14 @@
       <c r="A30" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
-      <c r="D30" s="153" t="e">
+      <c r="B30" s="167"/>
+      <c r="C30" s="168"/>
+      <c r="D30" s="173" t="e">
         <f>CONCATENATE(TEXT(G6-B30,"0,000"),"       ",TEXT((G6-B30)/B30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="154" t="str">
-        <f t="shared" ref="E30" si="5">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
+      <c r="E30" s="174" t="str">
+        <f t="shared" ref="E30" si="4">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F30" s="56"/>
@@ -4778,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="118" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="116"/>
@@ -4787,7 +4787,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="118" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4795,14 +4795,14 @@
       <c r="A31" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="151"/>
-      <c r="C31" s="152"/>
-      <c r="D31" s="153" t="e">
-        <f t="shared" ref="D31" si="6">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
+      <c r="B31" s="167"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="173" t="e">
+        <f t="shared" ref="D31" si="5">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="154" t="str">
-        <f t="shared" ref="E31:E32" si="7">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
+      <c r="E31" s="174" t="str">
+        <f t="shared" ref="E31:E32" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
       <c r="F31" s="56"/>
@@ -4819,7 +4819,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="118" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="116"/>
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="118" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4836,14 +4836,14 @@
       <c r="A32" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="151"/>
-      <c r="C32" s="152"/>
-      <c r="D32" s="153" t="e">
+      <c r="B32" s="167"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="173" t="e">
         <f>CONCATENATE(TEXT(G8-B32+G9,"0,000"),"       ",TEXT((G8-B32+G9)/B32,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="154" t="str">
-        <f t="shared" si="7"/>
+      <c r="E32" s="174" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F32" s="56"/>
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="121" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="116"/>
@@ -4869,7 +4869,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="121" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4877,21 +4877,21 @@
       <c r="A33" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="151">
-        <f>H33+SUM(B34:C36)</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="152"/>
-      <c r="D33" s="153" t="e">
+      <c r="B33" s="167">
+        <f>SUM(B34:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="168"/>
+      <c r="D33" s="173" t="e">
         <f>CONCATENATE(TEXT(E10-B33,"0,000"),"       ",TEXT((E10-B33)/B33,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="154" t="str">
+      <c r="E33" s="174" t="str">
         <f t="shared" si="1"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F33" s="56">
-        <f t="shared" si="2"/>
+        <f>SUM(F34:F36)</f>
         <v>0</v>
       </c>
       <c r="G33" s="19" t="e">
@@ -4907,7 +4907,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="115" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L33" s="113"/>
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="115" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4924,14 +4924,14 @@
       <c r="A34" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="151"/>
-      <c r="C34" s="152"/>
-      <c r="D34" s="153" t="e">
+      <c r="B34" s="167"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="173" t="e">
         <f>CONCATENATE(TEXT(E6-B34,"0,000"),"       ",TEXT((E6-B34)/B34,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="154" t="str">
-        <f t="shared" ref="E34" si="8">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
+      <c r="E34" s="174" t="str">
+        <f t="shared" ref="E34" si="7">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F34" s="56"/>
@@ -4948,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="118" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L34" s="116"/>
@@ -4957,7 +4957,7 @@
         <v>0</v>
       </c>
       <c r="N34" s="118" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4965,14 +4965,14 @@
       <c r="A35" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="151"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="153" t="e">
-        <f t="shared" ref="D35" si="9">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
+      <c r="B35" s="167"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="173" t="e">
+        <f t="shared" ref="D35" si="8">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="154" t="str">
-        <f t="shared" ref="E35:E37" si="10">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
+      <c r="E35" s="174" t="str">
+        <f t="shared" ref="E35:E37" si="9">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
       <c r="F35" s="56"/>
@@ -4989,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="K35" s="118" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L35" s="116"/>
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="N35" s="118" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5006,14 +5006,14 @@
       <c r="A36" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="151"/>
-      <c r="C36" s="152"/>
-      <c r="D36" s="153" t="e">
+      <c r="B36" s="167"/>
+      <c r="C36" s="168"/>
+      <c r="D36" s="173" t="e">
         <f>CONCATENATE(TEXT(E8-B36+E9,"0,000"),"       ",TEXT((E8-B36+E9)/B36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="154" t="str">
-        <f t="shared" si="10"/>
+      <c r="E36" s="174" t="str">
+        <f t="shared" si="9"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F36" s="56"/>
@@ -5047,14 +5047,14 @@
       <c r="A37" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="151"/>
-      <c r="C37" s="152"/>
-      <c r="D37" s="153" t="e">
+      <c r="B37" s="167"/>
+      <c r="C37" s="168"/>
+      <c r="D37" s="173" t="e">
         <f>CONCATENATE(TEXT(C10-B37,"0,000"),"       ",TEXT((C10-B37)/B37,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="154" t="str">
-        <f t="shared" si="10"/>
+      <c r="E37" s="174" t="str">
+        <f t="shared" si="9"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F37" s="56"/>
@@ -5088,16 +5088,16 @@
       <c r="A38" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="160" t="e">
+      <c r="B38" s="215" t="e">
         <f>F38=(B37+B33)/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="161"/>
-      <c r="D38" s="178" t="e">
+      <c r="C38" s="216"/>
+      <c r="D38" s="209" t="e">
         <f>F15-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="179"/>
+      <c r="E38" s="210"/>
       <c r="F38" s="60" t="e">
         <f>(F37+F33)/F29</f>
         <v>#DIV/0!</v>
@@ -5152,14 +5152,14 @@
       <c r="A40" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="166" t="s">
+      <c r="B40" s="205" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="167"/>
-      <c r="D40" s="166" t="s">
+      <c r="C40" s="206"/>
+      <c r="D40" s="205" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="167"/>
+      <c r="E40" s="206"/>
       <c r="F40" s="69" t="s">
         <v>3</v>
       </c>
@@ -5176,100 +5176,100 @@
     </row>
     <row r="41" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
-      <c r="B41" s="135"/>
-      <c r="C41" s="136"/>
-      <c r="D41" s="137"/>
-      <c r="E41" s="138"/>
+      <c r="B41" s="203"/>
+      <c r="C41" s="204"/>
+      <c r="D41" s="213"/>
+      <c r="E41" s="214"/>
       <c r="F41" s="11"/>
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="12"/>
-      <c r="B42" s="135"/>
-      <c r="C42" s="136"/>
-      <c r="D42" s="137"/>
-      <c r="E42" s="138"/>
+      <c r="B42" s="203"/>
+      <c r="C42" s="204"/>
+      <c r="D42" s="213"/>
+      <c r="E42" s="214"/>
       <c r="F42" s="11"/>
       <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="12"/>
-      <c r="B43" s="135"/>
-      <c r="C43" s="136"/>
-      <c r="D43" s="137"/>
-      <c r="E43" s="138"/>
+      <c r="B43" s="203"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="213"/>
+      <c r="E43" s="214"/>
       <c r="F43" s="11"/>
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="12"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="136"/>
-      <c r="D44" s="137"/>
-      <c r="E44" s="138"/>
+      <c r="B44" s="203"/>
+      <c r="C44" s="204"/>
+      <c r="D44" s="213"/>
+      <c r="E44" s="214"/>
       <c r="F44" s="11"/>
       <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="12"/>
-      <c r="B45" s="135"/>
-      <c r="C45" s="136"/>
-      <c r="D45" s="137"/>
-      <c r="E45" s="138"/>
+      <c r="B45" s="203"/>
+      <c r="C45" s="204"/>
+      <c r="D45" s="213"/>
+      <c r="E45" s="214"/>
       <c r="F45" s="11"/>
       <c r="G45" s="13"/>
     </row>
     <row r="46" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="12"/>
-      <c r="B46" s="135"/>
-      <c r="C46" s="136"/>
-      <c r="D46" s="137"/>
-      <c r="E46" s="138"/>
+      <c r="B46" s="203"/>
+      <c r="C46" s="204"/>
+      <c r="D46" s="213"/>
+      <c r="E46" s="214"/>
       <c r="F46" s="11"/>
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="12"/>
-      <c r="B47" s="135"/>
-      <c r="C47" s="136"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="136"/>
+      <c r="B47" s="203"/>
+      <c r="C47" s="204"/>
+      <c r="D47" s="203"/>
+      <c r="E47" s="204"/>
       <c r="F47" s="11"/>
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="12"/>
-      <c r="B48" s="135"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="136"/>
+      <c r="B48" s="203"/>
+      <c r="C48" s="204"/>
+      <c r="D48" s="203"/>
+      <c r="E48" s="204"/>
       <c r="F48" s="11"/>
       <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="12"/>
-      <c r="B49" s="135"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="136"/>
+      <c r="B49" s="203"/>
+      <c r="C49" s="204"/>
+      <c r="D49" s="203"/>
+      <c r="E49" s="204"/>
       <c r="F49" s="11"/>
       <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="12"/>
-      <c r="B50" s="135"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="136"/>
+      <c r="B50" s="203"/>
+      <c r="C50" s="204"/>
+      <c r="D50" s="203"/>
+      <c r="E50" s="204"/>
       <c r="F50" s="11"/>
       <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="12"/>
-      <c r="B51" s="135"/>
-      <c r="C51" s="136"/>
-      <c r="D51" s="135"/>
-      <c r="E51" s="136"/>
+      <c r="B51" s="203"/>
+      <c r="C51" s="204"/>
+      <c r="D51" s="203"/>
+      <c r="E51" s="204"/>
       <c r="F51" s="11"/>
       <c r="G51" s="10"/>
     </row>
@@ -5277,16 +5277,16 @@
       <c r="A52" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="156">
+      <c r="B52" s="211">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="156"/>
-      <c r="D52" s="156">
+      <c r="C52" s="211"/>
+      <c r="D52" s="211">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="156"/>
+      <c r="E52" s="211"/>
       <c r="F52" s="64" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
@@ -5304,16 +5304,16 @@
       <c r="A53" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="165">
+      <c r="B53" s="208">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="165"/>
-      <c r="D53" s="165">
+      <c r="C53" s="208"/>
+      <c r="D53" s="208">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="165"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="67">
         <f>F51-F49</f>
         <v>0</v>
@@ -5328,69 +5328,69 @@
       <c r="N53" s="8"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="157"/>
-      <c r="B54" s="164"/>
-      <c r="C54" s="164"/>
-      <c r="D54" s="177"/>
-      <c r="E54" s="177"/>
-      <c r="F54" s="169"/>
-      <c r="G54" s="176"/>
+      <c r="A54" s="212"/>
+      <c r="B54" s="219"/>
+      <c r="C54" s="219"/>
+      <c r="D54" s="207"/>
+      <c r="E54" s="207"/>
+      <c r="F54" s="197"/>
+      <c r="G54" s="202"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="157"/>
-      <c r="B55" s="164"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="177"/>
-      <c r="F55" s="169"/>
-      <c r="G55" s="176"/>
+      <c r="A55" s="212"/>
+      <c r="B55" s="219"/>
+      <c r="C55" s="219"/>
+      <c r="D55" s="207"/>
+      <c r="E55" s="207"/>
+      <c r="F55" s="197"/>
+      <c r="G55" s="202"/>
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="5"/>
-      <c r="B56" s="168"/>
-      <c r="C56" s="168"/>
-      <c r="D56" s="168"/>
-      <c r="E56" s="168"/>
-      <c r="F56" s="168"/>
-      <c r="G56" s="168"/>
+      <c r="B56" s="196"/>
+      <c r="C56" s="196"/>
+      <c r="D56" s="196"/>
+      <c r="E56" s="196"/>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A57" s="5"/>
-      <c r="B57" s="168"/>
-      <c r="C57" s="168"/>
-      <c r="D57" s="168"/>
-      <c r="E57" s="168"/>
-      <c r="F57" s="168"/>
-      <c r="G57" s="168"/>
+      <c r="B57" s="196"/>
+      <c r="C57" s="196"/>
+      <c r="D57" s="196"/>
+      <c r="E57" s="196"/>
+      <c r="F57" s="196"/>
+      <c r="G57" s="196"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A58" s="5"/>
-      <c r="B58" s="168"/>
-      <c r="C58" s="168"/>
-      <c r="D58" s="168"/>
-      <c r="E58" s="168"/>
-      <c r="F58" s="168"/>
-      <c r="G58" s="168"/>
+      <c r="B58" s="196"/>
+      <c r="C58" s="196"/>
+      <c r="D58" s="196"/>
+      <c r="E58" s="196"/>
+      <c r="F58" s="196"/>
+      <c r="G58" s="196"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A59" s="5"/>
-      <c r="B59" s="168"/>
-      <c r="C59" s="168"/>
-      <c r="D59" s="168"/>
-      <c r="E59" s="168"/>
-      <c r="F59" s="168"/>
-      <c r="G59" s="168"/>
+      <c r="B59" s="196"/>
+      <c r="C59" s="196"/>
+      <c r="D59" s="196"/>
+      <c r="E59" s="196"/>
+      <c r="F59" s="196"/>
+      <c r="G59" s="196"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A60" s="5"/>
-      <c r="B60" s="168"/>
-      <c r="C60" s="168"/>
-      <c r="D60" s="168"/>
-      <c r="E60" s="168"/>
-      <c r="F60" s="168"/>
-      <c r="G60" s="168"/>
+      <c r="B60" s="196"/>
+      <c r="C60" s="196"/>
+      <c r="D60" s="196"/>
+      <c r="E60" s="196"/>
+      <c r="F60" s="196"/>
+      <c r="G60" s="196"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.4">
       <c r="J62" s="4"/>
@@ -5404,19 +5404,71 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
@@ -5441,71 +5493,19 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B23:C25"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/05/30 週一 11:48:31.43
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -1328,7 +1328,7 @@
     <numFmt numFmtId="185" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="186" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="86" x14ac:knownFonts="1">
+  <fonts count="86">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2715,7 +2715,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3078,178 +3078,131 @@
     </xf>
     <xf numFmtId="181" fontId="34" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="46" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="54" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3305,55 +3258,93 @@
     <xf numFmtId="181" fontId="54" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4062,10 +4053,10 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D3:E4"/>
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="26" style="3" customWidth="1"/>
     <col min="2" max="2" width="7.08984375" style="3" customWidth="1"/>
@@ -4084,34 +4075,34 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="183" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="156" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
       <c r="H1" s="30"/>
       <c r="O1" s="30"/>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="220"/>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="142"/>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
       <c r="H2" s="30"/>
       <c r="J2" s="32"/>
-      <c r="K2" s="226"/>
-      <c r="L2" s="226"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
       <c r="A3" s="33" t="s">
         <v>66</v>
       </c>
@@ -4132,22 +4123,22 @@
       <c r="N3" s="72"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="184" t="s">
+    <row r="4" spans="1:15" ht="54.75" customHeight="1">
+      <c r="A4" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="185" t="s">
+      <c r="B4" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="186"/>
-      <c r="D4" s="187" t="s">
+      <c r="C4" s="160"/>
+      <c r="D4" s="161" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="188"/>
-      <c r="F4" s="189" t="s">
+      <c r="E4" s="162"/>
+      <c r="F4" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="221" t="s">
+      <c r="G4" s="143" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="71"/>
@@ -4158,8 +4149,8 @@
       <c r="M4" s="72"/>
       <c r="N4" s="72"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="149"/>
+    <row r="5" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A5" s="158"/>
       <c r="B5" s="36" t="s">
         <v>35</v>
       </c>
@@ -4172,8 +4163,8 @@
       <c r="E5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="190"/>
-      <c r="G5" s="222"/>
+      <c r="F5" s="164"/>
+      <c r="G5" s="144"/>
       <c r="H5" s="72"/>
       <c r="I5" s="72"/>
       <c r="J5" s="72"/>
@@ -4182,7 +4173,7 @@
       <c r="M5" s="72"/>
       <c r="N5" s="72"/>
     </row>
-    <row r="6" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" ht="22" customHeight="1">
       <c r="A6" s="70" t="s">
         <v>59</v>
       </c>
@@ -4197,8 +4188,8 @@
       <c r="G6" s="29"/>
       <c r="H6" s="75"/>
       <c r="I6" s="72"/>
-      <c r="J6" s="227"/>
-      <c r="K6" s="227"/>
+      <c r="J6" s="153"/>
+      <c r="K6" s="153"/>
       <c r="L6" s="76">
         <f>J6-G6</f>
         <v>0</v>
@@ -4206,7 +4197,7 @@
       <c r="M6" s="72"/>
       <c r="N6" s="72"/>
     </row>
-    <row r="7" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" ht="22" customHeight="1">
       <c r="A7" s="70" t="s">
         <v>58</v>
       </c>
@@ -4225,8 +4216,8 @@
       <c r="I7" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="227"/>
-      <c r="K7" s="227"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
       <c r="L7" s="76">
         <f>J7-G7</f>
         <v>0</v>
@@ -4234,7 +4225,7 @@
       <c r="M7" s="72"/>
       <c r="N7" s="72"/>
     </row>
-    <row r="8" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" ht="22" customHeight="1">
       <c r="A8" s="36" t="s">
         <v>55</v>
       </c>
@@ -4264,7 +4255,7 @@
       <c r="M8" s="72"/>
       <c r="N8" s="72"/>
     </row>
-    <row r="9" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="22" customHeight="1">
       <c r="A9" s="70" t="s">
         <v>54</v>
       </c>
@@ -4291,7 +4282,7 @@
       <c r="M9" s="72"/>
       <c r="N9" s="72"/>
     </row>
-    <row r="10" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="34.5" customHeight="1">
       <c r="A10" s="38" t="s">
         <v>53</v>
       </c>
@@ -4330,18 +4321,18 @@
       <c r="M10" s="72"/>
       <c r="N10" s="72"/>
     </row>
-    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="39" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="218" t="s">
+      <c r="D11" s="145"/>
+      <c r="E11" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="171"/>
-      <c r="G11" s="171"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
       <c r="H11" s="87"/>
       <c r="I11" s="88">
         <f>H11-E10</f>
@@ -4353,16 +4344,16 @@
       <c r="M11" s="72"/>
       <c r="N11" s="72"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="200" t="s">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A12" s="183" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="201"/>
-      <c r="C12" s="201"/>
-      <c r="D12" s="223"/>
-      <c r="E12" s="219"/>
-      <c r="F12" s="172"/>
-      <c r="G12" s="172"/>
+      <c r="B12" s="184"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="40"/>
       <c r="I12" s="40"/>
       <c r="J12" s="86"/>
@@ -4371,18 +4362,18 @@
       <c r="M12" s="72"/>
       <c r="N12" s="72"/>
     </row>
-    <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="202"/>
-      <c r="B13" s="203"/>
-      <c r="C13" s="203"/>
+    <row r="13" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A13" s="185"/>
+      <c r="B13" s="186"/>
+      <c r="C13" s="186"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="198" t="s">
+      <c r="E13" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="173" t="s">
+      <c r="F13" s="198" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="174"/>
+      <c r="G13" s="199"/>
       <c r="H13" s="89" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
@@ -4396,20 +4387,20 @@
       <c r="M13" s="72"/>
       <c r="N13" s="72"/>
     </row>
-    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="18">
       <c r="A14" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="228" t="s">
+      <c r="B14" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="229"/>
+      <c r="C14" s="155"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="199"/>
-      <c r="F14" s="175" t="s">
+      <c r="E14" s="182"/>
+      <c r="F14" s="200" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="176"/>
+      <c r="G14" s="201"/>
       <c r="H14" s="40"/>
       <c r="I14" s="40"/>
       <c r="J14" s="86"/>
@@ -4418,23 +4409,23 @@
       <c r="M14" s="91"/>
       <c r="N14" s="72"/>
     </row>
-    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="19.5" customHeight="1">
       <c r="A15" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="224" t="s">
+      <c r="B15" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="225"/>
+      <c r="C15" s="151"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="181" t="s">
+      <c r="E15" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="140" t="e">
+      <c r="F15" s="218" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="141"/>
+      <c r="G15" s="219"/>
       <c r="H15" s="40"/>
       <c r="I15" s="40"/>
       <c r="J15" s="86"/>
@@ -4443,19 +4434,19 @@
       <c r="M15" s="91"/>
       <c r="N15" s="72"/>
     </row>
-    <row r="16" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="181" t="s">
+    <row r="16" spans="1:15" ht="20.25" customHeight="1">
+      <c r="A16" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="194" t="e">
+      <c r="B16" s="177" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="195"/>
+      <c r="C16" s="178"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="143"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="220"/>
+      <c r="G16" s="221"/>
       <c r="H16" s="40"/>
       <c r="I16" s="92"/>
       <c r="J16" s="72"/>
@@ -4464,16 +4455,16 @@
       <c r="M16" s="72"/>
       <c r="N16" s="72"/>
     </row>
-    <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="182"/>
-      <c r="B17" s="196"/>
-      <c r="C17" s="197"/>
+    <row r="17" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A17" s="149"/>
+      <c r="B17" s="179"/>
+      <c r="C17" s="180"/>
       <c r="D17" s="40"/>
       <c r="E17" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="146"/>
-      <c r="G17" s="147"/>
+      <c r="F17" s="175"/>
+      <c r="G17" s="176"/>
       <c r="H17" s="93">
         <f>G10-H18</f>
         <v>0</v>
@@ -4490,21 +4481,21 @@
       <c r="M17" s="72"/>
       <c r="N17" s="72"/>
     </row>
-    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="208" t="s">
+    <row r="18" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A18" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="209" t="e">
+      <c r="B18" s="192" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="210"/>
+      <c r="C18" s="193"/>
       <c r="D18" s="40"/>
       <c r="E18" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="144"/>
-      <c r="G18" s="145"/>
+      <c r="F18" s="222"/>
+      <c r="G18" s="223"/>
       <c r="H18" s="93">
         <f>G7</f>
         <v>0</v>
@@ -4522,16 +4513,16 @@
       <c r="M18" s="72"/>
       <c r="N18" s="72"/>
     </row>
-    <row r="19" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="208"/>
-      <c r="B19" s="209"/>
-      <c r="C19" s="210"/>
+    <row r="19" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A19" s="191"/>
+      <c r="B19" s="192"/>
+      <c r="C19" s="193"/>
       <c r="D19" s="40"/>
       <c r="E19" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="146"/>
-      <c r="G19" s="147"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="176"/>
       <c r="H19" s="93">
         <f>G10-H20</f>
         <v>0</v>
@@ -4546,18 +4537,18 @@
       <c r="M19" s="72"/>
       <c r="N19" s="72"/>
     </row>
-    <row r="20" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="207" t="s">
+    <row r="20" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A20" s="190" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="204"/>
-      <c r="C20" s="205"/>
+      <c r="B20" s="187"/>
+      <c r="C20" s="188"/>
       <c r="D20" s="40"/>
       <c r="E20" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="144"/>
-      <c r="G20" s="145"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="223"/>
       <c r="H20" s="23"/>
       <c r="I20" s="96">
         <f>F7</f>
@@ -4572,10 +4563,10 @@
       <c r="M20" s="72"/>
       <c r="N20" s="72"/>
     </row>
-    <row r="21" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="207"/>
-      <c r="B21" s="204"/>
-      <c r="C21" s="205"/>
+    <row r="21" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A21" s="190"/>
+      <c r="B21" s="187"/>
+      <c r="C21" s="188"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
@@ -4588,18 +4579,18 @@
       <c r="M21" s="72"/>
       <c r="N21" s="72"/>
     </row>
-    <row r="22" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="207"/>
-      <c r="B22" s="204"/>
-      <c r="C22" s="205"/>
+    <row r="22" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A22" s="190"/>
+      <c r="B22" s="187"/>
+      <c r="C22" s="188"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="148" t="s">
+      <c r="E22" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="148" t="s">
+      <c r="F22" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="148" t="s">
+      <c r="G22" s="165" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="93"/>
@@ -4610,19 +4601,19 @@
       <c r="M22" s="72"/>
       <c r="N22" s="72"/>
     </row>
-    <row r="23" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="206" t="s">
+    <row r="23" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A23" s="189" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="211">
+      <c r="B23" s="194">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="212"/>
+      <c r="C23" s="195"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
+      <c r="E23" s="158"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="158"/>
       <c r="H23" s="93"/>
       <c r="I23" s="99"/>
       <c r="J23" s="72"/>
@@ -4631,10 +4622,10 @@
       <c r="M23" s="72"/>
       <c r="N23" s="72"/>
     </row>
-    <row r="24" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="206"/>
-      <c r="B24" s="211"/>
-      <c r="C24" s="212"/>
+    <row r="24" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="A24" s="189"/>
+      <c r="B24" s="194"/>
+      <c r="C24" s="195"/>
       <c r="D24" s="40"/>
       <c r="E24" s="47" t="s">
         <v>32</v>
@@ -4649,10 +4640,10 @@
       <c r="M24" s="72"/>
       <c r="N24" s="72"/>
     </row>
-    <row r="25" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="206"/>
-      <c r="B25" s="211"/>
-      <c r="C25" s="212"/>
+    <row r="25" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="A25" s="189"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="195"/>
       <c r="D25" s="40"/>
       <c r="E25" s="48" t="s">
         <v>31</v>
@@ -4670,12 +4661,12 @@
       <c r="M25" s="72"/>
       <c r="N25" s="72"/>
     </row>
-    <row r="26" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" ht="27" customHeight="1">
       <c r="A26" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="156"/>
-      <c r="C26" s="156"/>
+      <c r="B26" s="226"/>
+      <c r="C26" s="226"/>
       <c r="D26" s="50"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
@@ -4692,41 +4683,41 @@
       <c r="M26" s="72"/>
       <c r="N26" s="40"/>
     </row>
-    <row r="27" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="148" t="s">
+    <row r="27" spans="1:14" ht="19.149999999999999" customHeight="1">
+      <c r="A27" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="159"/>
-      <c r="C27" s="192"/>
-      <c r="D27" s="163" t="s">
+      <c r="B27" s="169"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="215" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="164"/>
-      <c r="F27" s="159"/>
+      <c r="E27" s="216"/>
+      <c r="F27" s="169"/>
       <c r="G27" s="51" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="104"/>
       <c r="I27" s="105"/>
-      <c r="J27" s="216" t="s">
+      <c r="J27" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="217"/>
-      <c r="L27" s="213" t="s">
+      <c r="K27" s="139"/>
+      <c r="L27" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="214"/>
-      <c r="N27" s="215"/>
-    </row>
-    <row r="28" spans="1:14" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="191"/>
-      <c r="B28" s="160"/>
-      <c r="C28" s="193"/>
-      <c r="D28" s="150" t="s">
+      <c r="M27" s="136"/>
+      <c r="N27" s="137"/>
+    </row>
+    <row r="28" spans="1:14" ht="19.149999999999999" customHeight="1">
+      <c r="A28" s="166"/>
+      <c r="B28" s="171"/>
+      <c r="C28" s="172"/>
+      <c r="D28" s="224" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="151"/>
-      <c r="F28" s="160"/>
+      <c r="E28" s="225"/>
+      <c r="F28" s="171"/>
       <c r="G28" s="52" t="s">
         <v>22</v>
       </c>
@@ -4738,20 +4729,20 @@
       <c r="M28" s="111"/>
       <c r="N28" s="112"/>
     </row>
-    <row r="29" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A29" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="152">
+      <c r="B29" s="167">
         <f>SUM(B30:C32)</f>
         <v>0</v>
       </c>
-      <c r="C29" s="153"/>
-      <c r="D29" s="154" t="e">
+      <c r="C29" s="168"/>
+      <c r="D29" s="173" t="e">
         <f>CONCATENATE(TEXT($G$10-B29,"0,000"),"       ",TEXT(($G$10-B29)/B29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="155" t="str">
+      <c r="E29" s="174" t="str">
         <f t="shared" ref="E29:E33" si="1">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4785,17 +4776,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A30" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="154" t="e">
+      <c r="B30" s="167"/>
+      <c r="C30" s="168"/>
+      <c r="D30" s="173" t="e">
         <f>CONCATENATE(TEXT(G6-B30,"0,000"),"       ",TEXT((G6-B30)/B30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="155" t="str">
+      <c r="E30" s="174" t="str">
         <f t="shared" ref="E30" si="4">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4826,17 +4817,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A31" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="152"/>
-      <c r="C31" s="153"/>
-      <c r="D31" s="154" t="e">
+      <c r="B31" s="167"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="173" t="e">
         <f t="shared" ref="D31" si="5">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="155" t="str">
+      <c r="E31" s="174" t="str">
         <f t="shared" ref="E31:E32" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
@@ -4867,17 +4858,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="153"/>
-      <c r="D32" s="154" t="e">
+      <c r="B32" s="167"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="173" t="e">
         <f>CONCATENATE(TEXT(G8-B32+G9,"0,000"),"       ",TEXT((G8-B32+G9)/B32,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="155" t="str">
+      <c r="E32" s="174" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4908,20 +4899,20 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="152">
+      <c r="B33" s="167">
         <f>SUM(B34:C36)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="153"/>
-      <c r="D33" s="154" t="e">
+      <c r="C33" s="168"/>
+      <c r="D33" s="173" t="e">
         <f>CONCATENATE(TEXT(E10-B33,"0,000"),"       ",TEXT((E10-B33)/B33,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="155" t="str">
+      <c r="E33" s="174" t="str">
         <f t="shared" si="1"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4955,17 +4946,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A34" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="152"/>
-      <c r="C34" s="153"/>
-      <c r="D34" s="154" t="e">
+      <c r="B34" s="167"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="173" t="e">
         <f>CONCATENATE(TEXT(E6-B34,"0,000"),"       ",TEXT((E6-B34)/B34,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="155" t="str">
+      <c r="E34" s="174" t="str">
         <f t="shared" ref="E34" si="7">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4996,17 +4987,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A35" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="152"/>
-      <c r="C35" s="153"/>
-      <c r="D35" s="154" t="e">
+      <c r="B35" s="167"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="173" t="e">
         <f t="shared" ref="D35" si="8">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="155" t="str">
+      <c r="E35" s="174" t="str">
         <f t="shared" ref="E35:E37" si="9">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
@@ -5037,17 +5028,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A36" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="152"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="154" t="e">
+      <c r="B36" s="167"/>
+      <c r="C36" s="168"/>
+      <c r="D36" s="173" t="e">
         <f>CONCATENATE(TEXT(E8-B36+E9,"0,000"),"       ",TEXT((E8-B36+E9)/B36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="155" t="str">
+      <c r="E36" s="174" t="str">
         <f t="shared" si="9"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5078,17 +5069,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A37" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="153"/>
-      <c r="D37" s="154" t="e">
+      <c r="B37" s="167"/>
+      <c r="C37" s="168"/>
+      <c r="D37" s="173" t="e">
         <f>CONCATENATE(TEXT(C10-B37,"0,000"),"       ",TEXT((C10-B37)/B37,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="155" t="str">
+      <c r="E37" s="174" t="str">
         <f t="shared" si="9"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5119,25 +5110,25 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A38" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="161" t="e">
+      <c r="B38" s="213" t="e">
         <f>(B37+B33)/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="162"/>
-      <c r="D38" s="179" t="e">
+      <c r="C38" s="214"/>
+      <c r="D38" s="213" t="e">
         <f>F15-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="180"/>
+      <c r="E38" s="214"/>
       <c r="F38" s="60" t="e">
         <f>(F37+F33)/F29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="134" t="e">
+      <c r="G38" s="60" t="e">
         <f>F15-F38</f>
         <v>#DIV/0!</v>
       </c>
@@ -5163,7 +5154,7 @@
       </c>
       <c r="N38" s="132"/>
     </row>
-    <row r="39" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A39" s="49" t="s">
         <v>7</v>
       </c>
@@ -5176,7 +5167,7 @@
         <v>65</v>
       </c>
       <c r="H39" s="133"/>
-      <c r="I39" s="135" t="s">
+      <c r="I39" s="134" t="s">
         <v>68</v>
       </c>
       <c r="J39" s="133"/>
@@ -5185,18 +5176,18 @@
       <c r="M39" s="133"/>
       <c r="N39" s="133"/>
     </row>
-    <row r="40" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" ht="20.149999999999999" customHeight="1">
       <c r="A40" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="167" t="s">
+      <c r="B40" s="205" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="168"/>
-      <c r="D40" s="167" t="s">
+      <c r="C40" s="206"/>
+      <c r="D40" s="205" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="168"/>
+      <c r="E40" s="206"/>
       <c r="F40" s="69" t="s">
         <v>3</v>
       </c>
@@ -5211,119 +5202,119 @@
       <c r="M40" s="133"/>
       <c r="N40" s="133"/>
     </row>
-    <row r="41" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="12"/>
-      <c r="B41" s="136"/>
-      <c r="C41" s="137"/>
-      <c r="D41" s="138"/>
-      <c r="E41" s="139"/>
+      <c r="B41" s="203"/>
+      <c r="C41" s="204"/>
+      <c r="D41" s="211"/>
+      <c r="E41" s="212"/>
       <c r="F41" s="11"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="12"/>
-      <c r="B42" s="136"/>
-      <c r="C42" s="137"/>
-      <c r="D42" s="138"/>
-      <c r="E42" s="139"/>
+      <c r="B42" s="203"/>
+      <c r="C42" s="204"/>
+      <c r="D42" s="211"/>
+      <c r="E42" s="212"/>
       <c r="F42" s="11"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="12"/>
-      <c r="B43" s="136"/>
-      <c r="C43" s="137"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="139"/>
+      <c r="B43" s="203"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="211"/>
+      <c r="E43" s="212"/>
       <c r="F43" s="11"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="12"/>
-      <c r="B44" s="136"/>
-      <c r="C44" s="137"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="139"/>
+      <c r="B44" s="203"/>
+      <c r="C44" s="204"/>
+      <c r="D44" s="211"/>
+      <c r="E44" s="212"/>
       <c r="F44" s="11"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="12"/>
-      <c r="B45" s="136"/>
-      <c r="C45" s="137"/>
-      <c r="D45" s="138"/>
-      <c r="E45" s="139"/>
+      <c r="B45" s="203"/>
+      <c r="C45" s="204"/>
+      <c r="D45" s="211"/>
+      <c r="E45" s="212"/>
       <c r="F45" s="11"/>
       <c r="G45" s="13"/>
     </row>
-    <row r="46" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="12"/>
-      <c r="B46" s="136"/>
-      <c r="C46" s="137"/>
-      <c r="D46" s="138"/>
-      <c r="E46" s="139"/>
+      <c r="B46" s="203"/>
+      <c r="C46" s="204"/>
+      <c r="D46" s="211"/>
+      <c r="E46" s="212"/>
       <c r="F46" s="11"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="12"/>
-      <c r="B47" s="136"/>
-      <c r="C47" s="137"/>
-      <c r="D47" s="136"/>
-      <c r="E47" s="137"/>
+      <c r="B47" s="203"/>
+      <c r="C47" s="204"/>
+      <c r="D47" s="203"/>
+      <c r="E47" s="204"/>
       <c r="F47" s="11"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="12"/>
-      <c r="B48" s="136"/>
-      <c r="C48" s="137"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="137"/>
+      <c r="B48" s="203"/>
+      <c r="C48" s="204"/>
+      <c r="D48" s="203"/>
+      <c r="E48" s="204"/>
       <c r="F48" s="11"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="12"/>
-      <c r="B49" s="136"/>
-      <c r="C49" s="137"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="137"/>
+      <c r="B49" s="203"/>
+      <c r="C49" s="204"/>
+      <c r="D49" s="203"/>
+      <c r="E49" s="204"/>
       <c r="F49" s="11"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="12"/>
-      <c r="B50" s="136"/>
-      <c r="C50" s="137"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="137"/>
+      <c r="B50" s="203"/>
+      <c r="C50" s="204"/>
+      <c r="D50" s="203"/>
+      <c r="E50" s="204"/>
       <c r="F50" s="11"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:14" s="9" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="12"/>
-      <c r="B51" s="136"/>
-      <c r="C51" s="137"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="137"/>
+      <c r="B51" s="203"/>
+      <c r="C51" s="204"/>
+      <c r="D51" s="203"/>
+      <c r="E51" s="204"/>
       <c r="F51" s="11"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:14" ht="21.75" customHeight="1">
       <c r="A52" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="157">
+      <c r="B52" s="209">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="157"/>
-      <c r="D52" s="157">
+      <c r="C52" s="209"/>
+      <c r="D52" s="209">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="157"/>
+      <c r="E52" s="209"/>
       <c r="F52" s="64" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
@@ -5337,20 +5328,20 @@
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
     </row>
-    <row r="53" spans="1:14" ht="18" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:14" ht="18">
       <c r="A53" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="166">
+      <c r="B53" s="208">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="166"/>
-      <c r="D53" s="166">
+      <c r="C53" s="208"/>
+      <c r="D53" s="208">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="166"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="67">
         <f>F51-F49</f>
         <v>0</v>
@@ -5364,96 +5355,148 @@
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
     </row>
-    <row r="54" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="158"/>
-      <c r="B54" s="165"/>
-      <c r="C54" s="165"/>
-      <c r="D54" s="178"/>
-      <c r="E54" s="178"/>
-      <c r="F54" s="170"/>
-      <c r="G54" s="177"/>
+    <row r="54" spans="1:14" ht="25.5" customHeight="1">
+      <c r="A54" s="210"/>
+      <c r="B54" s="217"/>
+      <c r="C54" s="217"/>
+      <c r="D54" s="207"/>
+      <c r="E54" s="207"/>
+      <c r="F54" s="197"/>
+      <c r="G54" s="202"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="158"/>
-      <c r="B55" s="165"/>
-      <c r="C55" s="165"/>
-      <c r="D55" s="178"/>
-      <c r="E55" s="178"/>
-      <c r="F55" s="170"/>
-      <c r="G55" s="177"/>
+    <row r="55" spans="1:14" ht="27" customHeight="1">
+      <c r="A55" s="210"/>
+      <c r="B55" s="217"/>
+      <c r="C55" s="217"/>
+      <c r="D55" s="207"/>
+      <c r="E55" s="207"/>
+      <c r="F55" s="197"/>
+      <c r="G55" s="202"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:14" ht="27" customHeight="1">
       <c r="A56" s="5"/>
-      <c r="B56" s="169"/>
-      <c r="C56" s="169"/>
-      <c r="D56" s="169"/>
-      <c r="E56" s="169"/>
-      <c r="F56" s="169"/>
-      <c r="G56" s="169"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B56" s="196"/>
+      <c r="C56" s="196"/>
+      <c r="D56" s="196"/>
+      <c r="E56" s="196"/>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="5"/>
-      <c r="B57" s="169"/>
-      <c r="C57" s="169"/>
-      <c r="D57" s="169"/>
-      <c r="E57" s="169"/>
-      <c r="F57" s="169"/>
-      <c r="G57" s="169"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B57" s="196"/>
+      <c r="C57" s="196"/>
+      <c r="D57" s="196"/>
+      <c r="E57" s="196"/>
+      <c r="F57" s="196"/>
+      <c r="G57" s="196"/>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="5"/>
-      <c r="B58" s="169"/>
-      <c r="C58" s="169"/>
-      <c r="D58" s="169"/>
-      <c r="E58" s="169"/>
-      <c r="F58" s="169"/>
-      <c r="G58" s="169"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B58" s="196"/>
+      <c r="C58" s="196"/>
+      <c r="D58" s="196"/>
+      <c r="E58" s="196"/>
+      <c r="F58" s="196"/>
+      <c r="G58" s="196"/>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="5"/>
-      <c r="B59" s="169"/>
-      <c r="C59" s="169"/>
-      <c r="D59" s="169"/>
-      <c r="E59" s="169"/>
-      <c r="F59" s="169"/>
-      <c r="G59" s="169"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B59" s="196"/>
+      <c r="C59" s="196"/>
+      <c r="D59" s="196"/>
+      <c r="E59" s="196"/>
+      <c r="F59" s="196"/>
+      <c r="G59" s="196"/>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="5"/>
-      <c r="B60" s="169"/>
-      <c r="C60" s="169"/>
-      <c r="D60" s="169"/>
-      <c r="E60" s="169"/>
-      <c r="F60" s="169"/>
-      <c r="G60" s="169"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B60" s="196"/>
+      <c r="C60" s="196"/>
+      <c r="D60" s="196"/>
+      <c r="E60" s="196"/>
+      <c r="F60" s="196"/>
+      <c r="G60" s="196"/>
+    </row>
+    <row r="62" spans="1:14">
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:14">
       <c r="I64" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
@@ -5478,71 +5521,19 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B23:C25"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/06 週三 16:44:52.77
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F41C0-DA41-474F-A41E-1ECD025DE2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431B68E0-24F2-4CDD-9443-DBEDDC400AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="830" windowWidth="18150" windowHeight="8710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="X月" sheetId="2" r:id="rId1"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>上季</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1299,6 +1299,14 @@
 20220518-以修正，明細已無差異，待BU確認。</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>單位：千元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本月</t>
+    <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1320,7 +1328,7 @@
     <numFmt numFmtId="185" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="186" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="86">
+  <fonts count="85">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1603,12 +1611,6 @@
       <name val="標楷體"/>
       <family val="4"/>
       <charset val="136"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2103,7 +2105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -2563,6 +2565,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2707,7 +2718,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2753,16 +2764,16 @@
     <xf numFmtId="183" fontId="34" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="50" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="53" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="49" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="34" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="57" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="65" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="43" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="56" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="64" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="42" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="32" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2777,13 +2788,13 @@
     <xf numFmtId="176" fontId="32" fillId="0" borderId="14" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="69" fillId="33" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="69" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="68" fillId="33" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
@@ -2836,10 +2847,10 @@
     <xf numFmtId="182" fontId="22" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2847,9 +2858,6 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2892,118 +2900,118 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="69" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="68" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="51" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="50" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="68" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="67" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="66" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="67" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="63" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="50" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="65" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="66" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="46" applyFont="1"/>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="63" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="46" applyFont="1"/>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="59" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="58" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="56" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="55" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="55" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="54" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="50" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="46" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="40" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="39" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="39" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3024,25 +3032,10 @@
     <xf numFmtId="10" fontId="34" fillId="0" borderId="23" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="23" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="34" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="25" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="20" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="39" fillId="0" borderId="23" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="22" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3067,6 +3060,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="39" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="30" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="39" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="39" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="27" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
@@ -3079,16 +3085,16 @@
     <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3109,8 +3115,8 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -3123,7 +3129,7 @@
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3132,10 +3138,10 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3144,7 +3150,7 @@
     <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
@@ -3192,22 +3198,22 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3223,22 +3229,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3255,10 +3261,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="51" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="51" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="50" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="50" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3267,34 +3273,34 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="58" fillId="0" borderId="11" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="13" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="54" fillId="0" borderId="12" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="54" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="54" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="57" fillId="0" borderId="11" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="13" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="12" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="53" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3321,10 +3327,10 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3782,9 +3788,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3822,9 +3828,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3857,26 +3863,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3909,26 +3898,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4108,54 +4080,54 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:G20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="26" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.08984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="22" style="3" customWidth="1"/>
-    <col min="7" max="7" width="28.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.6328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" style="2" customWidth="1"/>
     <col min="10" max="10" width="19" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="19.6328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="16" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="175" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
       <c r="H1" s="27"/>
       <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
+      <c r="A2" s="212"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
       <c r="H2" s="27"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="219"/>
-      <c r="L2" s="219"/>
+      <c r="K2" s="218"/>
+      <c r="L2" s="218"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
@@ -4170,43 +4142,43 @@
       <c r="G3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
       <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="176" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="177" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="181"/>
-      <c r="F4" s="182" t="s">
+      <c r="E4" s="180"/>
+      <c r="F4" s="181" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="214" t="s">
+      <c r="G4" s="213" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="144"/>
+      <c r="A5" s="143"/>
       <c r="B5" s="33" t="s">
         <v>35</v>
       </c>
@@ -4219,18 +4191,18 @@
       <c r="E5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="215"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-    </row>
-    <row r="6" spans="1:15" ht="22" customHeight="1">
-      <c r="A6" s="67" t="s">
+      <c r="F5" s="182"/>
+      <c r="G5" s="214"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+    </row>
+    <row r="6" spans="1:15" ht="22.05" customHeight="1">
+      <c r="A6" s="66" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="34"/>
@@ -4242,19 +4214,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="220"/>
-      <c r="K6" s="220"/>
-      <c r="L6" s="73">
+      <c r="H6" s="71"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="219"/>
+      <c r="K6" s="219"/>
+      <c r="L6" s="72">
         <f>J6-G6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-    </row>
-    <row r="7" spans="1:15" ht="22" customHeight="1">
-      <c r="A7" s="67" t="s">
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+    </row>
+    <row r="7" spans="1:15" ht="22.05" customHeight="1">
+      <c r="A7" s="66" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="25"/>
@@ -4266,22 +4238,22 @@
         <v>0</v>
       </c>
       <c r="G7" s="23"/>
-      <c r="H7" s="74" t="s">
+      <c r="H7" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="75" t="s">
+      <c r="I7" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="220"/>
-      <c r="K7" s="220"/>
-      <c r="L7" s="73">
+      <c r="J7" s="219"/>
+      <c r="K7" s="219"/>
+      <c r="L7" s="72">
         <f>J7-G7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-    </row>
-    <row r="8" spans="1:15" ht="22" customHeight="1">
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+    </row>
+    <row r="8" spans="1:15" ht="22.05" customHeight="1">
       <c r="A8" s="33" t="s">
         <v>55</v>
       </c>
@@ -4294,25 +4266,25 @@
         <v>0</v>
       </c>
       <c r="G8" s="23"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="77">
+      <c r="H8" s="75"/>
+      <c r="I8" s="76">
         <f>H8-G8</f>
         <v>0</v>
       </c>
-      <c r="J8" s="78">
+      <c r="J8" s="77">
         <f>[1]SKL_TOL!$H$882</f>
         <v>0</v>
       </c>
-      <c r="K8" s="79">
+      <c r="K8" s="78">
         <f>J8-E8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="80"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-    </row>
-    <row r="9" spans="1:15" ht="22" customHeight="1">
-      <c r="A9" s="67" t="s">
+      <c r="L8" s="79"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+    </row>
+    <row r="9" spans="1:15" ht="22.05" customHeight="1">
+      <c r="A9" s="66" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="24"/>
@@ -4327,16 +4299,16 @@
         <f>F9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="76"/>
-      <c r="I9" s="77">
+      <c r="H9" s="75"/>
+      <c r="I9" s="76">
         <f>H9-F9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="81"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
     </row>
     <row r="10" spans="1:15" ht="34.5" customHeight="1">
       <c r="A10" s="35" t="s">
@@ -4366,16 +4338,16 @@
         <f>SUM(G6:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="82"/>
-      <c r="I10" s="77">
+      <c r="H10" s="81"/>
+      <c r="I10" s="76">
         <f>H10-G10</f>
         <v>0</v>
       </c>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
     </row>
     <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="36" t="s">
@@ -4383,846 +4355,920 @@
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="211" t="s">
+      <c r="D11" s="165"/>
+      <c r="E11" s="210" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="85">
+      <c r="F11" s="165"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="84">
         <f>H11-E10</f>
         <v>0</v>
       </c>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="192" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="216"/>
-      <c r="E12" s="212"/>
-      <c r="F12" s="167"/>
-      <c r="G12" s="167"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="193"/>
+      <c r="D12" s="215"/>
+      <c r="E12" s="211"/>
+      <c r="F12" s="166"/>
+      <c r="G12" s="166"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="195"/>
-      <c r="B13" s="196"/>
-      <c r="C13" s="196"/>
+      <c r="A13" s="194"/>
+      <c r="B13" s="195"/>
+      <c r="C13" s="195"/>
       <c r="D13" s="37"/>
-      <c r="E13" s="191" t="s">
+      <c r="E13" s="190" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="168" t="s">
+      <c r="F13" s="167" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="169"/>
-      <c r="H13" s="86" t="e">
+      <c r="G13" s="168"/>
+      <c r="H13" s="85" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="87" t="s">
+      <c r="I13" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-    </row>
-    <row r="14" spans="1:15" ht="18">
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+    </row>
+    <row r="14" spans="1:15" ht="17.399999999999999">
       <c r="A14" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="221" t="s">
+      <c r="B14" s="220" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="222"/>
+      <c r="C14" s="221"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="192"/>
-      <c r="F14" s="170" t="s">
+      <c r="E14" s="191"/>
+      <c r="F14" s="169" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="171"/>
+      <c r="G14" s="170"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="69"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="68"/>
     </row>
     <row r="15" spans="1:15" ht="19.5" customHeight="1">
       <c r="A15" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="217" t="s">
+      <c r="B15" s="216" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="218"/>
+      <c r="C15" s="217"/>
       <c r="D15" s="37"/>
-      <c r="E15" s="174" t="s">
+      <c r="E15" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="135" t="e">
+      <c r="F15" s="134" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="136"/>
+      <c r="G15" s="135"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="69"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="68"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="174" t="s">
+      <c r="A16" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="187" t="e">
+      <c r="B16" s="186" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="188"/>
+      <c r="C16" s="187"/>
       <c r="D16" s="37"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="137"/>
-      <c r="G16" s="138"/>
+      <c r="E16" s="174"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="137"/>
       <c r="H16" s="37"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-    </row>
-    <row r="17" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A17" s="175"/>
-      <c r="B17" s="189"/>
-      <c r="C17" s="190"/>
+      <c r="I16" s="88"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+    </row>
+    <row r="17" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A17" s="174"/>
+      <c r="B17" s="188"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="37"/>
       <c r="E17" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="141" t="e">
+      <c r="F17" s="140" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="142"/>
-      <c r="H17" s="90">
+      <c r="G17" s="141"/>
+      <c r="H17" s="89">
         <f>G10-H18</f>
         <v>0</v>
       </c>
-      <c r="I17" s="91">
+      <c r="I17" s="90">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J17" s="92" t="s">
+      <c r="J17" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-    </row>
-    <row r="18" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A18" s="201" t="s">
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+    </row>
+    <row r="18" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A18" s="200" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="202" t="e">
+      <c r="B18" s="201" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="203"/>
+      <c r="C18" s="202"/>
       <c r="D18" s="37"/>
       <c r="E18" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="139" t="e">
+      <c r="F18" s="138" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="140"/>
-      <c r="H18" s="90">
+      <c r="G18" s="139"/>
+      <c r="H18" s="89">
         <f>G7</f>
         <v>0</v>
       </c>
-      <c r="I18" s="93">
+      <c r="I18" s="92">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J18" s="94">
+      <c r="J18" s="93">
         <f>SUM(H17:H18)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-    </row>
-    <row r="19" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A19" s="201"/>
-      <c r="B19" s="202"/>
-      <c r="C19" s="203"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+    </row>
+    <row r="19" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A19" s="200"/>
+      <c r="B19" s="201"/>
+      <c r="C19" s="202"/>
       <c r="D19" s="37"/>
       <c r="E19" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="141" t="e">
+      <c r="F19" s="140" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="142"/>
-      <c r="H19" s="90">
+      <c r="G19" s="141"/>
+      <c r="H19" s="89">
         <f>G10-H20</f>
         <v>0</v>
       </c>
-      <c r="I19" s="93">
+      <c r="I19" s="92">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J19" s="94"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-    </row>
-    <row r="20" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A20" s="200" t="s">
+      <c r="J19" s="93"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
+    </row>
+    <row r="20" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A20" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="197"/>
-      <c r="C20" s="198"/>
+      <c r="B20" s="196"/>
+      <c r="C20" s="197"/>
       <c r="D20" s="37"/>
       <c r="E20" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="139" t="e">
+      <c r="F20" s="138" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="140"/>
+      <c r="G20" s="139"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="93">
+      <c r="I20" s="92">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J20" s="94">
+      <c r="J20" s="93">
         <f>SUM(H19:H20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-    </row>
-    <row r="21" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A21" s="200"/>
-      <c r="B21" s="197"/>
-      <c r="C21" s="198"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A21" s="199"/>
+      <c r="B21" s="196"/>
+      <c r="C21" s="197"/>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-    </row>
-    <row r="22" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A22" s="200"/>
-      <c r="B22" s="197"/>
-      <c r="C22" s="198"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="95"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A22" s="199"/>
+      <c r="B22" s="196"/>
+      <c r="C22" s="197"/>
       <c r="D22" s="37"/>
-      <c r="E22" s="143" t="s">
+      <c r="E22" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="143" t="s">
+      <c r="F22" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="143" t="s">
+      <c r="G22" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="90"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="69"/>
-    </row>
-    <row r="23" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A23" s="199" t="s">
+      <c r="H22" s="89"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+    </row>
+    <row r="23" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A23" s="198" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="204">
+      <c r="B23" s="203">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="205"/>
+      <c r="C23" s="204"/>
       <c r="D23" s="37"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-    </row>
-    <row r="24" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A24" s="199"/>
-      <c r="B24" s="204"/>
-      <c r="C24" s="205"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68"/>
+    </row>
+    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="198"/>
+      <c r="B24" s="203"/>
+      <c r="C24" s="204"/>
       <c r="D24" s="37"/>
       <c r="E24" s="44" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="96"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-    </row>
-    <row r="25" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A25" s="199"/>
-      <c r="B25" s="204"/>
-      <c r="C25" s="205"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="95"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+    </row>
+    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="198"/>
+      <c r="B25" s="203"/>
+      <c r="C25" s="204"/>
       <c r="D25" s="37"/>
       <c r="E25" s="45" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="98">
+      <c r="H25" s="96"/>
+      <c r="I25" s="97">
         <f>H25-B23</f>
         <v>0</v>
       </c>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-    </row>
-    <row r="26" spans="1:14" ht="27" customHeight="1">
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
+    </row>
+    <row r="26" spans="1:15" ht="27" customHeight="1">
       <c r="A26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="151"/>
-      <c r="C26" s="151"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="150"/>
       <c r="D26" s="47"/>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
       <c r="G26" s="32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H26" s="17"/>
-      <c r="I26" s="99" t="s">
+      <c r="I26" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="69"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="99"/>
+      <c r="L26" s="99"/>
+      <c r="M26" s="68"/>
       <c r="N26" s="37"/>
     </row>
-    <row r="27" spans="1:14" ht="19.149999999999999" customHeight="1">
-      <c r="A27" s="143" t="s">
+    <row r="27" spans="1:15" ht="19.2" customHeight="1">
+      <c r="A27" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="185"/>
-      <c r="D27" s="158" t="s">
+      <c r="B27" s="153"/>
+      <c r="C27" s="184"/>
+      <c r="D27" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="159"/>
-      <c r="F27" s="154"/>
+      <c r="E27" s="158"/>
+      <c r="F27" s="153"/>
       <c r="G27" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="101"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="209" t="s">
+      <c r="H27" s="100"/>
+      <c r="I27" s="101"/>
+      <c r="J27" s="208" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="210"/>
-      <c r="L27" s="206" t="s">
+      <c r="K27" s="209"/>
+      <c r="L27" s="205" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="207"/>
-      <c r="N27" s="208"/>
-    </row>
-    <row r="28" spans="1:14" ht="19.149999999999999" customHeight="1">
-      <c r="A28" s="184"/>
-      <c r="B28" s="155"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="145" t="s">
+      <c r="M27" s="206"/>
+      <c r="N27" s="207"/>
+      <c r="O27" s="125" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="19.2" customHeight="1">
+      <c r="A28" s="183"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="144" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="146"/>
-      <c r="F28" s="155"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="154"/>
       <c r="G28" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="103"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="108"/>
-      <c r="N28" s="109"/>
-    </row>
-    <row r="29" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="H28" s="102"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="105"/>
+      <c r="L28" s="106"/>
+      <c r="M28" s="107"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="125"/>
+    </row>
+    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="147">
-        <f>SUM(B30:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="148"/>
-      <c r="D29" s="149" t="e">
-        <f>CONCATENATE(TEXT($G$10-B29,"0,000"),"       ",TEXT(($G$10-B29)/B29,"0.00%"))</f>
+      <c r="B29" s="146">
+        <f t="shared" ref="B29:B37" si="1">H29/1000</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="147"/>
+      <c r="D29" s="148" t="e">
+        <f t="shared" ref="D29:D37" si="2">CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="150" t="str">
-        <f t="shared" ref="E29:E33" si="1">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
+      <c r="E29" s="149" t="str">
+        <f t="shared" ref="E29" si="3">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F29" s="51">
-        <f>SUM(F30:F32)</f>
+        <f t="shared" ref="F29:F37" si="4">L29/1000</f>
         <v>0</v>
       </c>
       <c r="G29" s="16" t="e">
-        <f>CONCATENATE(TEXT($G$10-F29,"0,000"),"       ",TEXT(($G$10-F29)/F29,"0.00%"))</f>
+        <f t="shared" ref="G29:G37" si="5">CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(N29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="110"/>
+      <c r="H29" s="109">
+        <f>SUM(H30:H32)</f>
+        <v>0</v>
+      </c>
       <c r="I29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="111">
-        <f>(G10-H29)</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="112" t="e">
-        <f t="shared" ref="K29:K35" si="2">J29/B29</f>
+      <c r="J29" s="113">
+        <f t="shared" ref="J29:J37" si="6">(O29-H29)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="111" t="e">
+        <f t="shared" ref="K29:K35" si="7">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="110"/>
-      <c r="M29" s="111">
-        <f>(G10-L29)</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="112" t="e">
-        <f t="shared" ref="N29:N35" si="3">M29/F29</f>
+      <c r="L29" s="109">
+        <f>SUM(L30:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="110">
+        <f t="shared" ref="M29:M37" si="8">(O29-L29)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="126" t="e">
+        <f t="shared" ref="N29:N35" si="9">M29/F29</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="O29" s="127">
+        <f>SUM(O30:O32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="147"/>
-      <c r="C30" s="148"/>
-      <c r="D30" s="149" t="e">
-        <f>CONCATENATE(TEXT(G6-B30,"0,000"),"       ",TEXT((G6-B30)/B30,"0.00%"))</f>
+      <c r="B30" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="150" t="str">
-        <f t="shared" ref="E30" si="4">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
+      <c r="E30" s="149" t="str">
+        <f t="shared" ref="E30:E34" si="10">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F30" s="53"/>
+      <c r="F30" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G30" s="16" t="e">
-        <f>CONCATENATE(TEXT(G6-F30,"0,000"),"       ",TEXT((G6-F30)/F30,"0.00%"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="113"/>
+      <c r="H30" s="112"/>
       <c r="I30" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="114">
-        <f>(G6-H30)</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="115" t="e">
+      <c r="J30" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="114" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" s="112"/>
+      <c r="M30" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="114" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O30" s="125"/>
+    </row>
+    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C31" s="147"/>
+      <c r="D31" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L30" s="113"/>
-      <c r="M30" s="116">
-        <f>(G6-L30)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="115" t="e">
-        <f t="shared" si="3"/>
+      <c r="E31" s="149" t="str">
+        <f t="shared" ref="E31" si="11">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
+        <v>108年度現階段累積達成率上月增減     0.00</v>
+      </c>
+      <c r="F31" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A31" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="147"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="149" t="e">
-        <f t="shared" ref="D31" si="5">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="150" t="str">
-        <f t="shared" ref="E31:E32" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
-        <v>108年度現階段累積達成率上月增減     0.00</v>
-      </c>
-      <c r="F31" s="53"/>
-      <c r="G31" s="16" t="e">
-        <f>CONCATENATE(TEXT(G7-F31,"0,000"),"       ",TEXT((G7-F31)/F31,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H31" s="113"/>
+      <c r="H31" s="112"/>
       <c r="I31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="114">
-        <f>(G7-H31)</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="115" t="e">
+      <c r="J31" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="114" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="112"/>
+      <c r="M31" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="114" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" s="125"/>
+    </row>
+    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C32" s="147"/>
+      <c r="D32" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L31" s="113"/>
-      <c r="M31" s="116">
-        <f>(G7-L31)</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="115" t="e">
-        <f t="shared" si="3"/>
+      <c r="E32" s="149" t="str">
+        <f t="shared" ref="E32:E33" si="12">CONCATENATE("108年度現階段累積達成率",TEXT(J28,"0.00%"),"     ",TEXT(J24,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F32" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A32" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="147"/>
-      <c r="C32" s="148"/>
-      <c r="D32" s="149" t="e">
-        <f>CONCATENATE(TEXT(G8-B32+G9,"0,000"),"       ",TEXT((G8-B32+G9)/B32,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="150" t="str">
-        <f t="shared" si="6"/>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F32" s="53"/>
-      <c r="G32" s="16" t="e">
-        <f>CONCATENATE(TEXT(G8-F32+G9,"0,000"),"       ",TEXT((G8-F32+G9)/F32,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H32" s="113"/>
+      <c r="H32" s="112"/>
       <c r="I32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="117">
-        <f>(G8-H32+G9)</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="118" t="e">
+      <c r="J32" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="115" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L32" s="112"/>
+      <c r="M32" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="115" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O32" s="125"/>
+    </row>
+    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C33" s="147"/>
+      <c r="D33" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L32" s="113"/>
-      <c r="M32" s="119">
-        <f>(G8-L32+G9)</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="118" t="e">
-        <f t="shared" si="3"/>
+      <c r="E33" s="149" t="str">
+        <f t="shared" si="12"/>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F33" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A33" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="147">
-        <f>SUM(B34:C36)</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="148"/>
-      <c r="D33" s="149" t="e">
-        <f>CONCATENATE(TEXT(E10-B33,"0,000"),"       ",TEXT((E10-B33)/B33,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="150" t="str">
-        <f t="shared" si="1"/>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F33" s="53">
-        <f>SUM(F34:F36)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="16" t="e">
-        <f>CONCATENATE(TEXT(E10-F33,"0,000"),"       ",TEXT((E10-F33)/F33,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H33" s="110"/>
+      <c r="H33" s="110">
+        <f>SUM(H34:H36)</f>
+        <v>0</v>
+      </c>
       <c r="I33" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="111">
-        <f>(E10-H33)</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="112" t="e">
+      <c r="J33" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="111" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L33" s="110">
+        <f>SUM(L34:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="126" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O33" s="128">
+        <f>SUM(O34:O36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C34" s="147"/>
+      <c r="D34" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L33" s="110"/>
-      <c r="M33" s="120">
-        <f>(E10-L33)</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="112" t="e">
-        <f t="shared" si="3"/>
+      <c r="E34" s="149" t="str">
+        <f t="shared" si="10"/>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F34" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A34" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="147"/>
-      <c r="C34" s="148"/>
-      <c r="D34" s="149" t="e">
-        <f>CONCATENATE(TEXT(E6-B34,"0,000"),"       ",TEXT((E6-B34)/B34,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="150" t="str">
-        <f t="shared" ref="E34" si="7">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F34" s="53"/>
-      <c r="G34" s="16" t="e">
-        <f>CONCATENATE(TEXT(E6-F34,"0,000"),"       ",TEXT((E6-F34)/F34,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="121"/>
+      <c r="H34" s="116"/>
       <c r="I34" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="114">
-        <f>(E6-H34)</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="115" t="e">
+      <c r="J34" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="114" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L34" s="112"/>
+      <c r="M34" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="114" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O34" s="125"/>
+    </row>
+    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C35" s="147"/>
+      <c r="D35" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L34" s="113"/>
-      <c r="M34" s="116">
-        <f>(E6-L34)</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="115" t="e">
-        <f t="shared" si="3"/>
+      <c r="E35" s="149" t="str">
+        <f t="shared" ref="E35" si="13">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     上月增減</v>
+      </c>
+      <c r="F35" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A35" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="147"/>
-      <c r="C35" s="148"/>
-      <c r="D35" s="149" t="e">
-        <f t="shared" ref="D35" si="8">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E35" s="150" t="str">
-        <f t="shared" ref="E35:E37" si="9">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     上月增減</v>
-      </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="16" t="e">
-        <f>CONCATENATE(TEXT(E7-F35,"0,000"),"       ",TEXT((E7-F35)/F35,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H35" s="121"/>
+      <c r="H35" s="116"/>
       <c r="I35" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="122">
-        <f>(E7-H35)</f>
-        <v>0</v>
-      </c>
-      <c r="K35" s="115" t="e">
+      <c r="J35" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="114" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" s="112"/>
+      <c r="M35" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="114" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O35" s="125"/>
+    </row>
+    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C36" s="147"/>
+      <c r="D36" s="148" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="113"/>
-      <c r="M35" s="116">
-        <f>(E7-L35)</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="115" t="e">
-        <f t="shared" si="3"/>
+      <c r="E36" s="149" t="str">
+        <f t="shared" ref="E36" si="14">CONCATENATE("108年度現階段累積達成率",TEXT(J32,"0.00%"),"     ",TEXT(J28,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F36" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="16" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A36" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="147"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="149" t="e">
-        <f>CONCATENATE(TEXT(E8-B36+E9,"0,000"),"       ",TEXT((E8-B36+E9)/B36,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E36" s="150" t="str">
-        <f t="shared" si="9"/>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="16" t="e">
-        <f>CONCATENATE(TEXT(E8-F36,"0,000"),"       ",TEXT((E8-F36)/F36,"0.00%"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H36" s="121"/>
+      <c r="H36" s="116"/>
       <c r="I36" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="117">
-        <f>(E8-H36+E9)</f>
-        <v>0</v>
-      </c>
-      <c r="K36" s="115" t="e">
+      <c r="J36" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="114" t="e">
         <f>J36/B36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="123"/>
-      <c r="M36" s="119">
-        <f>(E8-L36)</f>
-        <v>0</v>
-      </c>
-      <c r="N36" s="118" t="e">
+      <c r="L36" s="117"/>
+      <c r="M36" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="115" t="e">
         <f>M36/F36</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A37" s="55" t="s">
+      <c r="O36" s="125"/>
+    </row>
+    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="147"/>
-      <c r="C37" s="148"/>
-      <c r="D37" s="149" t="e">
-        <f>CONCATENATE(TEXT(C10-B37,"0,000"),"       ",TEXT((C10-B37)/B37,"0.00%"))</f>
+      <c r="B37" s="146">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C37" s="147"/>
+      <c r="D37" s="148" t="e">
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="150" t="str">
-        <f t="shared" si="9"/>
+      <c r="E37" s="149" t="str">
+        <f t="shared" ref="E37" si="15">CONCATENATE("108年度現階段累積達成率",TEXT(J33,"0.00%"),"     ",TEXT(J29,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F37" s="53"/>
+      <c r="F37" s="51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G37" s="16" t="e">
-        <f>CONCATENATE(TEXT(C10-F37,"0,000"),"       ",TEXT((C10-F37)/F37,"0.00%"))</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="121"/>
+      <c r="H37" s="116"/>
       <c r="I37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="124">
-        <f>(C10-H37)</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="125" t="e">
+      <c r="J37" s="113">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="119" t="e">
         <f>J37/B37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L37" s="126"/>
-      <c r="M37" s="124">
-        <f>(C10-L37)</f>
-        <v>0</v>
-      </c>
-      <c r="N37" s="125" t="e">
+      <c r="L37" s="120"/>
+      <c r="M37" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="119" t="e">
         <f>M37/F37</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A38" s="56" t="s">
+      <c r="O37" s="125"/>
+    </row>
+    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="156" t="e">
-        <f>(B37+B33)/B29</f>
+      <c r="B38" s="155" t="e">
+        <f>H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="157"/>
-      <c r="D38" s="156" t="e">
-        <f>F15-B38</f>
+      <c r="C38" s="156"/>
+      <c r="D38" s="155" t="e">
+        <f>J38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="157"/>
-      <c r="F38" s="57" t="e">
-        <f>(F37+F33)/F29</f>
+      <c r="E38" s="156"/>
+      <c r="F38" s="129" t="e">
+        <f>L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="57" t="e">
-        <f>F15-F38</f>
+      <c r="G38" s="56" t="e">
+        <f>M38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="127" t="e">
-        <f>(H33+H37)/H29</f>
+      <c r="H38" s="121" t="e">
+        <f>H27/H28</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="128" t="e">
+      <c r="J38" s="122" t="e">
         <f>F15-H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="124"/>
-      <c r="L38" s="127" t="e">
+      <c r="K38" s="118"/>
+      <c r="L38" s="121" t="e">
         <f>(L33+L37)/L29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M38" s="128" t="e">
+      <c r="M38" s="122" t="e">
         <f>F15-L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N38" s="129"/>
-    </row>
-    <row r="39" spans="1:14" ht="20.149999999999999" customHeight="1">
+      <c r="N38" s="123"/>
+      <c r="O38" s="125"/>
+    </row>
+    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="46" t="s">
         <v>7</v>
       </c>
@@ -5230,12 +5276,12 @@
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
-      <c r="F39" s="58"/>
+      <c r="F39" s="57"/>
       <c r="G39" s="32" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="130" t="s">
+      <c r="I39" s="124" t="s">
         <v>68</v>
       </c>
       <c r="J39" s="6"/>
@@ -5244,25 +5290,25 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:14" ht="20.149999999999999" customHeight="1">
-      <c r="A40" s="59" t="s">
+    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="162" t="s">
+      <c r="B40" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="163"/>
-      <c r="D40" s="162" t="s">
+      <c r="C40" s="162"/>
+      <c r="D40" s="161" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="163"/>
-      <c r="F40" s="66" t="s">
+      <c r="E40" s="162"/>
+      <c r="F40" s="65" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="69"/>
+      <c r="H40" s="68"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -5270,124 +5316,124 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="131"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="133"/>
-      <c r="E41" s="134"/>
+      <c r="B41" s="130"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="133"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="131"/>
-      <c r="C42" s="132"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="134"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="132"/>
+      <c r="E42" s="133"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="131"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="134"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="131"/>
+      <c r="D43" s="132"/>
+      <c r="E43" s="133"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="131"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="134"/>
+      <c r="B44" s="130"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="133"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="131"/>
-      <c r="C45" s="132"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="134"/>
+      <c r="B45" s="130"/>
+      <c r="C45" s="131"/>
+      <c r="D45" s="132"/>
+      <c r="E45" s="133"/>
       <c r="F45" s="8"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="131"/>
-      <c r="C46" s="132"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="134"/>
+      <c r="B46" s="130"/>
+      <c r="C46" s="131"/>
+      <c r="D46" s="132"/>
+      <c r="E46" s="133"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="132"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="132"/>
+      <c r="B47" s="130"/>
+      <c r="C47" s="131"/>
+      <c r="D47" s="130"/>
+      <c r="E47" s="131"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="132"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="132"/>
+      <c r="B48" s="130"/>
+      <c r="C48" s="131"/>
+      <c r="D48" s="130"/>
+      <c r="E48" s="131"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="131"/>
-      <c r="E49" s="132"/>
+      <c r="B49" s="130"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="131"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="131"/>
-      <c r="C50" s="132"/>
-      <c r="D50" s="131"/>
-      <c r="E50" s="132"/>
+      <c r="B50" s="130"/>
+      <c r="C50" s="131"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="131"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="130"/>
+      <c r="E51" s="131"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="152">
+      <c r="B52" s="151">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="152"/>
-      <c r="D52" s="152">
+      <c r="C52" s="151"/>
+      <c r="D52" s="151">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="152"/>
-      <c r="F52" s="61" t="e">
+      <c r="E52" s="151"/>
+      <c r="F52" s="60" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G52" s="62"/>
+      <c r="G52" s="61"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
@@ -5396,25 +5442,25 @@
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
     </row>
-    <row r="53" spans="1:14" ht="18">
-      <c r="A53" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="161">
+    <row r="53" spans="1:14" ht="17.399999999999999">
+      <c r="A53" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="160">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="161"/>
-      <c r="D53" s="161">
+      <c r="C53" s="160"/>
+      <c r="D53" s="160">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="161"/>
-      <c r="F53" s="64">
+      <c r="E53" s="160"/>
+      <c r="F53" s="63">
         <f>F51-F49</f>
         <v>0</v>
       </c>
-      <c r="G53" s="65"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
@@ -5424,63 +5470,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="153"/>
-      <c r="B54" s="160"/>
-      <c r="C54" s="160"/>
-      <c r="D54" s="173"/>
-      <c r="E54" s="173"/>
-      <c r="F54" s="165"/>
-      <c r="G54" s="172"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="159"/>
+      <c r="C54" s="159"/>
+      <c r="D54" s="172"/>
+      <c r="E54" s="172"/>
+      <c r="F54" s="164"/>
+      <c r="G54" s="171"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="153"/>
-      <c r="B55" s="160"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="173"/>
-      <c r="E55" s="173"/>
-      <c r="F55" s="165"/>
-      <c r="G55" s="172"/>
+      <c r="A55" s="152"/>
+      <c r="B55" s="159"/>
+      <c r="C55" s="159"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="172"/>
+      <c r="F55" s="164"/>
+      <c r="G55" s="171"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="164"/>
-      <c r="C56" s="164"/>
-      <c r="D56" s="164"/>
-      <c r="E56" s="164"/>
-      <c r="F56" s="164"/>
-      <c r="G56" s="164"/>
+      <c r="B56" s="163"/>
+      <c r="C56" s="163"/>
+      <c r="D56" s="163"/>
+      <c r="E56" s="163"/>
+      <c r="F56" s="163"/>
+      <c r="G56" s="163"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="164"/>
-      <c r="C57" s="164"/>
-      <c r="D57" s="164"/>
-      <c r="E57" s="164"/>
-      <c r="F57" s="164"/>
-      <c r="G57" s="164"/>
+      <c r="B57" s="163"/>
+      <c r="C57" s="163"/>
+      <c r="D57" s="163"/>
+      <c r="E57" s="163"/>
+      <c r="F57" s="163"/>
+      <c r="G57" s="163"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="164"/>
-      <c r="C58" s="164"/>
-      <c r="D58" s="164"/>
-      <c r="E58" s="164"/>
-      <c r="F58" s="164"/>
-      <c r="G58" s="164"/>
+      <c r="B58" s="163"/>
+      <c r="C58" s="163"/>
+      <c r="D58" s="163"/>
+      <c r="E58" s="163"/>
+      <c r="F58" s="163"/>
+      <c r="G58" s="163"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="164"/>
-      <c r="C59" s="164"/>
-      <c r="D59" s="164"/>
-      <c r="E59" s="164"/>
-      <c r="F59" s="164"/>
-      <c r="G59" s="164"/>
+      <c r="B59" s="163"/>
+      <c r="C59" s="163"/>
+      <c r="D59" s="163"/>
+      <c r="E59" s="163"/>
+      <c r="F59" s="163"/>
+      <c r="G59" s="163"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="164"/>
-      <c r="C60" s="164"/>
-      <c r="D60" s="164"/>
-      <c r="E60" s="164"/>
-      <c r="F60" s="164"/>
-      <c r="G60" s="164"/>
+      <c r="B60" s="163"/>
+      <c r="C60" s="163"/>
+      <c r="D60" s="163"/>
+      <c r="E60" s="163"/>
+      <c r="F60" s="163"/>
+      <c r="G60" s="163"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>
@@ -5600,7 +5646,7 @@
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.31496062992125984" bottom="0" header="0.19685039370078741" footer="0"/>
-  <pageSetup paperSize="9" scale="79" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;R機密等級：密等</oddHeader>
     <oddFooter>&amp;L&amp;"標楷體,標準"&amp;10放款部 放款管理課製表 &amp;D</oddFooter>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/26 週二 11:42:52.85
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431B68E0-24F2-4CDD-9443-DBEDDC400AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4307A851-43E2-4708-A052-DCC11719C7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="X月" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
@@ -177,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>上季</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1299,14 +1296,6 @@
 20220518-以修正，明細已無差異，待BU確認。</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>單位：千元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本月</t>
-    <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1328,7 +1317,7 @@
     <numFmt numFmtId="185" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
     <numFmt numFmtId="186" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="85">
+  <fonts count="86">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1611,6 +1600,12 @@
       <name val="標楷體"/>
       <family val="4"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2105,7 +2100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -2565,15 +2560,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2718,7 +2704,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2764,16 +2750,16 @@
     <xf numFmtId="183" fontId="34" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="49" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="52" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="50" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="53" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="34" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="56" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="64" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="42" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="57" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="65" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="43" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="32" fillId="0" borderId="11" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2788,13 +2774,13 @@
     <xf numFmtId="176" fontId="32" fillId="0" borderId="14" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="68" fillId="33" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="69" fillId="33" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
@@ -2847,10 +2833,10 @@
     <xf numFmtId="182" fontId="22" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2858,6 +2844,9 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2900,118 +2889,118 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="176" fontId="69" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="51" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="68" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="68" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="50" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="66" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="67" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="67" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="63" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="50" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="65" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="66" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="63" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="46" applyFont="1"/>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="46" applyFont="1"/>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="59" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="52" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="56" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="178" fontId="55" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="58" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="51" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="55" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="178" fontId="54" fillId="0" borderId="0" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="50" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="46" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="40" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="39" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="39" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3032,10 +3021,25 @@
     <xf numFmtId="10" fontId="34" fillId="0" borderId="23" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="23" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="34" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="25" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="20" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="39" fillId="0" borderId="23" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="22" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3060,191 +3064,140 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="39" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="30" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="35" fillId="0" borderId="39" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="39" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="27" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="41" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="52" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="74" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="45" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3261,10 +3214,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="50" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="50" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3273,70 +3226,108 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="57" fillId="0" borderId="11" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="13" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="12" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="53" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="58" fillId="0" borderId="11" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="13" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="54" fillId="0" borderId="12" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="54" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="54" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="61" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="40" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3733,60 +3724,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="請求訊息"/>
-      <sheetName val="匯率記錄"/>
-      <sheetName val="SKL_TOL"/>
-      <sheetName val="SKL000_ALL"/>
-      <sheetName val="SKL000_AUD"/>
-      <sheetName val="SKL000_CNY"/>
-      <sheetName val="SKL000_EUD"/>
-      <sheetName val="SKL000_NTD"/>
-      <sheetName val="SKL000_USD"/>
-      <sheetName val="SKL000_00A_ALL"/>
-      <sheetName val="SKL000_00A_AUD"/>
-      <sheetName val="SKL000_00A_CNY"/>
-      <sheetName val="SKL000_00A_EUD"/>
-      <sheetName val="SKL000_00A_NTD"/>
-      <sheetName val="SKL000_00A_USD"/>
-      <sheetName val="XDO_METADATA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="870">
-          <cell r="K870">
-            <v>107253510700</v>
-          </cell>
-        </row>
-        <row r="882">
-          <cell r="H882">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -4081,7 +4018,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -4104,30 +4041,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="152" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
       <c r="H1" s="27"/>
       <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="212"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
+      <c r="A2" s="138"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
       <c r="H2" s="27"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="218"/>
-      <c r="L2" s="218"/>
+      <c r="K2" s="148"/>
+      <c r="L2" s="148"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
@@ -4142,43 +4079,43 @@
       <c r="G3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
       <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="155" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="179" t="s">
+      <c r="C4" s="156"/>
+      <c r="D4" s="157" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="180"/>
-      <c r="F4" s="181" t="s">
+      <c r="E4" s="158"/>
+      <c r="F4" s="159" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="213" t="s">
+      <c r="G4" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="143"/>
+      <c r="A5" s="154"/>
       <c r="B5" s="33" t="s">
         <v>35</v>
       </c>
@@ -4191,18 +4128,18 @@
       <c r="E5" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="182"/>
-      <c r="G5" s="214"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="67" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="34"/>
@@ -4214,19 +4151,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="219"/>
-      <c r="K6" s="219"/>
-      <c r="L6" s="72">
+      <c r="H6" s="72"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="73">
         <f>J6-G6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
     </row>
     <row r="7" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="67" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="25"/>
@@ -4238,20 +4175,20 @@
         <v>0</v>
       </c>
       <c r="G7" s="23"/>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="74" t="s">
+      <c r="I7" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="219"/>
-      <c r="K7" s="219"/>
-      <c r="L7" s="72">
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="73">
         <f>J7-G7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
     </row>
     <row r="8" spans="1:15" ht="22.05" customHeight="1">
       <c r="A8" s="33" t="s">
@@ -4266,25 +4203,22 @@
         <v>0</v>
       </c>
       <c r="G8" s="23"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="76">
+      <c r="H8" s="76"/>
+      <c r="I8" s="77">
         <f>H8-G8</f>
         <v>0</v>
       </c>
-      <c r="J8" s="77">
-        <f>[1]SKL_TOL!$H$882</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="78">
+      <c r="J8" s="78"/>
+      <c r="K8" s="79">
         <f>J8-E8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="79"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
     </row>
     <row r="9" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="67" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="24"/>
@@ -4299,16 +4233,16 @@
         <f>F9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76">
+      <c r="H9" s="76"/>
+      <c r="I9" s="77">
         <f>H9-F9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
     </row>
     <row r="10" spans="1:15" ht="34.5" customHeight="1">
       <c r="A10" s="35" t="s">
@@ -4338,16 +4272,16 @@
         <f>SUM(G6:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="81"/>
-      <c r="I10" s="76">
+      <c r="H10" s="82"/>
+      <c r="I10" s="77">
         <f>H10-G10</f>
         <v>0</v>
       </c>
-      <c r="J10" s="82"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
     </row>
     <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="A11" s="36" t="s">
@@ -4355,920 +4289,846 @@
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
-      <c r="D11" s="165"/>
-      <c r="E11" s="210" t="s">
+      <c r="D11" s="141"/>
+      <c r="E11" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="165"/>
-      <c r="G11" s="165"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84">
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="85">
         <f>H11-E10</f>
         <v>0</v>
       </c>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="192" t="s">
+      <c r="A12" s="179" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="193"/>
-      <c r="C12" s="193"/>
-      <c r="D12" s="215"/>
-      <c r="E12" s="211"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="166"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="142"/>
+      <c r="G12" s="142"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="194"/>
-      <c r="B13" s="195"/>
-      <c r="C13" s="195"/>
+      <c r="A13" s="181"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="182"/>
       <c r="D13" s="37"/>
-      <c r="E13" s="190" t="s">
+      <c r="E13" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="167" t="s">
+      <c r="F13" s="194" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="168"/>
-      <c r="H13" s="85" t="e">
+      <c r="G13" s="195"/>
+      <c r="H13" s="86" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="86" t="s">
+      <c r="I13" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
     </row>
     <row r="14" spans="1:15" ht="17.399999999999999">
       <c r="A14" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="220" t="s">
+      <c r="B14" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="221"/>
+      <c r="C14" s="151"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="191"/>
-      <c r="F14" s="169" t="s">
+      <c r="E14" s="178"/>
+      <c r="F14" s="196" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="170"/>
+      <c r="G14" s="197"/>
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="68"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="69"/>
     </row>
     <row r="15" spans="1:15" ht="19.5" customHeight="1">
       <c r="A15" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="216" t="s">
+      <c r="B15" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="217"/>
+      <c r="C15" s="147"/>
       <c r="D15" s="37"/>
-      <c r="E15" s="173" t="s">
+      <c r="E15" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="134" t="e">
+      <c r="F15" s="214" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="135"/>
+      <c r="G15" s="215"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="68"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="69"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="173" t="s">
+      <c r="A16" s="144" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="186" t="e">
+      <c r="B16" s="173" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="187"/>
+      <c r="C16" s="174"/>
       <c r="D16" s="37"/>
-      <c r="E16" s="174"/>
-      <c r="F16" s="136"/>
-      <c r="G16" s="137"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="216"/>
+      <c r="G16" s="217"/>
       <c r="H16" s="37"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
-    </row>
-    <row r="17" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A17" s="174"/>
-      <c r="B17" s="188"/>
-      <c r="C17" s="189"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+    </row>
+    <row r="17" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A17" s="145"/>
+      <c r="B17" s="175"/>
+      <c r="C17" s="176"/>
       <c r="D17" s="37"/>
       <c r="E17" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="140" t="e">
+      <c r="F17" s="171" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="141"/>
-      <c r="H17" s="89">
+      <c r="G17" s="172"/>
+      <c r="H17" s="90">
         <f>G10-H18</f>
         <v>0</v>
       </c>
-      <c r="I17" s="90">
+      <c r="I17" s="91">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J17" s="91" t="s">
+      <c r="J17" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
-      <c r="N17" s="68"/>
-    </row>
-    <row r="18" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A18" s="200" t="s">
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+    </row>
+    <row r="18" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A18" s="187" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="201" t="e">
+      <c r="B18" s="188" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="202"/>
+      <c r="C18" s="189"/>
       <c r="D18" s="37"/>
       <c r="E18" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="138" t="e">
+      <c r="F18" s="218" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="139"/>
-      <c r="H18" s="89">
+      <c r="G18" s="219"/>
+      <c r="H18" s="90">
         <f>G7</f>
         <v>0</v>
       </c>
-      <c r="I18" s="92">
+      <c r="I18" s="93">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J18" s="93">
+      <c r="J18" s="94">
         <f>SUM(H17:H18)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-    </row>
-    <row r="19" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A19" s="200"/>
-      <c r="B19" s="201"/>
-      <c r="C19" s="202"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+    </row>
+    <row r="19" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A19" s="187"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="189"/>
       <c r="D19" s="37"/>
       <c r="E19" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="140" t="e">
+      <c r="F19" s="171" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="141"/>
-      <c r="H19" s="89">
+      <c r="G19" s="172"/>
+      <c r="H19" s="90">
         <f>G10-H20</f>
         <v>0</v>
       </c>
-      <c r="I19" s="92">
+      <c r="I19" s="93">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J19" s="93"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-    </row>
-    <row r="20" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A20" s="199" t="s">
+      <c r="J19" s="94"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+    </row>
+    <row r="20" spans="1:14" ht="17.25" customHeight="1">
+      <c r="A20" s="186" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="196"/>
-      <c r="C20" s="197"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="184"/>
       <c r="D20" s="37"/>
       <c r="E20" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="138" t="e">
+      <c r="F20" s="218" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="139"/>
+      <c r="G20" s="219"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="92">
+      <c r="I20" s="93">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J20" s="93">
+      <c r="J20" s="94">
         <f>SUM(H19:H20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-    </row>
-    <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="199"/>
-      <c r="B21" s="196"/>
-      <c r="C21" s="197"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+    </row>
+    <row r="21" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A21" s="186"/>
+      <c r="B21" s="183"/>
+      <c r="C21" s="184"/>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-    </row>
-    <row r="22" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A22" s="199"/>
-      <c r="B22" s="196"/>
-      <c r="C22" s="197"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="96"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+    </row>
+    <row r="22" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A22" s="186"/>
+      <c r="B22" s="183"/>
+      <c r="C22" s="184"/>
       <c r="D22" s="37"/>
-      <c r="E22" s="142" t="s">
+      <c r="E22" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="142" t="s">
+      <c r="F22" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="142" t="s">
+      <c r="G22" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="89"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-    </row>
-    <row r="23" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A23" s="198" t="s">
+      <c r="H22" s="90"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+    </row>
+    <row r="23" spans="1:14" ht="16.5" customHeight="1">
+      <c r="A23" s="185" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="203">
+      <c r="B23" s="190">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="204"/>
+      <c r="C23" s="191"/>
       <c r="D23" s="37"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="198"/>
-      <c r="B24" s="203"/>
-      <c r="C24" s="204"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
+    </row>
+    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="185"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="191"/>
       <c r="D24" s="37"/>
       <c r="E24" s="44" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-    </row>
-    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="198"/>
-      <c r="B25" s="203"/>
-      <c r="C25" s="204"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="96"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+    </row>
+    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="185"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="191"/>
       <c r="D25" s="37"/>
       <c r="E25" s="45" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="97">
+      <c r="H25" s="97"/>
+      <c r="I25" s="98">
         <f>H25-B23</f>
         <v>0</v>
       </c>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
-      <c r="L25" s="68"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="68"/>
-    </row>
-    <row r="26" spans="1:15" ht="27" customHeight="1">
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="69"/>
+    </row>
+    <row r="26" spans="1:14" ht="27" customHeight="1">
       <c r="A26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="150"/>
-      <c r="C26" s="150"/>
+      <c r="B26" s="222"/>
+      <c r="C26" s="222"/>
       <c r="D26" s="47"/>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
       <c r="G26" s="32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H26" s="17"/>
-      <c r="I26" s="98" t="s">
+      <c r="I26" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="99"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="99"/>
-      <c r="M26" s="68"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="69"/>
       <c r="N26" s="37"/>
     </row>
-    <row r="27" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A27" s="142" t="s">
+    <row r="27" spans="1:14" ht="19.2" customHeight="1">
+      <c r="A27" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="153"/>
-      <c r="C27" s="184"/>
-      <c r="D27" s="157" t="s">
+      <c r="B27" s="165"/>
+      <c r="C27" s="166"/>
+      <c r="D27" s="211" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="158"/>
-      <c r="F27" s="153"/>
+      <c r="E27" s="212"/>
+      <c r="F27" s="165"/>
       <c r="G27" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="100"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="208" t="s">
+      <c r="H27" s="101"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="209"/>
-      <c r="L27" s="205" t="s">
+      <c r="K27" s="135"/>
+      <c r="L27" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="206"/>
-      <c r="N27" s="207"/>
-      <c r="O27" s="125" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A28" s="183"/>
-      <c r="B28" s="154"/>
-      <c r="C28" s="185"/>
-      <c r="D28" s="144" t="s">
+      <c r="M27" s="132"/>
+      <c r="N27" s="133"/>
+    </row>
+    <row r="28" spans="1:14" ht="19.2" customHeight="1">
+      <c r="A28" s="162"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="168"/>
+      <c r="D28" s="220" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="145"/>
-      <c r="F28" s="154"/>
+      <c r="E28" s="221"/>
+      <c r="F28" s="167"/>
       <c r="G28" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="102"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="104"/>
-      <c r="K28" s="105"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="108"/>
-      <c r="O28" s="125"/>
-    </row>
-    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H28" s="103"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="105"/>
+      <c r="K28" s="106"/>
+      <c r="L28" s="107"/>
+      <c r="M28" s="108"/>
+      <c r="N28" s="109"/>
+    </row>
+    <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="146">
-        <f t="shared" ref="B29:B37" si="1">H29/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="147"/>
-      <c r="D29" s="148" t="e">
-        <f t="shared" ref="D29:D37" si="2">CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
+      <c r="B29" s="163">
+        <f>SUM(B30:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="164"/>
+      <c r="D29" s="169" t="e">
+        <f>CONCATENATE(TEXT($G$10-B29,"0,000"),"       ",TEXT(($G$10-B29)/B29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="149" t="str">
-        <f t="shared" ref="E29" si="3">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
+      <c r="E29" s="170" t="str">
+        <f t="shared" ref="E29:E33" si="1">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F29" s="51">
-        <f t="shared" ref="F29:F37" si="4">L29/1000</f>
+        <f>SUM(F30:F32)</f>
         <v>0</v>
       </c>
       <c r="G29" s="16" t="e">
-        <f t="shared" ref="G29:G37" si="5">CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(N29,"0.00%"))</f>
+        <f>CONCATENATE(TEXT($G$10-F29,"0,000"),"       ",TEXT(($G$10-F29)/F29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="109">
-        <f>SUM(H30:H32)</f>
-        <v>0</v>
-      </c>
+      <c r="H29" s="110"/>
       <c r="I29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="113">
-        <f t="shared" ref="J29:J37" si="6">(O29-H29)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="111" t="e">
-        <f t="shared" ref="K29:K35" si="7">J29/B29</f>
+      <c r="J29" s="111">
+        <f>(G10-H29)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="112" t="e">
+        <f t="shared" ref="K29:K35" si="2">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="109">
-        <f>SUM(L30:L32)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="110">
-        <f t="shared" ref="M29:M37" si="8">(O29-L29)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="126" t="e">
-        <f t="shared" ref="N29:N35" si="9">M29/F29</f>
+      <c r="L29" s="110"/>
+      <c r="M29" s="111">
+        <f>(G10-L29)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="112" t="e">
+        <f t="shared" ref="N29:N35" si="3">M29/F29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O29" s="127">
-        <f>SUM(O30:O32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="30" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C30" s="147"/>
-      <c r="D30" s="148" t="e">
+      <c r="B30" s="163"/>
+      <c r="C30" s="164"/>
+      <c r="D30" s="169" t="e">
+        <f>CONCATENATE(TEXT(G6-B30,"0,000"),"       ",TEXT((G6-B30)/B30,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" s="170" t="str">
+        <f t="shared" ref="E30" si="4">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F30" s="53"/>
+      <c r="G30" s="16" t="e">
+        <f>CONCATENATE(TEXT(G6-F30,"0,000"),"       ",TEXT((G6-F30)/F30,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="113"/>
+      <c r="I30" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="114">
+        <f>(G6-H30)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="115" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="149" t="str">
-        <f t="shared" ref="E30:E34" si="10">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F30" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L30" s="113"/>
+      <c r="M30" s="116">
+        <f>(G6-L30)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="115" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="112"/>
-      <c r="I30" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="114" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L30" s="112"/>
-      <c r="M30" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="114" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="125"/>
-    </row>
-    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="31" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C31" s="147"/>
-      <c r="D31" s="148" t="e">
+      <c r="B31" s="163"/>
+      <c r="C31" s="164"/>
+      <c r="D31" s="169" t="e">
+        <f t="shared" ref="D31" si="5">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E31" s="170" t="str">
+        <f t="shared" ref="E31:E32" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
+        <v>108年度現階段累積達成率上月增減     0.00</v>
+      </c>
+      <c r="F31" s="53"/>
+      <c r="G31" s="16" t="e">
+        <f>CONCATENATE(TEXT(G7-F31,"0,000"),"       ",TEXT((G7-F31)/F31,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="113"/>
+      <c r="I31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="114">
+        <f>(G7-H31)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="115" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="149" t="str">
-        <f t="shared" ref="E31" si="11">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
-        <v>108年度現階段累積達成率上月增減     0.00</v>
-      </c>
-      <c r="F31" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L31" s="113"/>
+      <c r="M31" s="116">
+        <f>(G7-L31)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="115" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H31" s="112"/>
-      <c r="I31" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="113">
+    </row>
+    <row r="32" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="163"/>
+      <c r="C32" s="164"/>
+      <c r="D32" s="169" t="e">
+        <f>CONCATENATE(TEXT(G8-B32+G9,"0,000"),"       ",TEXT((G8-B32+G9)/B32,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E32" s="170" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="114" t="e">
-        <f t="shared" si="7"/>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F32" s="53"/>
+      <c r="G32" s="16" t="e">
+        <f>CONCATENATE(TEXT(G8-F32+G9,"0,000"),"       ",TEXT((G8-F32+G9)/F32,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L31" s="112"/>
-      <c r="M31" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="114" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="125"/>
-    </row>
-    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C32" s="147"/>
-      <c r="D32" s="148" t="e">
+      <c r="H32" s="113"/>
+      <c r="I32" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="117">
+        <f>(G8-H32+G9)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="118" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="149" t="str">
-        <f t="shared" ref="E32:E33" si="12">CONCATENATE("108年度現階段累積達成率",TEXT(J28,"0.00%"),"     ",TEXT(J24,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F32" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L32" s="113"/>
+      <c r="M32" s="119">
+        <f>(G8-L32+G9)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="118" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H32" s="112"/>
-      <c r="I32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="115" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L32" s="112"/>
-      <c r="M32" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="115" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="125"/>
-    </row>
-    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="33" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="146">
+      <c r="B33" s="163">
+        <f>SUM(B34:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="164"/>
+      <c r="D33" s="169" t="e">
+        <f>CONCATENATE(TEXT(E10-B33,"0,000"),"       ",TEXT((E10-B33)/B33,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" s="170" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C33" s="147"/>
-      <c r="D33" s="148" t="e">
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F33" s="53">
+        <f>SUM(F34:F36)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="16" t="e">
+        <f>CONCATENATE(TEXT(E10-F33,"0,000"),"       ",TEXT((E10-F33)/F33,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="110"/>
+      <c r="I33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="111">
+        <f>(E10-H33)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="112" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="149" t="str">
-        <f t="shared" si="12"/>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F33" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="120">
+        <f>(E10-L33)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="112" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H33" s="110">
-        <f>SUM(H34:H36)</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="111" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L33" s="110">
-        <f>SUM(L34:L36)</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="126" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" s="128">
-        <f>SUM(O34:O36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="34" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C34" s="147"/>
-      <c r="D34" s="148" t="e">
+      <c r="B34" s="163"/>
+      <c r="C34" s="164"/>
+      <c r="D34" s="169" t="e">
+        <f>CONCATENATE(TEXT(E6-B34,"0,000"),"       ",TEXT((E6-B34)/B34,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E34" s="170" t="str">
+        <f t="shared" ref="E34" si="7">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F34" s="53"/>
+      <c r="G34" s="16" t="e">
+        <f>CONCATENATE(TEXT(E6-F34,"0,000"),"       ",TEXT((E6-F34)/F34,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="121"/>
+      <c r="I34" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="114">
+        <f>(E6-H34)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="115" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="149" t="str">
-        <f t="shared" si="10"/>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F34" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="116">
+        <f>(E6-L34)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="115" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H34" s="116"/>
-      <c r="I34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="114" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L34" s="112"/>
-      <c r="M34" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="114" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" s="125"/>
-    </row>
-    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="35" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C35" s="147"/>
-      <c r="D35" s="148" t="e">
+      <c r="B35" s="163"/>
+      <c r="C35" s="164"/>
+      <c r="D35" s="169" t="e">
+        <f t="shared" ref="D35" si="8">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" s="170" t="str">
+        <f t="shared" ref="E35:E37" si="9">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
+        <v>108年度現階段累積達成率0.00%     上月增減</v>
+      </c>
+      <c r="F35" s="53"/>
+      <c r="G35" s="16" t="e">
+        <f>CONCATENATE(TEXT(E7-F35,"0,000"),"       ",TEXT((E7-F35)/F35,"0.00%"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="121"/>
+      <c r="I35" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="122">
+        <f>(E7-H35)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="115" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="149" t="str">
-        <f t="shared" ref="E35" si="13">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     上月增減</v>
-      </c>
-      <c r="F35" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="16" t="e">
-        <f t="shared" si="5"/>
+      <c r="L35" s="113"/>
+      <c r="M35" s="116">
+        <f>(E7-L35)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="115" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="116"/>
-      <c r="I35" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="114" t="e">
-        <f t="shared" si="7"/>
+    </row>
+    <row r="36" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="163"/>
+      <c r="C36" s="164"/>
+      <c r="D36" s="169" t="e">
+        <f>CONCATENATE(TEXT(E8-B36+E9,"0,000"),"       ",TEXT((E8-B36+E9)/B36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="112"/>
-      <c r="M35" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="114" t="e">
+      <c r="E36" s="170" t="str">
         <f t="shared" si="9"/>
+        <v>108年度現階段累積達成率0.00%     0.00</v>
+      </c>
+      <c r="F36" s="53"/>
+      <c r="G36" s="16" t="e">
+        <f>CONCATENATE(TEXT(E8-F36,"0,000"),"       ",TEXT((E8-F36)/F36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O35" s="125"/>
-    </row>
-    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C36" s="147"/>
-      <c r="D36" s="148" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E36" s="149" t="str">
-        <f t="shared" ref="E36" si="14">CONCATENATE("108年度現階段累積達成率",TEXT(J32,"0.00%"),"     ",TEXT(J28,"0.00"))</f>
-        <v>108年度現階段累積達成率0.00%     0.00</v>
-      </c>
-      <c r="F36" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="16" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H36" s="116"/>
+      <c r="H36" s="121"/>
       <c r="I36" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="114" t="e">
+      <c r="J36" s="117">
+        <f>(E8-H36+E9)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="115" t="e">
         <f>J36/B36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="117"/>
-      <c r="M36" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="115" t="e">
+      <c r="L36" s="123"/>
+      <c r="M36" s="119">
+        <f>(E8-L36)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="118" t="e">
         <f>M36/F36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O36" s="125"/>
-    </row>
-    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="54" t="s">
+    </row>
+    <row r="37" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="146">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C37" s="147"/>
-      <c r="D37" s="148" t="e">
-        <f t="shared" si="2"/>
+      <c r="B37" s="163"/>
+      <c r="C37" s="164"/>
+      <c r="D37" s="169" t="e">
+        <f>CONCATENATE(TEXT(C10-B37,"0,000"),"       ",TEXT((C10-B37)/B37,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="149" t="str">
-        <f t="shared" ref="E37" si="15">CONCATENATE("108年度現階段累積達成率",TEXT(J33,"0.00%"),"     ",TEXT(J29,"0.00"))</f>
+      <c r="E37" s="170" t="str">
+        <f t="shared" si="9"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F37" s="51">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="16" t="e">
-        <f t="shared" si="5"/>
+        <f>CONCATENATE(TEXT(C10-F37,"0,000"),"       ",TEXT((C10-F37)/F37,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="116"/>
+      <c r="H37" s="121"/>
       <c r="I37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K37" s="119" t="e">
+      <c r="J37" s="124">
+        <f>(C10-H37)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="125" t="e">
         <f>J37/B37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L37" s="120"/>
-      <c r="M37" s="110">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N37" s="119" t="e">
+      <c r="L37" s="126"/>
+      <c r="M37" s="124">
+        <f>(C10-L37)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="125" t="e">
         <f>M37/F37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O37" s="125"/>
-    </row>
-    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="55" t="s">
+    </row>
+    <row r="38" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="155" t="e">
-        <f>H38</f>
+      <c r="B38" s="205" t="e">
+        <f>(B37+B33)/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="156"/>
-      <c r="D38" s="155" t="e">
-        <f>J38</f>
+      <c r="C38" s="206"/>
+      <c r="D38" s="205" t="e">
+        <f>F15-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="156"/>
-      <c r="F38" s="129" t="e">
-        <f>L38</f>
+      <c r="E38" s="206"/>
+      <c r="F38" s="57" t="e">
+        <f>(F37+F33)/F29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="56" t="e">
-        <f>M38</f>
+      <c r="G38" s="57" t="e">
+        <f>F15-F38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="121" t="e">
-        <f>H27/H28</f>
+      <c r="H38" s="127" t="e">
+        <f>(H33+H37)/H29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="122" t="e">
+      <c r="J38" s="128" t="e">
         <f>F15-H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="118"/>
-      <c r="L38" s="121" t="e">
+      <c r="K38" s="124"/>
+      <c r="L38" s="127" t="e">
         <f>(L33+L37)/L29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M38" s="122" t="e">
+      <c r="M38" s="128" t="e">
         <f>F15-L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N38" s="123"/>
-      <c r="O38" s="125"/>
-    </row>
-    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="N38" s="129"/>
+    </row>
+    <row r="39" spans="1:14" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="46" t="s">
         <v>7</v>
       </c>
@@ -5276,12 +5136,12 @@
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
       <c r="E39" s="37"/>
-      <c r="F39" s="57"/>
+      <c r="F39" s="58"/>
       <c r="G39" s="32" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="124" t="s">
+      <c r="I39" s="130" t="s">
         <v>68</v>
       </c>
       <c r="J39" s="6"/>
@@ -5290,25 +5150,25 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="58" t="s">
+    <row r="40" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="161" t="s">
+      <c r="B40" s="201" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="162"/>
-      <c r="D40" s="161" t="s">
+      <c r="C40" s="202"/>
+      <c r="D40" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="162"/>
-      <c r="F40" s="65" t="s">
+      <c r="E40" s="202"/>
+      <c r="F40" s="66" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="68"/>
+      <c r="H40" s="69"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -5316,124 +5176,124 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="41" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="133"/>
+      <c r="B41" s="199"/>
+      <c r="C41" s="200"/>
+      <c r="D41" s="209"/>
+      <c r="E41" s="210"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="42" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="131"/>
-      <c r="D42" s="132"/>
-      <c r="E42" s="133"/>
+      <c r="B42" s="199"/>
+      <c r="C42" s="200"/>
+      <c r="D42" s="209"/>
+      <c r="E42" s="210"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="43" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="131"/>
-      <c r="D43" s="132"/>
-      <c r="E43" s="133"/>
+      <c r="B43" s="199"/>
+      <c r="C43" s="200"/>
+      <c r="D43" s="209"/>
+      <c r="E43" s="210"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="44" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="130"/>
-      <c r="C44" s="131"/>
-      <c r="D44" s="132"/>
-      <c r="E44" s="133"/>
+      <c r="B44" s="199"/>
+      <c r="C44" s="200"/>
+      <c r="D44" s="209"/>
+      <c r="E44" s="210"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="45" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="132"/>
-      <c r="E45" s="133"/>
+      <c r="B45" s="199"/>
+      <c r="C45" s="200"/>
+      <c r="D45" s="209"/>
+      <c r="E45" s="210"/>
       <c r="F45" s="8"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="46" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="130"/>
-      <c r="C46" s="131"/>
-      <c r="D46" s="132"/>
-      <c r="E46" s="133"/>
+      <c r="B46" s="199"/>
+      <c r="C46" s="200"/>
+      <c r="D46" s="209"/>
+      <c r="E46" s="210"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="47" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="130"/>
-      <c r="C47" s="131"/>
-      <c r="D47" s="130"/>
-      <c r="E47" s="131"/>
+      <c r="B47" s="199"/>
+      <c r="C47" s="200"/>
+      <c r="D47" s="199"/>
+      <c r="E47" s="200"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
+    <row r="48" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="130"/>
-      <c r="C48" s="131"/>
-      <c r="D48" s="130"/>
-      <c r="E48" s="131"/>
+      <c r="B48" s="199"/>
+      <c r="C48" s="200"/>
+      <c r="D48" s="199"/>
+      <c r="E48" s="200"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="130"/>
-      <c r="C49" s="131"/>
-      <c r="D49" s="130"/>
-      <c r="E49" s="131"/>
+      <c r="B49" s="199"/>
+      <c r="C49" s="200"/>
+      <c r="D49" s="199"/>
+      <c r="E49" s="200"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="130"/>
-      <c r="C50" s="131"/>
-      <c r="D50" s="130"/>
-      <c r="E50" s="131"/>
+      <c r="B50" s="199"/>
+      <c r="C50" s="200"/>
+      <c r="D50" s="199"/>
+      <c r="E50" s="200"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="130"/>
-      <c r="C51" s="131"/>
-      <c r="D51" s="130"/>
-      <c r="E51" s="131"/>
+      <c r="B51" s="199"/>
+      <c r="C51" s="200"/>
+      <c r="D51" s="199"/>
+      <c r="E51" s="200"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="151">
+      <c r="B52" s="207">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="151"/>
-      <c r="D52" s="151">
+      <c r="C52" s="207"/>
+      <c r="D52" s="207">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="151"/>
-      <c r="F52" s="60" t="e">
+      <c r="E52" s="207"/>
+      <c r="F52" s="61" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G52" s="61"/>
+      <c r="G52" s="62"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
@@ -5443,24 +5303,24 @@
       <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" ht="17.399999999999999">
-      <c r="A53" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="160">
+      <c r="A53" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="204">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="160"/>
-      <c r="D53" s="160">
+      <c r="C53" s="204"/>
+      <c r="D53" s="204">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="160"/>
-      <c r="F53" s="63">
+      <c r="E53" s="204"/>
+      <c r="F53" s="64">
         <f>F51-F49</f>
         <v>0</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="65"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
@@ -5470,63 +5330,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="152"/>
-      <c r="B54" s="159"/>
-      <c r="C54" s="159"/>
-      <c r="D54" s="172"/>
-      <c r="E54" s="172"/>
-      <c r="F54" s="164"/>
-      <c r="G54" s="171"/>
+      <c r="A54" s="208"/>
+      <c r="B54" s="213"/>
+      <c r="C54" s="213"/>
+      <c r="D54" s="203"/>
+      <c r="E54" s="203"/>
+      <c r="F54" s="193"/>
+      <c r="G54" s="198"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="152"/>
-      <c r="B55" s="159"/>
-      <c r="C55" s="159"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="172"/>
-      <c r="F55" s="164"/>
-      <c r="G55" s="171"/>
+      <c r="A55" s="208"/>
+      <c r="B55" s="213"/>
+      <c r="C55" s="213"/>
+      <c r="D55" s="203"/>
+      <c r="E55" s="203"/>
+      <c r="F55" s="193"/>
+      <c r="G55" s="198"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="163"/>
-      <c r="C56" s="163"/>
-      <c r="D56" s="163"/>
-      <c r="E56" s="163"/>
-      <c r="F56" s="163"/>
-      <c r="G56" s="163"/>
+      <c r="B56" s="192"/>
+      <c r="C56" s="192"/>
+      <c r="D56" s="192"/>
+      <c r="E56" s="192"/>
+      <c r="F56" s="192"/>
+      <c r="G56" s="192"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="163"/>
-      <c r="C57" s="163"/>
-      <c r="D57" s="163"/>
-      <c r="E57" s="163"/>
-      <c r="F57" s="163"/>
-      <c r="G57" s="163"/>
+      <c r="B57" s="192"/>
+      <c r="C57" s="192"/>
+      <c r="D57" s="192"/>
+      <c r="E57" s="192"/>
+      <c r="F57" s="192"/>
+      <c r="G57" s="192"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="163"/>
-      <c r="C58" s="163"/>
-      <c r="D58" s="163"/>
-      <c r="E58" s="163"/>
-      <c r="F58" s="163"/>
-      <c r="G58" s="163"/>
+      <c r="B58" s="192"/>
+      <c r="C58" s="192"/>
+      <c r="D58" s="192"/>
+      <c r="E58" s="192"/>
+      <c r="F58" s="192"/>
+      <c r="G58" s="192"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="163"/>
-      <c r="C59" s="163"/>
-      <c r="D59" s="163"/>
-      <c r="E59" s="163"/>
-      <c r="F59" s="163"/>
-      <c r="G59" s="163"/>
+      <c r="B59" s="192"/>
+      <c r="C59" s="192"/>
+      <c r="D59" s="192"/>
+      <c r="E59" s="192"/>
+      <c r="F59" s="192"/>
+      <c r="G59" s="192"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="163"/>
-      <c r="C60" s="163"/>
-      <c r="D60" s="163"/>
-      <c r="E60" s="163"/>
-      <c r="F60" s="163"/>
-      <c r="G60" s="163"/>
+      <c r="B60" s="192"/>
+      <c r="C60" s="192"/>
+      <c r="D60" s="192"/>
+      <c r="E60" s="192"/>
+      <c r="F60" s="192"/>
+      <c r="G60" s="192"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>
@@ -5540,19 +5400,71 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
@@ -5577,71 +5489,19 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B23:C25"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/12 週四 16:41:39.76
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AF4522-32C0-4BF7-A34E-88E4903410EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB3B24D-69BE-423B-ABD9-BF800C74A376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2098,7 +2098,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -2368,19 +2368,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2598,6 +2585,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2815,10 +2824,10 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2835,10 +2844,10 @@
     <xf numFmtId="182" fontId="34" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="37" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2866,16 +2875,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="27" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="26" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="23" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3010,62 +3019,44 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="46" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="46" applyBorder="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="39" fillId="0" borderId="29" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="29" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="39" fillId="0" borderId="28" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="35" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="25" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="25" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="39" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="25" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="24" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="20" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="23" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="23" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="23" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="34" fillId="0" borderId="22" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="34" fillId="0" borderId="21" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="34" fillId="0" borderId="25" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="20" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="35" fillId="0" borderId="22" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="34" fillId="0" borderId="15" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3087,6 +3078,39 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="29" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="36" fillId="0" borderId="39" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="40" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="41" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="15" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="42" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="23" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="35" fillId="0" borderId="43" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
@@ -3099,28 +3123,28 @@
     <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="184" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3130,7 +3154,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -3143,7 +3167,7 @@
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="36" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3152,7 +3176,7 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="27" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3164,10 +3188,10 @@
     <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3191,19 +3215,19 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="35" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="38" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="32" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3212,6 +3236,12 @@
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3243,25 +3273,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="35" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="27" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="53" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="53" fillId="0" borderId="32" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="53" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3271,10 +3301,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1"/>
-    <xf numFmtId="182" fontId="32" fillId="0" borderId="38" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="32" fillId="0" borderId="37" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="50" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3302,16 +3332,16 @@
     <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3320,7 +3350,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="38" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
@@ -3338,7 +3368,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="32" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3347,32 +3377,11 @@
     <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="39" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="36" fillId="0" borderId="40" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="28" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="41" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="42" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="35" fillId="0" borderId="15" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4061,8 +4070,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -4085,30 +4094,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
       <c r="H1" s="24"/>
       <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="208"/>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
       <c r="H2" s="24"/>
       <c r="J2" s="26"/>
-      <c r="K2" s="214"/>
-      <c r="L2" s="214"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
@@ -4133,21 +4142,21 @@
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="172" t="s">
+      <c r="A4" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="174"/>
-      <c r="D4" s="175" t="s">
+      <c r="C4" s="181"/>
+      <c r="D4" s="182" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="176"/>
-      <c r="F4" s="177" t="s">
+      <c r="E4" s="183"/>
+      <c r="F4" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="209" t="s">
+      <c r="G4" s="216" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="64"/>
@@ -4159,7 +4168,7 @@
       <c r="N4" s="65"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="139"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="30" t="s">
         <v>35</v>
       </c>
@@ -4172,8 +4181,8 @@
       <c r="E5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="178"/>
-      <c r="G5" s="210"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="217"/>
       <c r="H5" s="65"/>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
@@ -4197,8 +4206,8 @@
       <c r="G6" s="23"/>
       <c r="H6" s="68"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="215"/>
-      <c r="K6" s="215"/>
+      <c r="J6" s="222"/>
+      <c r="K6" s="222"/>
       <c r="L6" s="69">
         <f>J6-G6</f>
         <v>0</v>
@@ -4225,8 +4234,8 @@
       <c r="I7" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="215"/>
-      <c r="K7" s="215"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="222"/>
       <c r="L7" s="69">
         <f>J7-G7</f>
         <v>0</v>
@@ -4308,7 +4317,7 @@
         <f>SUM(E6:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4333,12 +4342,12 @@
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
-      <c r="D11" s="161"/>
-      <c r="E11" s="206" t="s">
+      <c r="D11" s="166"/>
+      <c r="E11" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="161"/>
-      <c r="G11" s="161"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
       <c r="H11" s="80"/>
       <c r="I11" s="81">
         <f>H11-E10</f>
@@ -4351,15 +4360,15 @@
       <c r="N11" s="65"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="188" t="s">
+      <c r="A12" s="195" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="189"/>
-      <c r="C12" s="189"/>
-      <c r="D12" s="211"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="162"/>
-      <c r="G12" s="162"/>
+      <c r="B12" s="196"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="218"/>
+      <c r="E12" s="214"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="79"/>
@@ -4369,17 +4378,17 @@
       <c r="N12" s="65"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="190"/>
-      <c r="B13" s="191"/>
-      <c r="C13" s="191"/>
+      <c r="A13" s="197"/>
+      <c r="B13" s="198"/>
+      <c r="C13" s="198"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="186" t="s">
+      <c r="E13" s="193" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="163" t="s">
+      <c r="F13" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="164"/>
+      <c r="G13" s="169"/>
       <c r="H13" s="82" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
@@ -4397,16 +4406,16 @@
       <c r="A14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="216" t="s">
+      <c r="B14" s="223" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="217"/>
+      <c r="C14" s="224"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="187"/>
-      <c r="F14" s="165" t="s">
+      <c r="E14" s="194"/>
+      <c r="F14" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="166"/>
+      <c r="G14" s="171"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="79"/>
@@ -4419,19 +4428,19 @@
       <c r="A15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="212" t="s">
+      <c r="B15" s="219" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="213"/>
+      <c r="C15" s="220"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="169" t="s">
+      <c r="E15" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="130" t="e">
+      <c r="F15" s="135" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="131"/>
+      <c r="G15" s="136"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="79"/>
@@ -4441,18 +4450,18 @@
       <c r="N15" s="65"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="169" t="s">
+      <c r="A16" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="182" t="e">
+      <c r="B16" s="189" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="183"/>
+      <c r="C16" s="190"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="133"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="138"/>
       <c r="H16" s="34"/>
       <c r="I16" s="85"/>
       <c r="J16" s="65"/>
@@ -4462,18 +4471,18 @@
       <c r="N16" s="65"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A17" s="170"/>
-      <c r="B17" s="184"/>
-      <c r="C17" s="185"/>
+      <c r="A17" s="177"/>
+      <c r="B17" s="191"/>
+      <c r="C17" s="192"/>
       <c r="D17" s="34"/>
       <c r="E17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="136" t="e">
+      <c r="F17" s="141" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="137"/>
+      <c r="G17" s="142"/>
       <c r="H17" s="86">
         <f>G10-H18</f>
         <v>0</v>
@@ -4491,23 +4500,23 @@
       <c r="N17" s="65"/>
     </row>
     <row r="18" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A18" s="196" t="s">
+      <c r="A18" s="203" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="197" t="e">
+      <c r="B18" s="204" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="198"/>
+      <c r="C18" s="205"/>
       <c r="D18" s="34"/>
       <c r="E18" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="134" t="e">
+      <c r="F18" s="139" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="135"/>
+      <c r="G18" s="140"/>
       <c r="H18" s="86">
         <f>G7</f>
         <v>0</v>
@@ -4526,18 +4535,18 @@
       <c r="N18" s="65"/>
     </row>
     <row r="19" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A19" s="196"/>
-      <c r="B19" s="197"/>
-      <c r="C19" s="198"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="205"/>
       <c r="D19" s="34"/>
       <c r="E19" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="136" t="e">
+      <c r="F19" s="141" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="137"/>
+      <c r="G19" s="142"/>
       <c r="H19" s="86">
         <f>G10-H20</f>
         <v>0</v>
@@ -4553,20 +4562,20 @@
       <c r="N19" s="65"/>
     </row>
     <row r="20" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A20" s="195" t="s">
+      <c r="A20" s="202" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="193"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="200"/>
       <c r="D20" s="34"/>
       <c r="E20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="134" t="e">
+      <c r="F20" s="139" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="135"/>
+      <c r="G20" s="140"/>
       <c r="H20" s="17"/>
       <c r="I20" s="89">
         <f>F7</f>
@@ -4582,9 +4591,9 @@
       <c r="N20" s="65"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="195"/>
-      <c r="B21" s="192"/>
-      <c r="C21" s="193"/>
+      <c r="A21" s="202"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="200"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
@@ -4598,17 +4607,17 @@
       <c r="N21" s="65"/>
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A22" s="195"/>
-      <c r="B22" s="192"/>
-      <c r="C22" s="193"/>
+      <c r="A22" s="202"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="200"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="138" t="s">
+      <c r="E22" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="138" t="s">
+      <c r="F22" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="138" t="s">
+      <c r="G22" s="143" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="86"/>
@@ -4620,18 +4629,18 @@
       <c r="N22" s="65"/>
     </row>
     <row r="23" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A23" s="194" t="s">
+      <c r="A23" s="201" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="199">
+      <c r="B23" s="206">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="200"/>
+      <c r="C23" s="207"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="139"/>
-      <c r="G23" s="139"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="144"/>
       <c r="H23" s="86"/>
       <c r="I23" s="92"/>
       <c r="J23" s="65"/>
@@ -4641,9 +4650,9 @@
       <c r="N23" s="65"/>
     </row>
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="194"/>
-      <c r="B24" s="199"/>
-      <c r="C24" s="200"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="206"/>
+      <c r="C24" s="207"/>
       <c r="D24" s="34"/>
       <c r="E24" s="41" t="s">
         <v>32</v>
@@ -4659,9 +4668,9 @@
       <c r="N24" s="65"/>
     </row>
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="194"/>
-      <c r="B25" s="199"/>
-      <c r="C25" s="200"/>
+      <c r="A25" s="201"/>
+      <c r="B25" s="206"/>
+      <c r="C25" s="207"/>
       <c r="D25" s="34"/>
       <c r="E25" s="42" t="s">
         <v>31</v>
@@ -4683,8 +4692,8 @@
       <c r="A26" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="146"/>
-      <c r="C26" s="146"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="151"/>
       <c r="D26" s="44"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
@@ -4702,40 +4711,40 @@
       <c r="N26" s="34"/>
     </row>
     <row r="27" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A27" s="138" t="s">
+      <c r="A27" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="149"/>
-      <c r="C27" s="180"/>
-      <c r="D27" s="153" t="s">
+      <c r="B27" s="154"/>
+      <c r="C27" s="187"/>
+      <c r="D27" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="154"/>
-      <c r="F27" s="149"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="154"/>
       <c r="G27" s="45" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="97"/>
       <c r="I27" s="98"/>
-      <c r="J27" s="204" t="s">
+      <c r="J27" s="211" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="205"/>
-      <c r="L27" s="201" t="s">
+      <c r="K27" s="212"/>
+      <c r="L27" s="208" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="202"/>
-      <c r="N27" s="203"/>
+      <c r="M27" s="209"/>
+      <c r="N27" s="210"/>
     </row>
     <row r="28" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A28" s="179"/>
-      <c r="B28" s="150"/>
-      <c r="C28" s="181"/>
-      <c r="D28" s="140" t="s">
+      <c r="A28" s="186"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="188"/>
+      <c r="D28" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="141"/>
-      <c r="F28" s="150"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="155"/>
       <c r="G28" s="46" t="s">
         <v>22</v>
       </c>
@@ -4751,17 +4760,17 @@
       <c r="A29" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="142">
-        <f>H29/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="143"/>
-      <c r="D29" s="144" t="e">
-        <f>CONCATENATE(TEXT($G$10-B29,"0,000"),"       ",TEXT(($G$10-B29)/B29,"0.00%"))</f>
+      <c r="B29" s="147">
+        <f t="shared" ref="B29:B37" si="1">H29/1000</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="148"/>
+      <c r="D29" s="149" t="e">
+        <f>CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="145" t="str">
-        <f t="shared" ref="E29:E33" si="1">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
+      <c r="E29" s="150" t="str">
+        <f t="shared" ref="E29" si="2">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F29" s="48">
@@ -4776,27 +4785,27 @@
         <f>SUM(H30:H32)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="218" t="s">
+      <c r="I29" s="120" t="s">
         <v>20</v>
       </c>
       <c r="J29" s="107">
         <f>(O29-H29)/1000</f>
         <v>0</v>
       </c>
-      <c r="K29" s="221" t="e">
-        <f t="shared" ref="K29:K35" si="2">J29/B29</f>
+      <c r="K29" s="123" t="e">
+        <f t="shared" ref="K29:K35" si="3">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="106">
+      <c r="L29" s="128">
         <f>SUM(L30:L32)</f>
         <v>0</v>
       </c>
       <c r="M29" s="107">
-        <f>(G10-L29)</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="108" t="e">
-        <f t="shared" ref="N29:N35" si="3">M29/F29</f>
+        <f>(O29-L29)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="123" t="e">
+        <f t="shared" ref="N29:N35" si="4">M29/F29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O29" s="1">
@@ -4808,46 +4817,46 @@
       <c r="A30" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="142">
-        <f>H30/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="143"/>
-      <c r="D30" s="144" t="e">
-        <f>CONCATENATE(TEXT(G6-B30,"0,000"),"       ",TEXT((G6-B30)/B30,"0.00%"))</f>
+      <c r="B30" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C30" s="148"/>
+      <c r="D30" s="149" t="e">
+        <f t="shared" ref="D30:D37" si="5">CONCATENATE(TEXT(J30,"0,000"),"       ",TEXT(K30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="145" t="str">
-        <f t="shared" ref="E30" si="4">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
+      <c r="E30" s="150" t="str">
+        <f t="shared" ref="E30:E37" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F30" s="48">
-        <f t="shared" ref="F30:F37" si="5">L30/1000</f>
+        <f t="shared" ref="F30:F37" si="7">L30/1000</f>
         <v>0</v>
       </c>
       <c r="G30" s="13" t="e">
         <f>CONCATENATE(TEXT(G6-F30,"0,000"),"       ",TEXT((G6-F30)/F30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="109"/>
-      <c r="I30" s="219" t="s">
+      <c r="H30" s="108"/>
+      <c r="I30" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="110">
-        <f t="shared" ref="J30:J36" si="6">(O30-H30)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="K30" s="222" t="e">
-        <f t="shared" si="2"/>
+      <c r="J30" s="109">
+        <f t="shared" ref="J30:J36" si="8">(O30-H30)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="124" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L30" s="109"/>
-      <c r="M30" s="112">
-        <f>(G6-L30)</f>
-        <v>0</v>
-      </c>
-      <c r="N30" s="111" t="e">
-        <f t="shared" si="3"/>
+      <c r="L30" s="129"/>
+      <c r="M30" s="109">
+        <f t="shared" ref="M30:M37" si="9">(O30-L30)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="124" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4855,46 +4864,46 @@
       <c r="A31" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="142">
-        <f>H31/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="143"/>
-      <c r="D31" s="144" t="e">
-        <f t="shared" ref="D31" si="7">CONCATENATE(TEXT(G7-B31,"0,000"),"       ",TEXT((G7-B31)/B31,"0.00%"))</f>
+      <c r="B31" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C31" s="148"/>
+      <c r="D31" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="145" t="str">
-        <f t="shared" ref="E31:E32" si="8">CONCATENATE("108年度現階段累積達成率",TEXT(J27,"0.00%"),"     ",TEXT(J23,"0.00"))</f>
+      <c r="E31" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
       <c r="F31" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G31" s="13" t="e">
         <f>CONCATENATE(TEXT(G7-F31,"0,000"),"       ",TEXT((G7-F31)/F31,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H31" s="109"/>
-      <c r="I31" s="219" t="s">
+      <c r="H31" s="108"/>
+      <c r="I31" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="110">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="222" t="e">
-        <f t="shared" si="2"/>
+      <c r="J31" s="109">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="124" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L31" s="109"/>
-      <c r="M31" s="112">
-        <f>(G7-L31)</f>
-        <v>0</v>
-      </c>
-      <c r="N31" s="111" t="e">
-        <f t="shared" si="3"/>
+      <c r="L31" s="129"/>
+      <c r="M31" s="109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="124" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4902,46 +4911,46 @@
       <c r="A32" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="142">
-        <f>H32/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="143"/>
-      <c r="D32" s="144" t="e">
-        <f>CONCATENATE(TEXT(G8-B32+G9,"0,000"),"       ",TEXT((G8-B32+G9)/B32,"0.00%"))</f>
+      <c r="B32" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C32" s="148"/>
+      <c r="D32" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="145" t="str">
-        <f t="shared" si="8"/>
+      <c r="E32" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F32" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G32" s="13" t="e">
         <f>CONCATENATE(TEXT(G8-F32+G9,"0,000"),"       ",TEXT((G8-F32+G9)/F32,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H32" s="109"/>
-      <c r="I32" s="220" t="s">
+      <c r="H32" s="108"/>
+      <c r="I32" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="110">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="223" t="e">
-        <f t="shared" si="2"/>
+      <c r="J32" s="109">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="125" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L32" s="109"/>
-      <c r="M32" s="115">
-        <f>(G8-L32+G9)</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="114" t="e">
-        <f t="shared" si="3"/>
+      <c r="L32" s="129"/>
+      <c r="M32" s="109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="125" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4949,21 +4958,21 @@
       <c r="A33" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="142">
-        <f>H33/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="143"/>
-      <c r="D33" s="144" t="e">
-        <f>CONCATENATE(TEXT(E10-B33,"0,000"),"       ",TEXT((E10-B33)/B33,"0.00%"))</f>
+      <c r="B33" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C33" s="148"/>
+      <c r="D33" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="145" t="str">
-        <f t="shared" si="1"/>
+      <c r="E33" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F33" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G33" s="13" t="e">
@@ -4974,24 +4983,27 @@
         <f>SUM(H34:H36)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="218" t="s">
+      <c r="I33" s="120" t="s">
         <v>18</v>
       </c>
       <c r="J33" s="107">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="221" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="123" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L33" s="106"/>
-      <c r="M33" s="116">
-        <f>(E10-L33)</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="108" t="e">
-        <f t="shared" si="3"/>
+      <c r="L33" s="128">
+        <f>SUM(L34:L36)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="107">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="123" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O33" s="1">
@@ -5003,46 +5015,46 @@
       <c r="A34" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="142">
-        <f>H34/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="143"/>
-      <c r="D34" s="144" t="e">
-        <f>CONCATENATE(TEXT(E6-B34,"0,000"),"       ",TEXT((E6-B34)/B34,"0.00%"))</f>
+      <c r="B34" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C34" s="148"/>
+      <c r="D34" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="145" t="str">
-        <f t="shared" ref="E34" si="9">CONCATENATE("108年度現階段累積達成率",TEXT(J30,"0.00%"),"     ",TEXT(J26,"0.00"))</f>
+      <c r="E34" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F34" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G34" s="13" t="e">
         <f>CONCATENATE(TEXT(E6-F34,"0,000"),"       ",TEXT((E6-F34)/F34,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H34" s="117"/>
-      <c r="I34" s="219" t="s">
+      <c r="H34" s="112"/>
+      <c r="I34" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="110">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="222" t="e">
-        <f t="shared" si="2"/>
+      <c r="J34" s="109">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="124" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L34" s="109"/>
-      <c r="M34" s="112">
-        <f>(E6-L34)</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="111" t="e">
-        <f t="shared" si="3"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="124" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5050,46 +5062,46 @@
       <c r="A35" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="142">
-        <f>H35/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="143"/>
-      <c r="D35" s="144" t="e">
-        <f t="shared" ref="D35" si="10">CONCATENATE(TEXT(E7-B35,"0,000"),"       ",TEXT((E7-B35)/B35,"0.00%"))</f>
+      <c r="B35" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C35" s="148"/>
+      <c r="D35" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="145" t="str">
-        <f t="shared" ref="E35:E37" si="11">CONCATENATE("108年度現階段累積達成率",TEXT(J31,"0.00%"),"     ",TEXT(J27,"0.00"))</f>
+      <c r="E35" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
       <c r="F35" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="13" t="e">
         <f>CONCATENATE(TEXT(E7-F35,"0,000"),"       ",TEXT((E7-F35)/F35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="117"/>
-      <c r="I35" s="219" t="s">
+      <c r="H35" s="112"/>
+      <c r="I35" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="110">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="222" t="e">
-        <f t="shared" si="2"/>
+      <c r="J35" s="109">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="124" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="109"/>
-      <c r="M35" s="112">
-        <f>(E7-L35)</f>
-        <v>0</v>
-      </c>
-      <c r="N35" s="111" t="e">
-        <f t="shared" si="3"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="124" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5097,45 +5109,45 @@
       <c r="A36" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="142">
-        <f>H36/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="143"/>
-      <c r="D36" s="144" t="e">
-        <f>CONCATENATE(TEXT(E8-B36+E9,"0,000"),"       ",TEXT((E8-B36+E9)/B36,"0.00%"))</f>
+      <c r="B36" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C36" s="148"/>
+      <c r="D36" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="145" t="str">
-        <f t="shared" si="11"/>
+      <c r="E36" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F36" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G36" s="13" t="e">
         <f>CONCATENATE(TEXT(E8-F36,"0,000"),"       ",TEXT((E8-F36)/F36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H36" s="117"/>
-      <c r="I36" s="220" t="s">
+      <c r="H36" s="112"/>
+      <c r="I36" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="113">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="222" t="e">
+      <c r="J36" s="110">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="124" t="e">
         <f>J36/B36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="118"/>
-      <c r="M36" s="115">
-        <f>(E8-L36)</f>
-        <v>0</v>
-      </c>
-      <c r="N36" s="114" t="e">
+      <c r="L36" s="130"/>
+      <c r="M36" s="110">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="125" t="e">
         <f>M36/F36</f>
         <v>#DIV/0!</v>
       </c>
@@ -5144,45 +5156,45 @@
       <c r="A37" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="142">
-        <f>H37/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="143"/>
-      <c r="D37" s="144" t="e">
-        <f>CONCATENATE(TEXT(C10-B37,"0,000"),"       ",TEXT((C10-B37)/B37,"0.00%"))</f>
+      <c r="B37" s="147">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C37" s="148"/>
+      <c r="D37" s="149" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="145" t="str">
-        <f t="shared" si="11"/>
+      <c r="E37" s="150" t="str">
+        <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
       <c r="F37" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G37" s="13" t="e">
         <f>CONCATENATE(TEXT(C10-F37,"0,000"),"       ",TEXT((C10-F37)/F37,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="224"/>
+      <c r="H37" s="126"/>
       <c r="I37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="115">
-        <f>(C10-H37)</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="120" t="e">
+      <c r="J37" s="111">
+        <f>(C10-H37)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="114" t="e">
         <f>J37/B37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L37" s="121"/>
-      <c r="M37" s="119">
-        <f>(C10-L37)</f>
-        <v>0</v>
-      </c>
-      <c r="N37" s="120" t="e">
+      <c r="L37" s="115"/>
+      <c r="M37" s="109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="114" t="e">
         <f>M37/F37</f>
         <v>#DIV/0!</v>
       </c>
@@ -5191,45 +5203,45 @@
       <c r="A38" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="151" t="e">
+      <c r="B38" s="156" t="e">
         <f>H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="152"/>
-      <c r="D38" s="151" t="e">
+      <c r="C38" s="157"/>
+      <c r="D38" s="174" t="e">
         <f>J38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="152"/>
+      <c r="E38" s="175"/>
       <c r="F38" s="53" t="e">
         <f>L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="53" t="e">
+      <c r="G38" s="127" t="e">
         <f>M38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="122" t="e">
+      <c r="H38" s="116" t="e">
         <f>(H33+H37)/H29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I38" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="123" t="e">
+      <c r="J38" s="117" t="e">
         <f>F15-H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="119"/>
-      <c r="L38" s="122" t="e">
+      <c r="K38" s="113"/>
+      <c r="L38" s="116" t="e">
         <f>(L33+L37)/L29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M38" s="123" t="e">
+      <c r="M38" s="117" t="e">
         <f>F15-L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N38" s="124"/>
+      <c r="N38" s="118"/>
     </row>
     <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="43" t="s">
@@ -5244,7 +5256,7 @@
         <v>69</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="125" t="s">
+      <c r="I39" s="119" t="s">
         <v>68</v>
       </c>
       <c r="J39" s="6"/>
@@ -5257,14 +5269,14 @@
       <c r="A40" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="157" t="s">
+      <c r="B40" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="158"/>
-      <c r="D40" s="157" t="s">
+      <c r="C40" s="163"/>
+      <c r="D40" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="158"/>
+      <c r="E40" s="163"/>
       <c r="F40" s="62" t="s">
         <v>3</v>
       </c>
@@ -5281,100 +5293,100 @@
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="127"/>
-      <c r="D41" s="128"/>
-      <c r="E41" s="129"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="132"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="134"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="126"/>
-      <c r="C42" s="127"/>
-      <c r="D42" s="128"/>
-      <c r="E42" s="129"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="134"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="126"/>
-      <c r="C43" s="127"/>
-      <c r="D43" s="128"/>
-      <c r="E43" s="129"/>
+      <c r="B43" s="131"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="133"/>
+      <c r="E43" s="134"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="126"/>
-      <c r="C44" s="127"/>
-      <c r="D44" s="128"/>
-      <c r="E44" s="129"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="132"/>
+      <c r="D44" s="133"/>
+      <c r="E44" s="134"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="126"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="129"/>
+      <c r="B45" s="131"/>
+      <c r="C45" s="132"/>
+      <c r="D45" s="133"/>
+      <c r="E45" s="134"/>
       <c r="F45" s="8"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="126"/>
-      <c r="C46" s="127"/>
-      <c r="D46" s="128"/>
-      <c r="E46" s="129"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="132"/>
+      <c r="D46" s="133"/>
+      <c r="E46" s="134"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="126"/>
-      <c r="C47" s="127"/>
-      <c r="D47" s="126"/>
-      <c r="E47" s="127"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="132"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="132"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="126"/>
-      <c r="C48" s="127"/>
-      <c r="D48" s="126"/>
-      <c r="E48" s="127"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="132"/>
+      <c r="D48" s="131"/>
+      <c r="E48" s="132"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="126"/>
-      <c r="C49" s="127"/>
-      <c r="D49" s="126"/>
-      <c r="E49" s="127"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="132"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="126"/>
-      <c r="C50" s="127"/>
-      <c r="D50" s="126"/>
-      <c r="E50" s="127"/>
+      <c r="B50" s="131"/>
+      <c r="C50" s="132"/>
+      <c r="D50" s="131"/>
+      <c r="E50" s="132"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="126"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="126"/>
-      <c r="E51" s="127"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="132"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="132"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
@@ -5382,16 +5394,16 @@
       <c r="A52" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="147">
+      <c r="B52" s="152">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="147"/>
-      <c r="D52" s="147">
+      <c r="C52" s="152"/>
+      <c r="D52" s="152">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="147"/>
+      <c r="E52" s="152"/>
       <c r="F52" s="57" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
@@ -5409,16 +5421,16 @@
       <c r="A53" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="156">
+      <c r="B53" s="161">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="156"/>
-      <c r="D53" s="156">
+      <c r="C53" s="161"/>
+      <c r="D53" s="161">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="156"/>
+      <c r="E53" s="161"/>
       <c r="F53" s="60">
         <f>F51-F49</f>
         <v>0</v>
@@ -5433,63 +5445,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="148"/>
-      <c r="B54" s="155"/>
-      <c r="C54" s="155"/>
-      <c r="D54" s="168"/>
-      <c r="E54" s="168"/>
-      <c r="F54" s="160"/>
-      <c r="G54" s="167"/>
+      <c r="A54" s="153"/>
+      <c r="B54" s="160"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="173"/>
+      <c r="E54" s="173"/>
+      <c r="F54" s="165"/>
+      <c r="G54" s="172"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="148"/>
-      <c r="B55" s="155"/>
-      <c r="C55" s="155"/>
-      <c r="D55" s="168"/>
-      <c r="E55" s="168"/>
-      <c r="F55" s="160"/>
-      <c r="G55" s="167"/>
+      <c r="A55" s="153"/>
+      <c r="B55" s="160"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="173"/>
+      <c r="E55" s="173"/>
+      <c r="F55" s="165"/>
+      <c r="G55" s="172"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="159"/>
-      <c r="C56" s="159"/>
-      <c r="D56" s="159"/>
-      <c r="E56" s="159"/>
-      <c r="F56" s="159"/>
-      <c r="G56" s="159"/>
+      <c r="B56" s="164"/>
+      <c r="C56" s="164"/>
+      <c r="D56" s="164"/>
+      <c r="E56" s="164"/>
+      <c r="F56" s="164"/>
+      <c r="G56" s="164"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="159"/>
-      <c r="C57" s="159"/>
-      <c r="D57" s="159"/>
-      <c r="E57" s="159"/>
-      <c r="F57" s="159"/>
-      <c r="G57" s="159"/>
+      <c r="B57" s="164"/>
+      <c r="C57" s="164"/>
+      <c r="D57" s="164"/>
+      <c r="E57" s="164"/>
+      <c r="F57" s="164"/>
+      <c r="G57" s="164"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="159"/>
-      <c r="C58" s="159"/>
-      <c r="D58" s="159"/>
-      <c r="E58" s="159"/>
-      <c r="F58" s="159"/>
-      <c r="G58" s="159"/>
+      <c r="B58" s="164"/>
+      <c r="C58" s="164"/>
+      <c r="D58" s="164"/>
+      <c r="E58" s="164"/>
+      <c r="F58" s="164"/>
+      <c r="G58" s="164"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="159"/>
-      <c r="C59" s="159"/>
-      <c r="D59" s="159"/>
-      <c r="E59" s="159"/>
-      <c r="F59" s="159"/>
-      <c r="G59" s="159"/>
+      <c r="B59" s="164"/>
+      <c r="C59" s="164"/>
+      <c r="D59" s="164"/>
+      <c r="E59" s="164"/>
+      <c r="F59" s="164"/>
+      <c r="G59" s="164"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="159"/>
-      <c r="C60" s="159"/>
-      <c r="D60" s="159"/>
-      <c r="E60" s="159"/>
-      <c r="F60" s="159"/>
-      <c r="G60" s="159"/>
+      <c r="B60" s="164"/>
+      <c r="C60" s="164"/>
+      <c r="D60" s="164"/>
+      <c r="E60" s="164"/>
+      <c r="F60" s="164"/>
+      <c r="G60" s="164"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/13 週五 11:46:03.57
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB3B24D-69BE-423B-ABD9-BF800C74A376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3505CA-C7B3-4E78-9EBD-134E9E5DC60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3099,9 +3099,6 @@
     <xf numFmtId="178" fontId="35" fillId="0" borderId="15" xfId="46" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="178" fontId="35" fillId="0" borderId="42" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3111,172 +3108,128 @@
     <xf numFmtId="178" fontId="35" fillId="0" borderId="43" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="53" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3332,55 +3285,102 @@
     <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4070,8 +4070,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:C25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -4094,30 +4094,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="151" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
       <c r="H1" s="24"/>
       <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="215"/>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
+      <c r="A2" s="137"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
       <c r="H2" s="24"/>
       <c r="J2" s="26"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
@@ -4142,21 +4142,21 @@
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="179" t="s">
+      <c r="A4" s="152" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="182" t="s">
+      <c r="C4" s="155"/>
+      <c r="D4" s="156" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="183"/>
-      <c r="F4" s="184" t="s">
+      <c r="E4" s="157"/>
+      <c r="F4" s="158" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="216" t="s">
+      <c r="G4" s="138" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="64"/>
@@ -4168,7 +4168,7 @@
       <c r="N4" s="65"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="144"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="30" t="s">
         <v>35</v>
       </c>
@@ -4181,8 +4181,8 @@
       <c r="E5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="185"/>
-      <c r="G5" s="217"/>
+      <c r="F5" s="159"/>
+      <c r="G5" s="139"/>
       <c r="H5" s="65"/>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
@@ -4206,8 +4206,8 @@
       <c r="G6" s="23"/>
       <c r="H6" s="68"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="222"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
       <c r="L6" s="69">
         <f>J6-G6</f>
         <v>0</v>
@@ -4234,8 +4234,8 @@
       <c r="I7" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="222"/>
-      <c r="K7" s="222"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
       <c r="L7" s="69">
         <f>J7-G7</f>
         <v>0</v>
@@ -4342,12 +4342,12 @@
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="213" t="s">
+      <c r="D11" s="140"/>
+      <c r="E11" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
       <c r="H11" s="80"/>
       <c r="I11" s="81">
         <f>H11-E10</f>
@@ -4360,15 +4360,15 @@
       <c r="N11" s="65"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="196"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="218"/>
-      <c r="E12" s="214"/>
-      <c r="F12" s="167"/>
-      <c r="G12" s="167"/>
+      <c r="B12" s="179"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="79"/>
@@ -4378,17 +4378,17 @@
       <c r="N12" s="65"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="197"/>
-      <c r="B13" s="198"/>
-      <c r="C13" s="198"/>
+      <c r="A13" s="180"/>
+      <c r="B13" s="181"/>
+      <c r="C13" s="181"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="193" t="s">
+      <c r="E13" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="168" t="s">
+      <c r="F13" s="193" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="169"/>
+      <c r="G13" s="194"/>
       <c r="H13" s="82" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
@@ -4406,16 +4406,16 @@
       <c r="A14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="223" t="s">
+      <c r="B14" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="224"/>
+      <c r="C14" s="150"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="170" t="s">
+      <c r="E14" s="177"/>
+      <c r="F14" s="195" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="171"/>
+      <c r="G14" s="196"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="79"/>
@@ -4428,19 +4428,19 @@
       <c r="A15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="219" t="s">
+      <c r="B15" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="220"/>
+      <c r="C15" s="146"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="176" t="s">
+      <c r="E15" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="135" t="e">
+      <c r="F15" s="221" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="136"/>
+      <c r="G15" s="222"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="79"/>
@@ -4450,18 +4450,18 @@
       <c r="N15" s="65"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="176" t="s">
+      <c r="A16" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="189" t="e">
+      <c r="B16" s="172" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="190"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="137"/>
-      <c r="G16" s="138"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="223"/>
+      <c r="G16" s="224"/>
       <c r="H16" s="34"/>
       <c r="I16" s="85"/>
       <c r="J16" s="65"/>
@@ -4471,18 +4471,18 @@
       <c r="N16" s="65"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A17" s="177"/>
-      <c r="B17" s="191"/>
-      <c r="C17" s="192"/>
+      <c r="A17" s="144"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
       <c r="D17" s="34"/>
       <c r="E17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="141" t="e">
+      <c r="F17" s="170" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="142"/>
+      <c r="G17" s="171"/>
       <c r="H17" s="86">
         <f>G10-H18</f>
         <v>0</v>
@@ -4500,23 +4500,23 @@
       <c r="N17" s="65"/>
     </row>
     <row r="18" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A18" s="203" t="s">
+      <c r="A18" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="204" t="e">
+      <c r="B18" s="187" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="205"/>
+      <c r="C18" s="188"/>
       <c r="D18" s="34"/>
       <c r="E18" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="139" t="e">
+      <c r="F18" s="213" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="140"/>
+      <c r="G18" s="214"/>
       <c r="H18" s="86">
         <f>G7</f>
         <v>0</v>
@@ -4535,18 +4535,18 @@
       <c r="N18" s="65"/>
     </row>
     <row r="19" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A19" s="203"/>
-      <c r="B19" s="204"/>
-      <c r="C19" s="205"/>
+      <c r="A19" s="186"/>
+      <c r="B19" s="187"/>
+      <c r="C19" s="188"/>
       <c r="D19" s="34"/>
       <c r="E19" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="141" t="e">
+      <c r="F19" s="170" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="142"/>
+      <c r="G19" s="171"/>
       <c r="H19" s="86">
         <f>G10-H20</f>
         <v>0</v>
@@ -4562,20 +4562,20 @@
       <c r="N19" s="65"/>
     </row>
     <row r="20" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A20" s="202" t="s">
+      <c r="A20" s="185" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="199"/>
-      <c r="C20" s="200"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="183"/>
       <c r="D20" s="34"/>
       <c r="E20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="139" t="e">
+      <c r="F20" s="213" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="140"/>
+      <c r="G20" s="214"/>
       <c r="H20" s="17"/>
       <c r="I20" s="89">
         <f>F7</f>
@@ -4591,9 +4591,9 @@
       <c r="N20" s="65"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="202"/>
-      <c r="B21" s="199"/>
-      <c r="C21" s="200"/>
+      <c r="A21" s="185"/>
+      <c r="B21" s="182"/>
+      <c r="C21" s="183"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
@@ -4607,17 +4607,17 @@
       <c r="N21" s="65"/>
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A22" s="202"/>
-      <c r="B22" s="199"/>
-      <c r="C22" s="200"/>
+      <c r="A22" s="185"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="183"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="143" t="s">
+      <c r="E22" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="143" t="s">
+      <c r="F22" s="160" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="143" t="s">
+      <c r="G22" s="160" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="86"/>
@@ -4629,18 +4629,18 @@
       <c r="N22" s="65"/>
     </row>
     <row r="23" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="206">
+      <c r="B23" s="189">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="207"/>
+      <c r="C23" s="190"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="153"/>
+      <c r="G23" s="153"/>
       <c r="H23" s="86"/>
       <c r="I23" s="92"/>
       <c r="J23" s="65"/>
@@ -4650,9 +4650,9 @@
       <c r="N23" s="65"/>
     </row>
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="201"/>
-      <c r="B24" s="206"/>
-      <c r="C24" s="207"/>
+      <c r="A24" s="184"/>
+      <c r="B24" s="189"/>
+      <c r="C24" s="190"/>
       <c r="D24" s="34"/>
       <c r="E24" s="41" t="s">
         <v>32</v>
@@ -4668,9 +4668,9 @@
       <c r="N24" s="65"/>
     </row>
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="201"/>
-      <c r="B25" s="206"/>
-      <c r="C25" s="207"/>
+      <c r="A25" s="184"/>
+      <c r="B25" s="189"/>
+      <c r="C25" s="190"/>
       <c r="D25" s="34"/>
       <c r="E25" s="42" t="s">
         <v>31</v>
@@ -4692,8 +4692,8 @@
       <c r="A26" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="151"/>
-      <c r="C26" s="151"/>
+      <c r="B26" s="217"/>
+      <c r="C26" s="217"/>
       <c r="D26" s="44"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
@@ -4711,40 +4711,40 @@
       <c r="N26" s="34"/>
     </row>
     <row r="27" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A27" s="143" t="s">
+      <c r="A27" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="187"/>
-      <c r="D27" s="158" t="s">
+      <c r="B27" s="164"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="210" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="159"/>
-      <c r="F27" s="154"/>
+      <c r="E27" s="211"/>
+      <c r="F27" s="164"/>
       <c r="G27" s="45" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="97"/>
       <c r="I27" s="98"/>
-      <c r="J27" s="211" t="s">
+      <c r="J27" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="212"/>
-      <c r="L27" s="208" t="s">
+      <c r="K27" s="134"/>
+      <c r="L27" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="209"/>
-      <c r="N27" s="210"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="132"/>
     </row>
     <row r="28" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A28" s="186"/>
-      <c r="B28" s="155"/>
-      <c r="C28" s="188"/>
-      <c r="D28" s="145" t="s">
+      <c r="A28" s="161"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="215" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="146"/>
-      <c r="F28" s="155"/>
+      <c r="E28" s="216"/>
+      <c r="F28" s="166"/>
       <c r="G28" s="46" t="s">
         <v>22</v>
       </c>
@@ -4760,16 +4760,16 @@
       <c r="A29" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="147">
+      <c r="B29" s="162">
         <f t="shared" ref="B29:B37" si="1">H29/1000</f>
         <v>0</v>
       </c>
-      <c r="C29" s="148"/>
-      <c r="D29" s="149" t="e">
+      <c r="C29" s="163"/>
+      <c r="D29" s="168" t="e">
         <f>CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="150" t="str">
+      <c r="E29" s="169" t="str">
         <f t="shared" ref="E29" si="2">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="13" t="e">
-        <f>CONCATENATE(TEXT($G$10-F29,"0,000"),"       ",TEXT(($G$10-F29)/F29,"0.00%"))</f>
+        <f>CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(($G$10-F29)/F29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H29" s="106">
@@ -4796,7 +4796,7 @@
         <f t="shared" ref="K29:K35" si="3">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="128">
+      <c r="L29" s="127">
         <f>SUM(L30:L32)</f>
         <v>0</v>
       </c>
@@ -4817,16 +4817,16 @@
       <c r="A30" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="147">
+      <c r="B30" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C30" s="148"/>
-      <c r="D30" s="149" t="e">
+      <c r="C30" s="163"/>
+      <c r="D30" s="168" t="e">
         <f t="shared" ref="D30:D37" si="5">CONCATENATE(TEXT(J30,"0,000"),"       ",TEXT(K30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="150" t="str">
+      <c r="E30" s="169" t="str">
         <f t="shared" ref="E30:E37" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="13" t="e">
-        <f>CONCATENATE(TEXT(G6-F30,"0,000"),"       ",TEXT((G6-F30)/F30,"0.00%"))</f>
+        <f t="shared" ref="G30:G37" si="8">CONCATENATE(TEXT(M30,"0,000"),"       ",TEXT(($G$10-F30)/F30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H30" s="108"/>
@@ -4843,16 +4843,16 @@
         <v>16</v>
       </c>
       <c r="J30" s="109">
-        <f t="shared" ref="J30:J36" si="8">(O30-H30)/1000</f>
+        <f t="shared" ref="J30:J36" si="9">(O30-H30)/1000</f>
         <v>0</v>
       </c>
       <c r="K30" s="124" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L30" s="129"/>
+      <c r="L30" s="128"/>
       <c r="M30" s="109">
-        <f t="shared" ref="M30:M37" si="9">(O30-L30)/1000</f>
+        <f t="shared" ref="M30:M37" si="10">(O30-L30)/1000</f>
         <v>0</v>
       </c>
       <c r="N30" s="124" t="e">
@@ -4864,16 +4864,16 @@
       <c r="A31" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="147">
+      <c r="B31" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C31" s="148"/>
-      <c r="D31" s="149" t="e">
+      <c r="C31" s="163"/>
+      <c r="D31" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="150" t="str">
+      <c r="E31" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="13" t="e">
-        <f>CONCATENATE(TEXT(G7-F31,"0,000"),"       ",TEXT((G7-F31)/F31,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H31" s="108"/>
@@ -4890,16 +4890,16 @@
         <v>14</v>
       </c>
       <c r="J31" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K31" s="124" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L31" s="129"/>
+      <c r="L31" s="128"/>
       <c r="M31" s="109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N31" s="124" t="e">
@@ -4911,16 +4911,16 @@
       <c r="A32" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="147">
+      <c r="B32" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C32" s="148"/>
-      <c r="D32" s="149" t="e">
+      <c r="C32" s="163"/>
+      <c r="D32" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="150" t="str">
+      <c r="E32" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="13" t="e">
-        <f>CONCATENATE(TEXT(G8-F32+G9,"0,000"),"       ",TEXT((G8-F32+G9)/F32,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H32" s="108"/>
@@ -4937,16 +4937,16 @@
         <v>12</v>
       </c>
       <c r="J32" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K32" s="125" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L32" s="129"/>
+      <c r="L32" s="128"/>
       <c r="M32" s="109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N32" s="125" t="e">
@@ -4958,16 +4958,16 @@
       <c r="A33" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="147">
+      <c r="B33" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C33" s="148"/>
-      <c r="D33" s="149" t="e">
+      <c r="C33" s="163"/>
+      <c r="D33" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="150" t="str">
+      <c r="E33" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="13" t="e">
-        <f>CONCATENATE(TEXT(E10-F33,"0,000"),"       ",TEXT((E10-F33)/F33,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H33" s="106">
@@ -4987,19 +4987,19 @@
         <v>18</v>
       </c>
       <c r="J33" s="107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K33" s="123" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L33" s="128">
+      <c r="L33" s="127">
         <f>SUM(L34:L36)</f>
         <v>0</v>
       </c>
       <c r="M33" s="107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N33" s="123" t="e">
@@ -5015,16 +5015,16 @@
       <c r="A34" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="147">
+      <c r="B34" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C34" s="148"/>
-      <c r="D34" s="149" t="e">
+      <c r="C34" s="163"/>
+      <c r="D34" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="150" t="str">
+      <c r="E34" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="13" t="e">
-        <f>CONCATENATE(TEXT(E6-F34,"0,000"),"       ",TEXT((E6-F34)/F34,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H34" s="112"/>
@@ -5041,16 +5041,16 @@
         <v>16</v>
       </c>
       <c r="J34" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K34" s="124" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L34" s="129"/>
+      <c r="L34" s="128"/>
       <c r="M34" s="109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N34" s="124" t="e">
@@ -5062,16 +5062,16 @@
       <c r="A35" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="147">
+      <c r="B35" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C35" s="148"/>
-      <c r="D35" s="149" t="e">
+      <c r="C35" s="163"/>
+      <c r="D35" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="150" t="str">
+      <c r="E35" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="e">
-        <f>CONCATENATE(TEXT(E7-F35,"0,000"),"       ",TEXT((E7-F35)/F35,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H35" s="112"/>
@@ -5088,16 +5088,16 @@
         <v>14</v>
       </c>
       <c r="J35" s="109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K35" s="124" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="129"/>
+      <c r="L35" s="128"/>
       <c r="M35" s="109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N35" s="124" t="e">
@@ -5109,16 +5109,16 @@
       <c r="A36" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="147">
+      <c r="B36" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C36" s="148"/>
-      <c r="D36" s="149" t="e">
+      <c r="C36" s="163"/>
+      <c r="D36" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="150" t="str">
+      <c r="E36" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="13" t="e">
-        <f>CONCATENATE(TEXT(E8-F36,"0,000"),"       ",TEXT((E8-F36)/F36,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H36" s="112"/>
@@ -5135,16 +5135,16 @@
         <v>12</v>
       </c>
       <c r="J36" s="110">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K36" s="124" t="e">
         <f>J36/B36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="130"/>
+      <c r="L36" s="129"/>
       <c r="M36" s="110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N36" s="125" t="e">
@@ -5156,16 +5156,16 @@
       <c r="A37" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="147">
+      <c r="B37" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C37" s="148"/>
-      <c r="D37" s="149" t="e">
+      <c r="C37" s="163"/>
+      <c r="D37" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="150" t="str">
+      <c r="E37" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="13" t="e">
-        <f>CONCATENATE(TEXT(C10-F37,"0,000"),"       ",TEXT((C10-F37)/F37,"0.00%"))</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H37" s="126"/>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="L37" s="115"/>
       <c r="M37" s="109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N37" s="114" t="e">
@@ -5203,21 +5203,21 @@
       <c r="A38" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="156" t="e">
+      <c r="B38" s="208" t="e">
         <f>H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="157"/>
-      <c r="D38" s="174" t="e">
+      <c r="C38" s="209"/>
+      <c r="D38" s="219" t="e">
         <f>J38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="175"/>
+      <c r="E38" s="220"/>
       <c r="F38" s="53" t="e">
         <f>L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="127" t="e">
+      <c r="G38" s="218" t="e">
         <f>M38</f>
         <v>#DIV/0!</v>
       </c>
@@ -5269,14 +5269,14 @@
       <c r="A40" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="162" t="s">
+      <c r="B40" s="200" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="163"/>
-      <c r="D40" s="162" t="s">
+      <c r="C40" s="201"/>
+      <c r="D40" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="163"/>
+      <c r="E40" s="201"/>
       <c r="F40" s="62" t="s">
         <v>3</v>
       </c>
@@ -5293,100 +5293,100 @@
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="131"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="133"/>
-      <c r="E41" s="134"/>
+      <c r="B41" s="198"/>
+      <c r="C41" s="199"/>
+      <c r="D41" s="206"/>
+      <c r="E41" s="207"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="131"/>
-      <c r="C42" s="132"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="134"/>
+      <c r="B42" s="198"/>
+      <c r="C42" s="199"/>
+      <c r="D42" s="206"/>
+      <c r="E42" s="207"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="131"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="134"/>
+      <c r="B43" s="198"/>
+      <c r="C43" s="199"/>
+      <c r="D43" s="206"/>
+      <c r="E43" s="207"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="131"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="134"/>
+      <c r="B44" s="198"/>
+      <c r="C44" s="199"/>
+      <c r="D44" s="206"/>
+      <c r="E44" s="207"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="131"/>
-      <c r="C45" s="132"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="134"/>
+      <c r="B45" s="198"/>
+      <c r="C45" s="199"/>
+      <c r="D45" s="206"/>
+      <c r="E45" s="207"/>
       <c r="F45" s="8"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="131"/>
-      <c r="C46" s="132"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="134"/>
+      <c r="B46" s="198"/>
+      <c r="C46" s="199"/>
+      <c r="D46" s="206"/>
+      <c r="E46" s="207"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="132"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="132"/>
+      <c r="B47" s="198"/>
+      <c r="C47" s="199"/>
+      <c r="D47" s="198"/>
+      <c r="E47" s="199"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="132"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="132"/>
+      <c r="B48" s="198"/>
+      <c r="C48" s="199"/>
+      <c r="D48" s="198"/>
+      <c r="E48" s="199"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="131"/>
-      <c r="E49" s="132"/>
+      <c r="B49" s="198"/>
+      <c r="C49" s="199"/>
+      <c r="D49" s="198"/>
+      <c r="E49" s="199"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="131"/>
-      <c r="C50" s="132"/>
-      <c r="D50" s="131"/>
-      <c r="E50" s="132"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="199"/>
+      <c r="D50" s="198"/>
+      <c r="E50" s="199"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
+      <c r="B51" s="198"/>
+      <c r="C51" s="199"/>
+      <c r="D51" s="198"/>
+      <c r="E51" s="199"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
@@ -5394,16 +5394,16 @@
       <c r="A52" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="152">
+      <c r="B52" s="204">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="152"/>
-      <c r="D52" s="152">
+      <c r="C52" s="204"/>
+      <c r="D52" s="204">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="152"/>
+      <c r="E52" s="204"/>
       <c r="F52" s="57" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
@@ -5421,16 +5421,16 @@
       <c r="A53" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="161">
+      <c r="B53" s="203">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="161"/>
-      <c r="D53" s="161">
+      <c r="C53" s="203"/>
+      <c r="D53" s="203">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="161"/>
+      <c r="E53" s="203"/>
       <c r="F53" s="60">
         <f>F51-F49</f>
         <v>0</v>
@@ -5445,63 +5445,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="153"/>
-      <c r="B54" s="160"/>
-      <c r="C54" s="160"/>
-      <c r="D54" s="173"/>
-      <c r="E54" s="173"/>
-      <c r="F54" s="165"/>
-      <c r="G54" s="172"/>
+      <c r="A54" s="205"/>
+      <c r="B54" s="212"/>
+      <c r="C54" s="212"/>
+      <c r="D54" s="202"/>
+      <c r="E54" s="202"/>
+      <c r="F54" s="192"/>
+      <c r="G54" s="197"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="153"/>
-      <c r="B55" s="160"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="173"/>
-      <c r="E55" s="173"/>
-      <c r="F55" s="165"/>
-      <c r="G55" s="172"/>
+      <c r="A55" s="205"/>
+      <c r="B55" s="212"/>
+      <c r="C55" s="212"/>
+      <c r="D55" s="202"/>
+      <c r="E55" s="202"/>
+      <c r="F55" s="192"/>
+      <c r="G55" s="197"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="164"/>
-      <c r="C56" s="164"/>
-      <c r="D56" s="164"/>
-      <c r="E56" s="164"/>
-      <c r="F56" s="164"/>
-      <c r="G56" s="164"/>
+      <c r="B56" s="191"/>
+      <c r="C56" s="191"/>
+      <c r="D56" s="191"/>
+      <c r="E56" s="191"/>
+      <c r="F56" s="191"/>
+      <c r="G56" s="191"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="164"/>
-      <c r="C57" s="164"/>
-      <c r="D57" s="164"/>
-      <c r="E57" s="164"/>
-      <c r="F57" s="164"/>
-      <c r="G57" s="164"/>
+      <c r="B57" s="191"/>
+      <c r="C57" s="191"/>
+      <c r="D57" s="191"/>
+      <c r="E57" s="191"/>
+      <c r="F57" s="191"/>
+      <c r="G57" s="191"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="164"/>
-      <c r="C58" s="164"/>
-      <c r="D58" s="164"/>
-      <c r="E58" s="164"/>
-      <c r="F58" s="164"/>
-      <c r="G58" s="164"/>
+      <c r="B58" s="191"/>
+      <c r="C58" s="191"/>
+      <c r="D58" s="191"/>
+      <c r="E58" s="191"/>
+      <c r="F58" s="191"/>
+      <c r="G58" s="191"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="164"/>
-      <c r="C59" s="164"/>
-      <c r="D59" s="164"/>
-      <c r="E59" s="164"/>
-      <c r="F59" s="164"/>
-      <c r="G59" s="164"/>
+      <c r="B59" s="191"/>
+      <c r="C59" s="191"/>
+      <c r="D59" s="191"/>
+      <c r="E59" s="191"/>
+      <c r="F59" s="191"/>
+      <c r="G59" s="191"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="164"/>
-      <c r="C60" s="164"/>
-      <c r="D60" s="164"/>
-      <c r="E60" s="164"/>
-      <c r="F60" s="164"/>
-      <c r="G60" s="164"/>
+      <c r="B60" s="191"/>
+      <c r="C60" s="191"/>
+      <c r="D60" s="191"/>
+      <c r="E60" s="191"/>
+      <c r="F60" s="191"/>
+      <c r="G60" s="191"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>
@@ -5515,19 +5515,71 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
@@ -5552,76 +5604,24 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B23:C25"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.31496062992125984" bottom="0" header="0.19685039370078741" footer="0"/>
-  <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;R機密等級：密等</oddHeader>
     <oddFooter>&amp;L&amp;"標楷體,標準"&amp;10放款部 放款管理課製表 &amp;D</oddFooter>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/16 週一 11:50:20.46
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3505CA-C7B3-4E78-9EBD-134E9E5DC60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9B629-3B68-40DF-BA2E-1F4E16E6F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="X月" sheetId="2" r:id="rId1"/>
@@ -3108,35 +3108,109 @@
     <xf numFmtId="178" fontId="35" fillId="0" borderId="43" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3144,8 +3218,29 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3153,31 +3248,10 @@
     <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3196,40 +3270,13 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="53" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3285,102 +3332,55 @@
     <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="6"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4070,8 +4070,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -4094,30 +4094,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
       <c r="H1" s="24"/>
       <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
+      <c r="A2" s="215"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
       <c r="H2" s="24"/>
       <c r="J2" s="26"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
@@ -4142,21 +4142,21 @@
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="155"/>
-      <c r="D4" s="156" t="s">
+      <c r="C4" s="181"/>
+      <c r="D4" s="182" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="157"/>
-      <c r="F4" s="158" t="s">
+      <c r="E4" s="183"/>
+      <c r="F4" s="184" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="138" t="s">
+      <c r="G4" s="216" t="s">
         <v>60</v>
       </c>
       <c r="H4" s="64"/>
@@ -4168,7 +4168,7 @@
       <c r="N4" s="65"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="153"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="30" t="s">
         <v>35</v>
       </c>
@@ -4181,8 +4181,8 @@
       <c r="E5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="159"/>
-      <c r="G5" s="139"/>
+      <c r="F5" s="185"/>
+      <c r="G5" s="217"/>
       <c r="H5" s="65"/>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
@@ -4206,8 +4206,8 @@
       <c r="G6" s="23"/>
       <c r="H6" s="68"/>
       <c r="I6" s="65"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
+      <c r="J6" s="222"/>
+      <c r="K6" s="222"/>
       <c r="L6" s="69">
         <f>J6-G6</f>
         <v>0</v>
@@ -4234,8 +4234,8 @@
       <c r="I7" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="148"/>
-      <c r="K7" s="148"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="222"/>
       <c r="L7" s="69">
         <f>J7-G7</f>
         <v>0</v>
@@ -4342,12 +4342,12 @@
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="135" t="s">
+      <c r="D11" s="166"/>
+      <c r="E11" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
       <c r="H11" s="80"/>
       <c r="I11" s="81">
         <f>H11-E10</f>
@@ -4360,15 +4360,15 @@
       <c r="N11" s="65"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="178" t="s">
+      <c r="A12" s="195" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="179"/>
-      <c r="C12" s="179"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="141"/>
+      <c r="B12" s="196"/>
+      <c r="C12" s="196"/>
+      <c r="D12" s="218"/>
+      <c r="E12" s="214"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="79"/>
@@ -4378,17 +4378,17 @@
       <c r="N12" s="65"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="180"/>
-      <c r="B13" s="181"/>
-      <c r="C13" s="181"/>
+      <c r="A13" s="197"/>
+      <c r="B13" s="198"/>
+      <c r="C13" s="198"/>
       <c r="D13" s="34"/>
-      <c r="E13" s="176" t="s">
+      <c r="E13" s="193" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="193" t="s">
+      <c r="F13" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="194"/>
+      <c r="G13" s="169"/>
       <c r="H13" s="82" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
@@ -4406,16 +4406,16 @@
       <c r="A14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="149" t="s">
+      <c r="B14" s="223" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="150"/>
+      <c r="C14" s="224"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="177"/>
-      <c r="F14" s="195" t="s">
+      <c r="E14" s="194"/>
+      <c r="F14" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="196"/>
+      <c r="G14" s="171"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
       <c r="J14" s="79"/>
@@ -4428,19 +4428,19 @@
       <c r="A15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="145" t="s">
+      <c r="B15" s="219" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="146"/>
+      <c r="C15" s="220"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="143" t="s">
+      <c r="E15" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="221" t="e">
+      <c r="F15" s="135" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="222"/>
+      <c r="G15" s="136"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="79"/>
@@ -4450,18 +4450,18 @@
       <c r="N15" s="65"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="172" t="e">
+      <c r="B16" s="189" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="173"/>
+      <c r="C16" s="190"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="223"/>
-      <c r="G16" s="224"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="138"/>
       <c r="H16" s="34"/>
       <c r="I16" s="85"/>
       <c r="J16" s="65"/>
@@ -4471,18 +4471,18 @@
       <c r="N16" s="65"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A17" s="144"/>
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
+      <c r="A17" s="177"/>
+      <c r="B17" s="191"/>
+      <c r="C17" s="192"/>
       <c r="D17" s="34"/>
       <c r="E17" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="170" t="e">
+      <c r="F17" s="141" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="171"/>
+      <c r="G17" s="142"/>
       <c r="H17" s="86">
         <f>G10-H18</f>
         <v>0</v>
@@ -4500,23 +4500,23 @@
       <c r="N17" s="65"/>
     </row>
     <row r="18" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A18" s="186" t="s">
+      <c r="A18" s="203" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="187" t="e">
+      <c r="B18" s="204" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="188"/>
+      <c r="C18" s="205"/>
       <c r="D18" s="34"/>
       <c r="E18" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="213" t="e">
+      <c r="F18" s="139" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="214"/>
+      <c r="G18" s="140"/>
       <c r="H18" s="86">
         <f>G7</f>
         <v>0</v>
@@ -4535,18 +4535,18 @@
       <c r="N18" s="65"/>
     </row>
     <row r="19" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A19" s="186"/>
-      <c r="B19" s="187"/>
-      <c r="C19" s="188"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="204"/>
+      <c r="C19" s="205"/>
       <c r="D19" s="34"/>
       <c r="E19" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="170" t="e">
+      <c r="F19" s="141" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="171"/>
+      <c r="G19" s="142"/>
       <c r="H19" s="86">
         <f>G10-H20</f>
         <v>0</v>
@@ -4562,20 +4562,20 @@
       <c r="N19" s="65"/>
     </row>
     <row r="20" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A20" s="185" t="s">
+      <c r="A20" s="202" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="182"/>
-      <c r="C20" s="183"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="200"/>
       <c r="D20" s="34"/>
       <c r="E20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="213" t="e">
+      <c r="F20" s="139" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="214"/>
+      <c r="G20" s="140"/>
       <c r="H20" s="17"/>
       <c r="I20" s="89">
         <f>F7</f>
@@ -4591,9 +4591,9 @@
       <c r="N20" s="65"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="185"/>
-      <c r="B21" s="182"/>
-      <c r="C21" s="183"/>
+      <c r="A21" s="202"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="200"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
@@ -4607,17 +4607,17 @@
       <c r="N21" s="65"/>
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A22" s="185"/>
-      <c r="B22" s="182"/>
-      <c r="C22" s="183"/>
+      <c r="A22" s="202"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="200"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="160" t="s">
+      <c r="E22" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="160" t="s">
+      <c r="F22" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="160" t="s">
+      <c r="G22" s="143" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="86"/>
@@ -4629,18 +4629,18 @@
       <c r="N22" s="65"/>
     </row>
     <row r="23" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A23" s="184" t="s">
+      <c r="A23" s="201" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="189">
+      <c r="B23" s="206">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="190"/>
+      <c r="C23" s="207"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="153"/>
-      <c r="G23" s="153"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="144"/>
       <c r="H23" s="86"/>
       <c r="I23" s="92"/>
       <c r="J23" s="65"/>
@@ -4650,9 +4650,9 @@
       <c r="N23" s="65"/>
     </row>
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="184"/>
-      <c r="B24" s="189"/>
-      <c r="C24" s="190"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="206"/>
+      <c r="C24" s="207"/>
       <c r="D24" s="34"/>
       <c r="E24" s="41" t="s">
         <v>32</v>
@@ -4668,9 +4668,9 @@
       <c r="N24" s="65"/>
     </row>
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="184"/>
-      <c r="B25" s="189"/>
-      <c r="C25" s="190"/>
+      <c r="A25" s="201"/>
+      <c r="B25" s="206"/>
+      <c r="C25" s="207"/>
       <c r="D25" s="34"/>
       <c r="E25" s="42" t="s">
         <v>31</v>
@@ -4692,8 +4692,8 @@
       <c r="A26" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="217"/>
-      <c r="C26" s="217"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="151"/>
       <c r="D26" s="44"/>
       <c r="E26" s="34"/>
       <c r="F26" s="34"/>
@@ -4711,40 +4711,40 @@
       <c r="N26" s="34"/>
     </row>
     <row r="27" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A27" s="160" t="s">
+      <c r="A27" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="164"/>
-      <c r="C27" s="165"/>
-      <c r="D27" s="210" t="s">
+      <c r="B27" s="154"/>
+      <c r="C27" s="187"/>
+      <c r="D27" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="211"/>
-      <c r="F27" s="164"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="154"/>
       <c r="G27" s="45" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="97"/>
       <c r="I27" s="98"/>
-      <c r="J27" s="133" t="s">
+      <c r="J27" s="211" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="134"/>
-      <c r="L27" s="130" t="s">
+      <c r="K27" s="212"/>
+      <c r="L27" s="208" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="131"/>
-      <c r="N27" s="132"/>
+      <c r="M27" s="209"/>
+      <c r="N27" s="210"/>
     </row>
     <row r="28" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A28" s="161"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="215" t="s">
+      <c r="A28" s="186"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="188"/>
+      <c r="D28" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="216"/>
-      <c r="F28" s="166"/>
+      <c r="E28" s="146"/>
+      <c r="F28" s="155"/>
       <c r="G28" s="46" t="s">
         <v>22</v>
       </c>
@@ -4760,16 +4760,16 @@
       <c r="A29" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="162">
+      <c r="B29" s="147">
         <f t="shared" ref="B29:B37" si="1">H29/1000</f>
         <v>0</v>
       </c>
-      <c r="C29" s="163"/>
-      <c r="D29" s="168" t="e">
+      <c r="C29" s="148"/>
+      <c r="D29" s="149" t="e">
         <f>CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="169" t="str">
+      <c r="E29" s="150" t="str">
         <f t="shared" ref="E29" si="2">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="13" t="e">
-        <f>CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(($G$10-F29)/F29,"0.00%"))</f>
+        <f>CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(N29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H29" s="106">
@@ -4817,16 +4817,16 @@
       <c r="A30" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="162">
+      <c r="B30" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C30" s="163"/>
-      <c r="D30" s="168" t="e">
+      <c r="C30" s="148"/>
+      <c r="D30" s="149" t="e">
         <f t="shared" ref="D30:D37" si="5">CONCATENATE(TEXT(J30,"0,000"),"       ",TEXT(K30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="169" t="str">
+      <c r="E30" s="150" t="str">
         <f t="shared" ref="E30:E37" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="13" t="e">
-        <f t="shared" ref="G30:G37" si="8">CONCATENATE(TEXT(M30,"0,000"),"       ",TEXT(($G$10-F30)/F30,"0.00%"))</f>
+        <f t="shared" ref="G30:G37" si="8">CONCATENATE(TEXT(M30,"0,000"),"       ",TEXT(N30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H30" s="108"/>
@@ -4864,16 +4864,16 @@
       <c r="A31" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="162">
+      <c r="B31" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C31" s="163"/>
-      <c r="D31" s="168" t="e">
+      <c r="C31" s="148"/>
+      <c r="D31" s="149" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="169" t="str">
+      <c r="E31" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
@@ -4911,16 +4911,16 @@
       <c r="A32" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="162">
+      <c r="B32" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C32" s="163"/>
-      <c r="D32" s="168" t="e">
+      <c r="C32" s="148"/>
+      <c r="D32" s="149" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="169" t="str">
+      <c r="E32" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -4958,16 +4958,16 @@
       <c r="A33" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="162">
+      <c r="B33" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="168" t="e">
+      <c r="C33" s="148"/>
+      <c r="D33" s="149" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="169" t="str">
+      <c r="E33" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5015,16 +5015,16 @@
       <c r="A34" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="162">
+      <c r="B34" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C34" s="163"/>
-      <c r="D34" s="168" t="e">
-        <f t="shared" si="5"/>
+      <c r="C34" s="148"/>
+      <c r="D34" s="149" t="e">
+        <f>CONCATENATE(TEXT(J34,"0,00"),"       ",TEXT(K34,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="169" t="str">
+      <c r="E34" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5062,16 +5062,16 @@
       <c r="A35" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="162">
+      <c r="B35" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C35" s="163"/>
-      <c r="D35" s="168" t="e">
-        <f t="shared" si="5"/>
+      <c r="C35" s="148"/>
+      <c r="D35" s="149" t="e">
+        <f>CONCATENATE(TEXT(J35,"0"),"       ",TEXT(K35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="169" t="str">
+      <c r="E35" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="13" t="e">
-        <f t="shared" si="8"/>
+        <f>CONCATENATE(TEXT(M35,"0"),"       ",TEXT(N35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H35" s="112"/>
@@ -5109,16 +5109,16 @@
       <c r="A36" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="162">
+      <c r="B36" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C36" s="163"/>
-      <c r="D36" s="168" t="e">
-        <f t="shared" si="5"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="149" t="e">
+        <f>CONCATENATE(TEXT(J36,"0"),"       ",TEXT(K36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="169" t="str">
+      <c r="E36" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="13" t="e">
-        <f t="shared" si="8"/>
+        <f>CONCATENATE(TEXT(M36,"0"),"       ",TEXT(N36,"0.0%"))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H36" s="112"/>
@@ -5156,16 +5156,16 @@
       <c r="A37" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="162">
+      <c r="B37" s="147">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C37" s="163"/>
-      <c r="D37" s="168" t="e">
+      <c r="C37" s="148"/>
+      <c r="D37" s="149" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="169" t="str">
+      <c r="E37" s="150" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
@@ -5203,21 +5203,21 @@
       <c r="A38" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="208" t="e">
+      <c r="B38" s="156" t="e">
         <f>H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="209"/>
-      <c r="D38" s="219" t="e">
+      <c r="C38" s="157"/>
+      <c r="D38" s="174" t="e">
         <f>J38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="220"/>
+      <c r="E38" s="175"/>
       <c r="F38" s="53" t="e">
         <f>L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="218" t="e">
+      <c r="G38" s="130" t="e">
         <f>M38</f>
         <v>#DIV/0!</v>
       </c>
@@ -5269,14 +5269,14 @@
       <c r="A40" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="200" t="s">
+      <c r="B40" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="201"/>
-      <c r="D40" s="200" t="s">
+      <c r="C40" s="163"/>
+      <c r="D40" s="162" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="201"/>
+      <c r="E40" s="163"/>
       <c r="F40" s="62" t="s">
         <v>3</v>
       </c>
@@ -5293,100 +5293,100 @@
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="198"/>
-      <c r="C41" s="199"/>
-      <c r="D41" s="206"/>
-      <c r="E41" s="207"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="132"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="134"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="198"/>
-      <c r="C42" s="199"/>
-      <c r="D42" s="206"/>
-      <c r="E42" s="207"/>
+      <c r="B42" s="131"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="134"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="198"/>
-      <c r="C43" s="199"/>
-      <c r="D43" s="206"/>
-      <c r="E43" s="207"/>
+      <c r="B43" s="131"/>
+      <c r="C43" s="132"/>
+      <c r="D43" s="133"/>
+      <c r="E43" s="134"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="198"/>
-      <c r="C44" s="199"/>
-      <c r="D44" s="206"/>
-      <c r="E44" s="207"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="132"/>
+      <c r="D44" s="133"/>
+      <c r="E44" s="134"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="198"/>
-      <c r="C45" s="199"/>
-      <c r="D45" s="206"/>
-      <c r="E45" s="207"/>
+      <c r="B45" s="131"/>
+      <c r="C45" s="132"/>
+      <c r="D45" s="133"/>
+      <c r="E45" s="134"/>
       <c r="F45" s="8"/>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="198"/>
-      <c r="C46" s="199"/>
-      <c r="D46" s="206"/>
-      <c r="E46" s="207"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="132"/>
+      <c r="D46" s="133"/>
+      <c r="E46" s="134"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="198"/>
-      <c r="C47" s="199"/>
-      <c r="D47" s="198"/>
-      <c r="E47" s="199"/>
+      <c r="B47" s="131"/>
+      <c r="C47" s="132"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="132"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="198"/>
-      <c r="C48" s="199"/>
-      <c r="D48" s="198"/>
-      <c r="E48" s="199"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="132"/>
+      <c r="D48" s="131"/>
+      <c r="E48" s="132"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="198"/>
-      <c r="C49" s="199"/>
-      <c r="D49" s="198"/>
-      <c r="E49" s="199"/>
+      <c r="B49" s="131"/>
+      <c r="C49" s="132"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="132"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="198"/>
-      <c r="C50" s="199"/>
-      <c r="D50" s="198"/>
-      <c r="E50" s="199"/>
+      <c r="B50" s="131"/>
+      <c r="C50" s="132"/>
+      <c r="D50" s="131"/>
+      <c r="E50" s="132"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="198"/>
-      <c r="C51" s="199"/>
-      <c r="D51" s="198"/>
-      <c r="E51" s="199"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="132"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="132"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
@@ -5394,16 +5394,16 @@
       <c r="A52" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="204">
+      <c r="B52" s="152">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="204"/>
-      <c r="D52" s="204">
+      <c r="C52" s="152"/>
+      <c r="D52" s="152">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="204"/>
+      <c r="E52" s="152"/>
       <c r="F52" s="57" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
@@ -5421,16 +5421,16 @@
       <c r="A53" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="203">
+      <c r="B53" s="161">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="203"/>
-      <c r="D53" s="203">
+      <c r="C53" s="161"/>
+      <c r="D53" s="161">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="203"/>
+      <c r="E53" s="161"/>
       <c r="F53" s="60">
         <f>F51-F49</f>
         <v>0</v>
@@ -5445,63 +5445,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="205"/>
-      <c r="B54" s="212"/>
-      <c r="C54" s="212"/>
-      <c r="D54" s="202"/>
-      <c r="E54" s="202"/>
-      <c r="F54" s="192"/>
-      <c r="G54" s="197"/>
+      <c r="A54" s="153"/>
+      <c r="B54" s="160"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="173"/>
+      <c r="E54" s="173"/>
+      <c r="F54" s="165"/>
+      <c r="G54" s="172"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="205"/>
-      <c r="B55" s="212"/>
-      <c r="C55" s="212"/>
-      <c r="D55" s="202"/>
-      <c r="E55" s="202"/>
-      <c r="F55" s="192"/>
-      <c r="G55" s="197"/>
+      <c r="A55" s="153"/>
+      <c r="B55" s="160"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="173"/>
+      <c r="E55" s="173"/>
+      <c r="F55" s="165"/>
+      <c r="G55" s="172"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="191"/>
-      <c r="C56" s="191"/>
-      <c r="D56" s="191"/>
-      <c r="E56" s="191"/>
-      <c r="F56" s="191"/>
-      <c r="G56" s="191"/>
+      <c r="B56" s="164"/>
+      <c r="C56" s="164"/>
+      <c r="D56" s="164"/>
+      <c r="E56" s="164"/>
+      <c r="F56" s="164"/>
+      <c r="G56" s="164"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="191"/>
-      <c r="C57" s="191"/>
-      <c r="D57" s="191"/>
-      <c r="E57" s="191"/>
-      <c r="F57" s="191"/>
-      <c r="G57" s="191"/>
+      <c r="B57" s="164"/>
+      <c r="C57" s="164"/>
+      <c r="D57" s="164"/>
+      <c r="E57" s="164"/>
+      <c r="F57" s="164"/>
+      <c r="G57" s="164"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="191"/>
-      <c r="C58" s="191"/>
-      <c r="D58" s="191"/>
-      <c r="E58" s="191"/>
-      <c r="F58" s="191"/>
-      <c r="G58" s="191"/>
+      <c r="B58" s="164"/>
+      <c r="C58" s="164"/>
+      <c r="D58" s="164"/>
+      <c r="E58" s="164"/>
+      <c r="F58" s="164"/>
+      <c r="G58" s="164"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="191"/>
-      <c r="C59" s="191"/>
-      <c r="D59" s="191"/>
-      <c r="E59" s="191"/>
-      <c r="F59" s="191"/>
-      <c r="G59" s="191"/>
+      <c r="B59" s="164"/>
+      <c r="C59" s="164"/>
+      <c r="D59" s="164"/>
+      <c r="E59" s="164"/>
+      <c r="F59" s="164"/>
+      <c r="G59" s="164"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="191"/>
-      <c r="C60" s="191"/>
-      <c r="D60" s="191"/>
-      <c r="E60" s="191"/>
-      <c r="F60" s="191"/>
-      <c r="G60" s="191"/>
+      <c r="B60" s="164"/>
+      <c r="C60" s="164"/>
+      <c r="D60" s="164"/>
+      <c r="E60" s="164"/>
+      <c r="F60" s="164"/>
+      <c r="G60" s="164"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>
@@ -5515,23 +5515,67 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A12:C13"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B20:C22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="B23:C25"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="A54:A55"/>
@@ -5556,67 +5600,23 @@
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B20:C22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="B23:C25"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/16 週一 16:51:18.32
</commit_message>
<xml_diff>
--- a/Program/Other/LM085_底稿_放款逾期月報表.xlsx
+++ b/Program/Other/LM085_底稿_放款逾期月報表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9B629-3B68-40DF-BA2E-1F4E16E6F516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829F584-9DD2-4D3C-A4AF-15192CFA55EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2751,7 +2751,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2775,9 +2775,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="22" fillId="0" borderId="11" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3111,172 +3108,128 @@
     <xf numFmtId="179" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="178" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="59" fillId="0" borderId="17" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="73" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="72" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="44" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="34" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="53" fillId="0" borderId="26" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3332,55 +3285,99 @@
     <xf numFmtId="181" fontId="53" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="33" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="32" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="40" fillId="0" borderId="16" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="37" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="34" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="37" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="34" fillId="0" borderId="31" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="25" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="179" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="180" fontId="27" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="181" fontId="22" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="13" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="34" fillId="0" borderId="12" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="33" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="51" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="26" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="26" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="34" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="18" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="60" fillId="0" borderId="31" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="34" fillId="0" borderId="31" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="31" xfId="46" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="39" fillId="0" borderId="35" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4070,8 +4067,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -4094,717 +4091,717 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="151" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="23"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="215"/>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="24"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="O2" s="24"/>
+      <c r="A2" s="137"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="23"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="O2" s="23"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="25"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="54.75" customHeight="1">
-      <c r="A4" s="179" t="s">
+      <c r="A4" s="152" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="182" t="s">
+      <c r="C4" s="155"/>
+      <c r="D4" s="156" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="183"/>
-      <c r="F4" s="184" t="s">
+      <c r="E4" s="157"/>
+      <c r="F4" s="158" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="216" t="s">
+      <c r="G4" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
     </row>
     <row r="5" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A5" s="144"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="153"/>
+      <c r="B5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="185"/>
-      <c r="G5" s="217"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="F5" s="159"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
     </row>
     <row r="6" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21">
+      <c r="B6" s="30"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20">
         <f>C6+E6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="222"/>
-      <c r="L6" s="69">
+      <c r="G6" s="22"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="68">
         <f>J6-G6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
     </row>
     <row r="7" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21">
+      <c r="B7" s="21"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20">
         <f t="shared" ref="F7:F10" si="0">C7+E7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="70" t="s">
+      <c r="G7" s="19"/>
+      <c r="H7" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="71" t="s">
+      <c r="I7" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="222"/>
-      <c r="K7" s="222"/>
-      <c r="L7" s="69">
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
+      <c r="L7" s="68">
         <f>J7-G7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73">
+      <c r="G8" s="19"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="72">
         <f>H8-G8</f>
         <v>0</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="75">
+      <c r="J8" s="73"/>
+      <c r="K8" s="74">
         <f>J8-E8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="76"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
     </row>
     <row r="9" spans="1:15" ht="22.05" customHeight="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="19">
         <f>F9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="73">
+      <c r="H9" s="71"/>
+      <c r="I9" s="72">
         <f>H9-F9</f>
         <v>0</v>
       </c>
-      <c r="J9" s="77"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
     </row>
     <row r="10" spans="1:15" ht="34.5" customHeight="1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <f>SUM(B6:B9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <f>SUM(C6:C9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <f>SUM(D6:D9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="18">
         <f>SUM(E6:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <f>SUM(G6:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="78"/>
-      <c r="I10" s="73">
+      <c r="H10" s="77"/>
+      <c r="I10" s="72">
         <f>H10-G10</f>
         <v>0</v>
       </c>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
     </row>
     <row r="11" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="213" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="81">
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80">
         <f>H11-E10</f>
         <v>0</v>
       </c>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="196"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="218"/>
-      <c r="E12" s="214"/>
-      <c r="F12" s="167"/>
-      <c r="G12" s="167"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
+      <c r="B12" s="179"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A13" s="197"/>
-      <c r="B13" s="198"/>
-      <c r="C13" s="198"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="193" t="s">
+      <c r="A13" s="180"/>
+      <c r="B13" s="181"/>
+      <c r="C13" s="181"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="168" t="s">
+      <c r="F13" s="193" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="169"/>
-      <c r="H13" s="82" t="e">
+      <c r="G13" s="194"/>
+      <c r="H13" s="81" t="e">
         <f>-B20/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="83" t="s">
+      <c r="I13" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
     </row>
     <row r="14" spans="1:15" ht="17.399999999999999">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="223" t="s">
+      <c r="B14" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="224"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="170" t="s">
+      <c r="C14" s="150"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="195" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="171"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="65"/>
+      <c r="G14" s="196"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="64"/>
     </row>
     <row r="15" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="219" t="s">
+      <c r="B15" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="220"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="176" t="s">
+      <c r="C15" s="146"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="135" t="e">
+      <c r="F15" s="215" t="e">
         <f>F10/G10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="136"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="65"/>
+      <c r="G15" s="216"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="64"/>
     </row>
     <row r="16" spans="1:15" ht="20.25" customHeight="1">
-      <c r="A16" s="176" t="s">
+      <c r="A16" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="189" t="e">
+      <c r="B16" s="172" t="e">
         <f>F10/B23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C16" s="190"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="137"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="217"/>
+      <c r="G16" s="218"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A17" s="177"/>
-      <c r="B17" s="191"/>
-      <c r="C17" s="192"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="37" t="s">
+      <c r="A17" s="144"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="141" t="e">
+      <c r="F17" s="170" t="e">
         <f>$I$17/$H$17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="142"/>
-      <c r="H17" s="86">
+      <c r="G17" s="171"/>
+      <c r="H17" s="85">
         <f>G10-H18</f>
         <v>0</v>
       </c>
-      <c r="I17" s="87">
+      <c r="I17" s="86">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J17" s="88" t="s">
+      <c r="J17" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
     </row>
     <row r="18" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A18" s="203" t="s">
+      <c r="A18" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="204" t="e">
+      <c r="B18" s="187" t="e">
         <f>-B20/F10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C18" s="205"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="38" t="s">
+      <c r="C18" s="188"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="139" t="e">
+      <c r="F18" s="219" t="e">
         <f>I18/H18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="140"/>
-      <c r="H18" s="86">
+      <c r="G18" s="220"/>
+      <c r="H18" s="85">
         <f>G7</f>
         <v>0</v>
       </c>
-      <c r="I18" s="89">
+      <c r="I18" s="88">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J18" s="90">
+      <c r="J18" s="89">
         <f>SUM(H17:H18)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
     </row>
     <row r="19" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A19" s="203"/>
-      <c r="B19" s="204"/>
-      <c r="C19" s="205"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="39" t="s">
+      <c r="A19" s="186"/>
+      <c r="B19" s="187"/>
+      <c r="C19" s="188"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="141" t="e">
+      <c r="F19" s="170" t="e">
         <f>I19/H19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="142"/>
-      <c r="H19" s="86">
+      <c r="G19" s="171"/>
+      <c r="H19" s="85">
         <f>G10-H20</f>
         <v>0</v>
       </c>
-      <c r="I19" s="89">
+      <c r="I19" s="88">
         <f>F10-F7</f>
         <v>0</v>
       </c>
-      <c r="J19" s="90"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
     </row>
     <row r="20" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A20" s="202" t="s">
+      <c r="A20" s="185" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="199"/>
-      <c r="C20" s="200"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="40" t="s">
+      <c r="B20" s="182"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="139" t="e">
+      <c r="F20" s="219" t="e">
         <f>I20/H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="140"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="89">
+      <c r="G20" s="220"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="88">
         <f>F7</f>
         <v>0</v>
       </c>
-      <c r="J20" s="90">
+      <c r="J20" s="89">
         <f>SUM(H19:H20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
     </row>
     <row r="21" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A21" s="202"/>
-      <c r="B21" s="199"/>
-      <c r="C21" s="200"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="92"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
+      <c r="A21" s="185"/>
+      <c r="B21" s="182"/>
+      <c r="C21" s="183"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
     </row>
     <row r="22" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A22" s="202"/>
-      <c r="B22" s="199"/>
-      <c r="C22" s="200"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="143" t="s">
+      <c r="A22" s="185"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="183"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="143" t="s">
+      <c r="F22" s="160" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="143" t="s">
+      <c r="G22" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="86"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
     </row>
     <row r="23" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="184" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="206">
+      <c r="B23" s="189">
         <f>G10+H26</f>
         <v>0</v>
       </c>
-      <c r="C23" s="207"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="153"/>
+      <c r="F23" s="153"/>
+      <c r="G23" s="153"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
     </row>
     <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="201"/>
-      <c r="B24" s="206"/>
-      <c r="C24" s="207"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="41" t="s">
+      <c r="A24" s="184"/>
+      <c r="B24" s="189"/>
+      <c r="C24" s="190"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="91"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
     </row>
     <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="201"/>
-      <c r="B25" s="206"/>
-      <c r="C25" s="207"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="42" t="s">
+      <c r="A25" s="184"/>
+      <c r="B25" s="189"/>
+      <c r="C25" s="190"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="94">
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="93">
         <f>H25-B23</f>
         <v>0</v>
       </c>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
     </row>
     <row r="26" spans="1:15" ht="27" customHeight="1">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="151"/>
-      <c r="C26" s="151"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="29" t="s">
+      <c r="B26" s="223"/>
+      <c r="C26" s="223"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="95" t="s">
+      <c r="H26" s="13"/>
+      <c r="I26" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="96"/>
-      <c r="K26" s="96"/>
-      <c r="L26" s="96"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="34"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="33"/>
     </row>
     <row r="27" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A27" s="143" t="s">
+      <c r="A27" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="187"/>
-      <c r="D27" s="158" t="s">
+      <c r="B27" s="164"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="212" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="159"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="45" t="s">
+      <c r="E27" s="213"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="97"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="211" t="s">
+      <c r="H27" s="96"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="212"/>
-      <c r="L27" s="208" t="s">
+      <c r="K27" s="134"/>
+      <c r="L27" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="M27" s="209"/>
-      <c r="N27" s="210"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="132"/>
     </row>
     <row r="28" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A28" s="186"/>
-      <c r="B28" s="155"/>
-      <c r="C28" s="188"/>
-      <c r="D28" s="145" t="s">
+      <c r="A28" s="161"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="221" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="146"/>
-      <c r="F28" s="155"/>
-      <c r="G28" s="46" t="s">
+      <c r="E28" s="222"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="99"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="102"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="104"/>
-      <c r="N28" s="105"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="99"/>
+      <c r="J28" s="100"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="103"/>
+      <c r="N28" s="104"/>
     </row>
     <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="147">
+      <c r="B29" s="162">
         <f t="shared" ref="B29:B37" si="1">H29/1000</f>
         <v>0</v>
       </c>
-      <c r="C29" s="148"/>
-      <c r="D29" s="149" t="e">
+      <c r="C29" s="163"/>
+      <c r="D29" s="168" t="e">
         <f>CONCATENATE(TEXT(J29,"0,000"),"       ",TEXT(K29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E29" s="150" t="str">
+      <c r="E29" s="169" t="str">
         <f t="shared" ref="E29" si="2">CONCATENATE("108年度現階段累積達成率",TEXT(J25,"0.00%"),"     ",TEXT(J21,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F29" s="48">
+      <c r="F29" s="47">
         <f>L29/1000</f>
         <v>0</v>
       </c>
-      <c r="G29" s="13" t="e">
+      <c r="G29" s="12" t="e">
         <f>CONCATENATE(TEXT(M29,"0,000"),"       ",TEXT(N29,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="106">
+      <c r="H29" s="105">
         <f>SUM(H30:H32)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="120" t="s">
+      <c r="I29" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="107">
+      <c r="J29" s="106">
         <f>(O29-H29)/1000</f>
         <v>0</v>
       </c>
-      <c r="K29" s="123" t="e">
+      <c r="K29" s="122" t="e">
         <f t="shared" ref="K29:K35" si="3">J29/B29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L29" s="127">
+      <c r="L29" s="126">
         <f>SUM(L30:L32)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="107">
+      <c r="M29" s="106">
         <f>(O29-L29)/1000</f>
         <v>0</v>
       </c>
-      <c r="N29" s="123" t="e">
+      <c r="N29" s="122" t="e">
         <f t="shared" ref="N29:N35" si="4">M29/F29</f>
         <v>#DIV/0!</v>
       </c>
@@ -4814,195 +4811,195 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="147">
+      <c r="B30" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C30" s="148"/>
-      <c r="D30" s="149" t="e">
+      <c r="C30" s="163"/>
+      <c r="D30" s="168" t="e">
         <f t="shared" ref="D30:D37" si="5">CONCATENATE(TEXT(J30,"0,000"),"       ",TEXT(K30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="150" t="str">
+      <c r="E30" s="169" t="str">
         <f t="shared" ref="E30:E37" si="6">CONCATENATE("108年度現階段累積達成率",TEXT(J26,"0.00%"),"     ",TEXT(J22,"0.00"))</f>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F30" s="48">
+      <c r="F30" s="47">
         <f t="shared" ref="F30:F37" si="7">L30/1000</f>
         <v>0</v>
       </c>
-      <c r="G30" s="13" t="e">
+      <c r="G30" s="12" t="e">
         <f t="shared" ref="G30:G37" si="8">CONCATENATE(TEXT(M30,"0,000"),"       ",TEXT(N30,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="108"/>
-      <c r="I30" s="121" t="s">
+      <c r="H30" s="107"/>
+      <c r="I30" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="109">
+      <c r="J30" s="108">
         <f t="shared" ref="J30:J36" si="9">(O30-H30)/1000</f>
         <v>0</v>
       </c>
-      <c r="K30" s="124" t="e">
+      <c r="K30" s="123" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L30" s="128"/>
-      <c r="M30" s="109">
+      <c r="L30" s="127"/>
+      <c r="M30" s="108">
         <f t="shared" ref="M30:M37" si="10">(O30-L30)/1000</f>
         <v>0</v>
       </c>
-      <c r="N30" s="124" t="e">
+      <c r="N30" s="123" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="147">
+      <c r="B31" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C31" s="148"/>
-      <c r="D31" s="149" t="e">
+      <c r="C31" s="163"/>
+      <c r="D31" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="150" t="str">
+      <c r="E31" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率上月增減     0.00</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G31" s="13" t="e">
+      <c r="G31" s="12" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H31" s="108"/>
-      <c r="I31" s="121" t="s">
+      <c r="H31" s="107"/>
+      <c r="I31" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="109">
+      <c r="J31" s="108">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K31" s="124" t="e">
+      <c r="K31" s="123" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L31" s="128"/>
-      <c r="M31" s="109">
+      <c r="L31" s="127"/>
+      <c r="M31" s="108">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N31" s="124" t="e">
+      <c r="N31" s="123" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="147">
+      <c r="B32" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C32" s="148"/>
-      <c r="D32" s="149" t="e">
+      <c r="C32" s="163"/>
+      <c r="D32" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E32" s="150" t="str">
+      <c r="E32" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G32" s="13" t="e">
+      <c r="G32" s="12" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H32" s="108"/>
-      <c r="I32" s="122" t="s">
+      <c r="H32" s="107"/>
+      <c r="I32" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="109">
+      <c r="J32" s="108">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K32" s="125" t="e">
+      <c r="K32" s="124" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L32" s="128"/>
-      <c r="M32" s="109">
+      <c r="L32" s="127"/>
+      <c r="M32" s="108">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N32" s="125" t="e">
+      <c r="N32" s="124" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="147">
+      <c r="B33" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C33" s="148"/>
-      <c r="D33" s="149" t="e">
+      <c r="C33" s="163"/>
+      <c r="D33" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="150" t="str">
+      <c r="E33" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F33" s="48">
+      <c r="F33" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G33" s="13" t="e">
+      <c r="G33" s="12" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H33" s="106">
+      <c r="H33" s="105">
         <f>SUM(H34:H36)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="120" t="s">
+      <c r="I33" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="107">
+      <c r="J33" s="106">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K33" s="123" t="e">
+      <c r="K33" s="122" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L33" s="127">
+      <c r="L33" s="126">
         <f>SUM(L34:L36)</f>
         <v>0</v>
       </c>
-      <c r="M33" s="107">
+      <c r="M33" s="106">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N33" s="123" t="e">
+      <c r="N33" s="122" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
@@ -5012,251 +5009,251 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="147">
+      <c r="B34" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C34" s="148"/>
-      <c r="D34" s="149" t="e">
+      <c r="C34" s="163"/>
+      <c r="D34" s="168" t="e">
         <f>CONCATENATE(TEXT(J34,"0,00"),"       ",TEXT(K34,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E34" s="150" t="str">
+      <c r="E34" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F34" s="48">
+      <c r="F34" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G34" s="13" t="e">
+      <c r="G34" s="12" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H34" s="112"/>
-      <c r="I34" s="121" t="s">
+      <c r="H34" s="111"/>
+      <c r="I34" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="109">
+      <c r="J34" s="108">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K34" s="124" t="e">
+      <c r="K34" s="123" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L34" s="128"/>
-      <c r="M34" s="109">
+      <c r="L34" s="127"/>
+      <c r="M34" s="108">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N34" s="124" t="e">
+      <c r="N34" s="123" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="49" t="s">
+      <c r="A35" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="147">
+      <c r="B35" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C35" s="148"/>
-      <c r="D35" s="149" t="e">
+      <c r="C35" s="163"/>
+      <c r="D35" s="168" t="e">
         <f>CONCATENATE(TEXT(J35,"0"),"       ",TEXT(K35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E35" s="150" t="str">
+      <c r="E35" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     上月增減</v>
       </c>
-      <c r="F35" s="48">
+      <c r="F35" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G35" s="13" t="e">
+      <c r="G35" s="12" t="e">
         <f>CONCATENATE(TEXT(M35,"0"),"       ",TEXT(N35,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H35" s="112"/>
-      <c r="I35" s="121" t="s">
+      <c r="H35" s="111"/>
+      <c r="I35" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="J35" s="109">
+      <c r="J35" s="108">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K35" s="124" t="e">
+      <c r="K35" s="123" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="128"/>
-      <c r="M35" s="109">
+      <c r="L35" s="127"/>
+      <c r="M35" s="108">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N35" s="124" t="e">
+      <c r="N35" s="123" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="147">
+      <c r="B36" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C36" s="148"/>
-      <c r="D36" s="149" t="e">
+      <c r="C36" s="163"/>
+      <c r="D36" s="168" t="e">
         <f>CONCATENATE(TEXT(J36,"0"),"       ",TEXT(K36,"0.00%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E36" s="150" t="str">
+      <c r="E36" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G36" s="13" t="e">
+      <c r="G36" s="12" t="e">
         <f>CONCATENATE(TEXT(M36,"0"),"       ",TEXT(N36,"0.0%"))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H36" s="112"/>
-      <c r="I36" s="122" t="s">
+      <c r="H36" s="111"/>
+      <c r="I36" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="110">
+      <c r="J36" s="109">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K36" s="124" t="e">
+      <c r="K36" s="123" t="e">
         <f>J36/B36</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L36" s="129"/>
-      <c r="M36" s="110">
+      <c r="L36" s="128"/>
+      <c r="M36" s="109">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N36" s="125" t="e">
+      <c r="N36" s="124" t="e">
         <f>M36/F36</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="147">
+      <c r="B37" s="162">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C37" s="148"/>
-      <c r="D37" s="149" t="e">
+      <c r="C37" s="163"/>
+      <c r="D37" s="168" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E37" s="150" t="str">
+      <c r="E37" s="169" t="str">
         <f t="shared" si="6"/>
         <v>108年度現階段累積達成率0.00%     0.00</v>
       </c>
-      <c r="F37" s="48">
+      <c r="F37" s="47">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G37" s="13" t="e">
+      <c r="G37" s="12" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H37" s="126"/>
-      <c r="I37" s="12" t="s">
+      <c r="H37" s="125"/>
+      <c r="I37" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="111">
+      <c r="J37" s="110">
         <f>(C10-H37)/1000</f>
         <v>0</v>
       </c>
-      <c r="K37" s="114" t="e">
+      <c r="K37" s="113" t="e">
         <f>J37/B37</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L37" s="115"/>
-      <c r="M37" s="109">
+      <c r="L37" s="114"/>
+      <c r="M37" s="108">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N37" s="114" t="e">
+      <c r="N37" s="113" t="e">
         <f>M37/F37</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="156" t="e">
+      <c r="B38" s="210" t="e">
         <f>H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" s="157"/>
-      <c r="D38" s="174" t="e">
+      <c r="C38" s="211"/>
+      <c r="D38" s="204" t="e">
         <f>J38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E38" s="175"/>
-      <c r="F38" s="53" t="e">
+      <c r="E38" s="205"/>
+      <c r="F38" s="52" t="e">
         <f>L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="130" t="e">
+      <c r="G38" s="129" t="e">
         <f>M38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H38" s="116" t="e">
+      <c r="H38" s="115" t="e">
         <f>(H33+H37)/H29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I38" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="117" t="e">
+      <c r="J38" s="116" t="e">
         <f>F15-H38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K38" s="113"/>
-      <c r="L38" s="116" t="e">
+      <c r="K38" s="112"/>
+      <c r="L38" s="115" t="e">
         <f>(L33+L37)/L29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M38" s="117" t="e">
+      <c r="M38" s="116" t="e">
         <f>F15-L38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N38" s="118"/>
+      <c r="N38" s="117"/>
     </row>
     <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="29" t="s">
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="119" t="s">
+      <c r="I39" s="118" t="s">
         <v>68</v>
       </c>
       <c r="J39" s="6"/>
@@ -5266,24 +5263,24 @@
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="162" t="s">
+      <c r="B40" s="200" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="163"/>
-      <c r="D40" s="162" t="s">
+      <c r="C40" s="201"/>
+      <c r="D40" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="163"/>
-      <c r="F40" s="62" t="s">
+      <c r="E40" s="201"/>
+      <c r="F40" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="30" t="s">
+      <c r="G40" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="65"/>
+      <c r="H40" s="64"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -5293,122 +5290,122 @@
     </row>
     <row r="41" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="131"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="133"/>
-      <c r="E41" s="134"/>
+      <c r="B41" s="198"/>
+      <c r="C41" s="199"/>
+      <c r="D41" s="208"/>
+      <c r="E41" s="209"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A42" s="9"/>
-      <c r="B42" s="131"/>
-      <c r="C42" s="132"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="134"/>
+      <c r="B42" s="198"/>
+      <c r="C42" s="199"/>
+      <c r="D42" s="208"/>
+      <c r="E42" s="209"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="131"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="133"/>
-      <c r="E43" s="134"/>
+      <c r="B43" s="198"/>
+      <c r="C43" s="199"/>
+      <c r="D43" s="208"/>
+      <c r="E43" s="209"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="131"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="134"/>
+      <c r="B44" s="198"/>
+      <c r="C44" s="199"/>
+      <c r="D44" s="208"/>
+      <c r="E44" s="209"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="131"/>
-      <c r="C45" s="132"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="134"/>
+      <c r="B45" s="198"/>
+      <c r="C45" s="199"/>
+      <c r="D45" s="208"/>
+      <c r="E45" s="209"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="10"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="131"/>
-      <c r="C46" s="132"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="134"/>
+      <c r="B46" s="198"/>
+      <c r="C46" s="199"/>
+      <c r="D46" s="208"/>
+      <c r="E46" s="209"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="131"/>
-      <c r="C47" s="132"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="132"/>
+      <c r="B47" s="198"/>
+      <c r="C47" s="199"/>
+      <c r="D47" s="198"/>
+      <c r="E47" s="199"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:15" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="132"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="132"/>
+      <c r="B48" s="198"/>
+      <c r="C48" s="199"/>
+      <c r="D48" s="198"/>
+      <c r="E48" s="199"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="132"/>
-      <c r="D49" s="131"/>
-      <c r="E49" s="132"/>
+      <c r="B49" s="198"/>
+      <c r="C49" s="199"/>
+      <c r="D49" s="198"/>
+      <c r="E49" s="199"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="131"/>
-      <c r="C50" s="132"/>
-      <c r="D50" s="131"/>
-      <c r="E50" s="132"/>
+      <c r="B50" s="198"/>
+      <c r="C50" s="199"/>
+      <c r="D50" s="198"/>
+      <c r="E50" s="199"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:14" s="6" customFormat="1" ht="21" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
+      <c r="B51" s="198"/>
+      <c r="C51" s="199"/>
+      <c r="D51" s="198"/>
+      <c r="E51" s="199"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="152">
+      <c r="B52" s="206">
         <f>B51-B29</f>
         <v>0</v>
       </c>
-      <c r="C52" s="152"/>
-      <c r="D52" s="152">
+      <c r="C52" s="206"/>
+      <c r="D52" s="206">
         <f>D51-B33-B37</f>
         <v>0</v>
       </c>
-      <c r="E52" s="152"/>
-      <c r="F52" s="57" t="e">
+      <c r="E52" s="206"/>
+      <c r="F52" s="56" t="e">
         <f>F51-B38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G52" s="58"/>
+      <c r="G52" s="57"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
@@ -5418,24 +5415,24 @@
       <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" ht="17.399999999999999">
-      <c r="A53" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="161">
+      <c r="A53" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="203">
         <f>B51-B49</f>
         <v>0</v>
       </c>
-      <c r="C53" s="161"/>
-      <c r="D53" s="161">
+      <c r="C53" s="203"/>
+      <c r="D53" s="203">
         <f>D51-D49</f>
         <v>0</v>
       </c>
-      <c r="E53" s="161"/>
-      <c r="F53" s="60">
+      <c r="E53" s="203"/>
+      <c r="F53" s="59">
         <f>F51-F49</f>
         <v>0</v>
       </c>
-      <c r="G53" s="61"/>
+      <c r="G53" s="60"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
@@ -5445,63 +5442,63 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="25.5" customHeight="1">
-      <c r="A54" s="153"/>
-      <c r="B54" s="160"/>
-      <c r="C54" s="160"/>
-      <c r="D54" s="173"/>
-      <c r="E54" s="173"/>
-      <c r="F54" s="165"/>
-      <c r="G54" s="172"/>
+      <c r="A54" s="207"/>
+      <c r="B54" s="214"/>
+      <c r="C54" s="214"/>
+      <c r="D54" s="202"/>
+      <c r="E54" s="202"/>
+      <c r="F54" s="192"/>
+      <c r="G54" s="197"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:14" ht="27" customHeight="1">
-      <c r="A55" s="153"/>
-      <c r="B55" s="160"/>
-      <c r="C55" s="160"/>
-      <c r="D55" s="173"/>
-      <c r="E55" s="173"/>
-      <c r="F55" s="165"/>
-      <c r="G55" s="172"/>
+      <c r="A55" s="207"/>
+      <c r="B55" s="214"/>
+      <c r="C55" s="214"/>
+      <c r="D55" s="202"/>
+      <c r="E55" s="202"/>
+      <c r="F55" s="192"/>
+      <c r="G55" s="197"/>
     </row>
     <row r="56" spans="1:14" ht="27" customHeight="1">
-      <c r="B56" s="164"/>
-      <c r="C56" s="164"/>
-      <c r="D56" s="164"/>
-      <c r="E56" s="164"/>
-      <c r="F56" s="164"/>
-      <c r="G56" s="164"/>
+      <c r="B56" s="191"/>
+      <c r="C56" s="191"/>
+      <c r="D56" s="191"/>
+      <c r="E56" s="191"/>
+      <c r="F56" s="191"/>
+      <c r="G56" s="191"/>
     </row>
     <row r="57" spans="1:14">
-      <c r="B57" s="164"/>
-      <c r="C57" s="164"/>
-      <c r="D57" s="164"/>
-      <c r="E57" s="164"/>
-      <c r="F57" s="164"/>
-      <c r="G57" s="164"/>
+      <c r="B57" s="191"/>
+      <c r="C57" s="191"/>
+      <c r="D57" s="191"/>
+      <c r="E57" s="191"/>
+      <c r="F57" s="191"/>
+      <c r="G57" s="191"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="B58" s="164"/>
-      <c r="C58" s="164"/>
-      <c r="D58" s="164"/>
-      <c r="E58" s="164"/>
-      <c r="F58" s="164"/>
-      <c r="G58" s="164"/>
+      <c r="B58" s="191"/>
+      <c r="C58" s="191"/>
+      <c r="D58" s="191"/>
+      <c r="E58" s="191"/>
+      <c r="F58" s="191"/>
+      <c r="G58" s="191"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="B59" s="164"/>
-      <c r="C59" s="164"/>
-      <c r="D59" s="164"/>
-      <c r="E59" s="164"/>
-      <c r="F59" s="164"/>
-      <c r="G59" s="164"/>
+      <c r="B59" s="191"/>
+      <c r="C59" s="191"/>
+      <c r="D59" s="191"/>
+      <c r="E59" s="191"/>
+      <c r="F59" s="191"/>
+      <c r="G59" s="191"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="B60" s="164"/>
-      <c r="C60" s="164"/>
-      <c r="D60" s="164"/>
-      <c r="E60" s="164"/>
-      <c r="F60" s="164"/>
-      <c r="G60" s="164"/>
+      <c r="B60" s="191"/>
+      <c r="C60" s="191"/>
+      <c r="D60" s="191"/>
+      <c r="E60" s="191"/>
+      <c r="F60" s="191"/>
+      <c r="G60" s="191"/>
     </row>
     <row r="62" spans="1:14">
       <c r="J62" s="4"/>
@@ -5515,19 +5512,71 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B56:C60"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="D56:E60"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
@@ -5552,71 +5601,19 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="B23:C25"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B56:C60"/>
-    <mergeCell ref="D54:E55"/>
-    <mergeCell ref="D56:E60"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>